<commit_message>
many added snippets :)
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="489">
   <si>
     <t>set</t>
   </si>
@@ -122,9 +122,6 @@
     <t>@List.Toolbar</t>
   </si>
   <si>
-    <t>&lt;div class=\sc-element\&gt;@List.Toolbar&lt;/div&gt;</t>
-  </si>
-  <si>
     <t>AllModules</t>
   </si>
   <si>
@@ -947,9 +944,6 @@
     <t>Content</t>
   </si>
   <si>
-    <t>List</t>
-  </si>
-  <si>
     <t>Module</t>
   </si>
   <si>
@@ -1421,9 +1415,97 @@
     <t>List-ToolbarFloat</t>
   </si>
   <si>
-    <t>&lt;div class=\sc-element\&gt;
+    <t>@Content</t>
+  </si>
+  <si>
+    <t>@List</t>
+  </si>
+  <si>
+    <t>&lt;div class="sc-element"&gt;
     @${1:Content}.Toolbar
 &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sc-element"&gt;
+    @List.Toolbar
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>@C#</t>
+  </si>
+  <si>
+    <t>Basics</t>
+  </si>
+  <si>
+    <t>@foreach(var ${1:cont} in AsDynamic(Data["${2:Default}"])){
+    &lt;div class="sc-element"&gt;
+        @${1}.EntityTitle
+        @${1}.Toolbar
+    &lt;/div&gt;
+}</t>
+  </si>
+  <si>
+    <t>foreach loop</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t>script</t>
+  </si>
+  <si>
+    <t>[Html</t>
+  </si>
+  <si>
+    <t>&lt;script src="[App:Path]/dist/${1:myscripts}.js" type="text/javascript" data-enableoptimizations="100"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>@Html</t>
+  </si>
+  <si>
+    <t>&lt;script src="@App.Path/dist/${1:myscripts}.js" type="text/javascript" data-enableoptimizations="100"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>css, style-sheet</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" href="@App.Path/assets/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" href="[App:Path]/assets/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
+  </si>
+  <si>
+    <t>comment, server-side</t>
+  </si>
+  <si>
+    <t>@* 
+server side multi-line comment
+*@</t>
+  </si>
+  <si>
+    <t>using</t>
+  </si>
+  <si>
+    <t>@using ${1:System.Data.Linq}</t>
+  </si>
+  <si>
+    <t>functions block server-side</t>
+  </si>
+  <si>
+    <t>@functions{
+}</t>
+  </si>
+  <si>
+    <t>Permissions</t>
+  </si>
+  <si>
+    <t>IsEditMode</t>
+  </si>
+  <si>
+    <t>@if (DotNetNuke.Common.Globals.IsEditMode())
+{
+        &lt;div&gt; stuff here which only appears in edit mode &lt;/div&gt;
+}</t>
   </si>
 </sst>
 </file>
@@ -1459,10 +1541,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1483,8 +1568,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F217" totalsRowShown="0">
-  <autoFilter ref="A1:F217"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F228" totalsRowShown="0">
+  <autoFilter ref="A1:F228"/>
   <tableColumns count="6">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -1759,11 +1844,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F216"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="E157" sqref="E157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,8 +1857,8 @@
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="106.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.7109375" customWidth="1"/>
+    <col min="6" max="6" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1784,7 +1869,7 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D1" t="s">
         <v>20</v>
@@ -1798,7 +1883,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1818,7 +1903,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1838,7 +1923,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -1858,7 +1943,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1878,7 +1963,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1898,7 +1983,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -1918,13 +2003,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>322</v>
+        <v>463</v>
       </c>
       <c r="B8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E8" t="s">
         <v>30</v>
@@ -1932,13 +2017,13 @@
     </row>
     <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>322</v>
+        <v>463</v>
       </c>
       <c r="B9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>465</v>
@@ -1946,3065 +2031,3200 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>322</v>
+        <v>464</v>
       </c>
       <c r="B10" t="s">
-        <v>307</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D10" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E10" t="s">
         <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>322</v>
+        <v>464</v>
       </c>
       <c r="B11" t="s">
-        <v>307</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
+        <v>462</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>322</v>
-      </c>
       <c r="B12" t="s">
-        <v>308</v>
+        <v>326</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
+        <v>470</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B13" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B15" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B16" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B17" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B18" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B19" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B20" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B21" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B22" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B24" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B25" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B26" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B27" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E27" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B28" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E28" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B29" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E29" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B30" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E30" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B31" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E31" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B32" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C32" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B33" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E33" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B34" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E34" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B35" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E35" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B36" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E36" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B37" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E37" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B38" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C38" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E38" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B39" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C39" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E39" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B40" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C40" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E40" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B41" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E41" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B42" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C42" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E42" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B43" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C43" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E43" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B44" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C44" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E44" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B45" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C45" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E45" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B46" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C46" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E46" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B47" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C47" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E47" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B48" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C48" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E48" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B49" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C49" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="E49" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B50" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C50" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E50" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B51" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C51" t="s">
-        <v>109</v>
+        <v>46</v>
       </c>
       <c r="E51" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B52" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C52" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E52" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B53" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C53" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E53" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B54" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C54" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E54" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B55" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C55" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="E55" t="s">
-        <v>117</v>
-      </c>
-      <c r="F55" t="s">
-        <v>448</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B56" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C56" t="s">
-        <v>118</v>
+        <v>56</v>
       </c>
       <c r="E56" t="s">
-        <v>119</v>
+        <v>116</v>
+      </c>
+      <c r="F56" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B57" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C57" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E57" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B58" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C58" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E58" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B59" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C59" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E59" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B60" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C60" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E60" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B61" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C61" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E61" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B62" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C62" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E62" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B63" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C63" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E63" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B64" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C64" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E64" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B65" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C65" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E65" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B66" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C66" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E66" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B67" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C67" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E67" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B68" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C68" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E68" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B69" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C69" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E69" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B70" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C70" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E70" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B71" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C71" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E71" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B72" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C72" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E72" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B73" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C73" t="s">
-        <v>91</v>
+        <v>149</v>
       </c>
       <c r="E73" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B74" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C74" t="s">
-        <v>153</v>
+        <v>90</v>
       </c>
       <c r="E74" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B75" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C75" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E75" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B76" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C76" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E76" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B77" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C77" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E77" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B78" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C78" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E78" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B79" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C79" t="s">
-        <v>93</v>
+        <v>160</v>
       </c>
       <c r="E79" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B80" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C80" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E80" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B81" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C81" t="s">
-        <v>165</v>
+        <v>94</v>
       </c>
       <c r="E81" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B82" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C82" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E82" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B83" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C83" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E83" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B84" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C84" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E84" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B85" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C85" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E85" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B86" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C86" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E86" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B87" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C87" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E87" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B88" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C88" t="s">
-        <v>101</v>
+        <v>176</v>
       </c>
       <c r="E88" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B89" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C89" t="s">
-        <v>180</v>
+        <v>100</v>
       </c>
       <c r="E89" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B90" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C90" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E90" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B91" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C91" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E91" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B92" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C92" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E92" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B93" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C93" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E93" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B94" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C94" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E94" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B95" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C95" t="s">
-        <v>109</v>
+        <v>189</v>
       </c>
       <c r="E95" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B96" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C96" t="s">
-        <v>193</v>
+        <v>108</v>
       </c>
       <c r="E96" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B97" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C97" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E97" t="s">
-        <v>196</v>
-      </c>
-      <c r="F97" t="s">
-        <v>314</v>
+        <v>193</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B98" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C98" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E98" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F98" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B99" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C99" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E99" t="s">
-        <v>200</v>
+        <v>197</v>
+      </c>
+      <c r="F99" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B100" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C100" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E100" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B101" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C101" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E101" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B102" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C102" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E102" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B103" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C103" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="E103" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B104" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C104" t="s">
-        <v>208</v>
+        <v>114</v>
       </c>
       <c r="E104" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B105" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C105" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E105" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B106" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C106" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E106" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B107" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C107" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E107" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B108" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C108" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E108" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B109" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C109" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E109" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B110" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C110" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E110" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B111" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C111" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E111" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B112" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C112" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E112" t="s">
-        <v>225</v>
-      </c>
-      <c r="F112" t="s">
-        <v>316</v>
+        <v>222</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B113" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C113" t="s">
-        <v>134</v>
+        <v>223</v>
       </c>
       <c r="E113" t="s">
-        <v>226</v>
+        <v>224</v>
+      </c>
+      <c r="F113" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B114" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C114" t="s">
-        <v>227</v>
+        <v>133</v>
       </c>
       <c r="E114" t="s">
-        <v>228</v>
-      </c>
-      <c r="F114" t="s">
-        <v>317</v>
+        <v>225</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B115" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C115" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E115" t="s">
-        <v>230</v>
+        <v>227</v>
+      </c>
+      <c r="F115" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B116" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C116" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E116" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B117" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C117" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E117" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B118" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C118" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E118" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B119" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C119" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E119" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B120" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C120" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E120" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B121" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C121" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E121" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B122" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C122" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E122" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B123" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C123" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E123" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B124" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C124" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E124" t="s">
-        <v>248</v>
-      </c>
-      <c r="F124" t="s">
-        <v>318</v>
+        <v>245</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B125" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C125" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E125" t="s">
-        <v>250</v>
+        <v>247</v>
+      </c>
+      <c r="F125" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B126" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C126" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E126" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B127" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C127" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E127" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B128" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C128" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E128" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B129" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C129" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E129" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B130" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C130" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E130" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B131" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C131" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E131" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B132" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C132" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E132" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B133" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C133" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E133" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B134" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C134" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E134" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B135" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C135" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E135" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B136" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C136" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E136" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B137" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C137" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E137" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B138" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C138" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E138" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B139" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C139" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E139" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B140" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C140" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E140" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>449</v>
+        <v>320</v>
       </c>
       <c r="B141" t="s">
-        <v>433</v>
+        <v>308</v>
       </c>
       <c r="C141" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E141" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B142" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C142" t="s">
-        <v>208</v>
+        <v>280</v>
       </c>
       <c r="E142" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B143" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C143" t="s">
-        <v>284</v>
+        <v>207</v>
       </c>
       <c r="E143" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B144" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C144" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E144" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B145" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C145" t="s">
-        <v>124</v>
+        <v>285</v>
       </c>
       <c r="E145" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B146" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C146" t="s">
-        <v>289</v>
+        <v>123</v>
       </c>
       <c r="E146" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B147" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C147" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E147" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B148" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C148" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E148" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B149" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C149" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E149" t="s">
-        <v>296</v>
-      </c>
-      <c r="F149" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B150" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C150" t="s">
-        <v>235</v>
+        <v>294</v>
       </c>
       <c r="E150" t="s">
-        <v>297</v>
+        <v>295</v>
+      </c>
+      <c r="F150" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B151" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C151" t="s">
-        <v>298</v>
+        <v>234</v>
       </c>
       <c r="E151" t="s">
-        <v>299</v>
-      </c>
-      <c r="F151" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B152" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C152" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E152" t="s">
-        <v>301</v>
+        <v>298</v>
+      </c>
+      <c r="F152" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B153" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C153" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E153" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B154" t="s">
-        <v>311</v>
+        <v>431</v>
       </c>
       <c r="C154" t="s">
+        <v>301</v>
+      </c>
+      <c r="E154" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B155" t="s">
+        <v>309</v>
+      </c>
+      <c r="C155" t="s">
+        <v>303</v>
+      </c>
+      <c r="E155" t="s">
         <v>304</v>
       </c>
-      <c r="E154" t="s">
-        <v>305</v>
-      </c>
-      <c r="F154" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+      <c r="F155" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B156" t="s">
+        <v>486</v>
+      </c>
+      <c r="C156" t="s">
+        <v>487</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B157" t="s">
+        <v>468</v>
+      </c>
+      <c r="C157" t="s">
+        <v>482</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B158" t="s">
+        <v>468</v>
+      </c>
+      <c r="C158" t="s">
+        <v>480</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B159" t="s">
+        <v>468</v>
+      </c>
+      <c r="C159" t="s">
+        <v>484</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B160" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>361</v>
+      </c>
+      <c r="B161" t="s">
+        <v>365</v>
+      </c>
+      <c r="C161" t="s">
+        <v>366</v>
+      </c>
+      <c r="E161" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>361</v>
+      </c>
+      <c r="B162" t="s">
+        <v>365</v>
+      </c>
+      <c r="C162" t="s">
+        <v>367</v>
+      </c>
+      <c r="E162" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>362</v>
+      </c>
+      <c r="B163" t="s">
+        <v>60</v>
+      </c>
+      <c r="C163" t="s">
+        <v>461</v>
+      </c>
+      <c r="E163" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>362</v>
+      </c>
+      <c r="B164" t="s">
+        <v>60</v>
+      </c>
+      <c r="C164" t="s">
+        <v>462</v>
+      </c>
+      <c r="E164" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>362</v>
+      </c>
+      <c r="B165" t="s">
+        <v>326</v>
+      </c>
+      <c r="C165" t="s">
+        <v>326</v>
+      </c>
+      <c r="E165" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>362</v>
+      </c>
+      <c r="B166" t="s">
+        <v>364</v>
+      </c>
+      <c r="C166" t="s">
+        <v>328</v>
+      </c>
+      <c r="E166" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>362</v>
+      </c>
+      <c r="B167" t="s">
+        <v>364</v>
+      </c>
+      <c r="C167" t="s">
+        <v>330</v>
+      </c>
+      <c r="E167" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>362</v>
+      </c>
+      <c r="B168" t="s">
+        <v>364</v>
+      </c>
+      <c r="C168" t="s">
+        <v>332</v>
+      </c>
+      <c r="E168" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>362</v>
+      </c>
+      <c r="B169" t="s">
+        <v>364</v>
+      </c>
+      <c r="C169" t="s">
+        <v>334</v>
+      </c>
+      <c r="E169" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>362</v>
+      </c>
+      <c r="B170" t="s">
+        <v>364</v>
+      </c>
+      <c r="C170" t="s">
+        <v>336</v>
+      </c>
+      <c r="E170" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>362</v>
+      </c>
+      <c r="B171" t="s">
+        <v>364</v>
+      </c>
+      <c r="C171" t="s">
+        <v>338</v>
+      </c>
+      <c r="E171" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>362</v>
+      </c>
+      <c r="B172" t="s">
+        <v>364</v>
+      </c>
+      <c r="C172" t="s">
+        <v>340</v>
+      </c>
+      <c r="E172" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>362</v>
+      </c>
+      <c r="B173" t="s">
+        <v>364</v>
+      </c>
+      <c r="C173" t="s">
+        <v>342</v>
+      </c>
+      <c r="E173" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>362</v>
+      </c>
+      <c r="B174" t="s">
+        <v>364</v>
+      </c>
+      <c r="C174" t="s">
+        <v>344</v>
+      </c>
+      <c r="E174" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>363</v>
       </c>
-      <c r="B155" t="s">
-        <v>367</v>
-      </c>
-      <c r="C155" t="s">
+      <c r="B175" t="s">
+        <v>1</v>
+      </c>
+      <c r="C175" t="s">
+        <v>2</v>
+      </c>
+      <c r="E175" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>363</v>
+      </c>
+      <c r="B176" t="s">
+        <v>1</v>
+      </c>
+      <c r="C176" t="s">
         <v>368</v>
       </c>
-      <c r="E155" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>363</v>
-      </c>
-      <c r="B156" t="s">
-        <v>367</v>
-      </c>
-      <c r="C156" t="s">
-        <v>369</v>
-      </c>
-      <c r="E156" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>364</v>
-      </c>
-      <c r="B157" t="s">
-        <v>61</v>
-      </c>
-      <c r="C157" t="s">
-        <v>463</v>
-      </c>
-      <c r="E157" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>364</v>
-      </c>
-      <c r="B158" t="s">
-        <v>61</v>
-      </c>
-      <c r="C158" t="s">
-        <v>464</v>
-      </c>
-      <c r="E158" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>364</v>
-      </c>
-      <c r="B159" t="s">
-        <v>328</v>
-      </c>
-      <c r="C159" t="s">
-        <v>328</v>
-      </c>
-      <c r="E159" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>364</v>
-      </c>
-      <c r="B160" t="s">
-        <v>366</v>
-      </c>
-      <c r="C160" t="s">
-        <v>330</v>
-      </c>
-      <c r="E160" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>364</v>
-      </c>
-      <c r="B161" t="s">
-        <v>366</v>
-      </c>
-      <c r="C161" t="s">
-        <v>332</v>
-      </c>
-      <c r="E161" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>364</v>
-      </c>
-      <c r="B162" t="s">
-        <v>366</v>
-      </c>
-      <c r="C162" t="s">
-        <v>334</v>
-      </c>
-      <c r="E162" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>364</v>
-      </c>
-      <c r="B163" t="s">
-        <v>366</v>
-      </c>
-      <c r="C163" t="s">
-        <v>336</v>
-      </c>
-      <c r="E163" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>364</v>
-      </c>
-      <c r="B164" t="s">
-        <v>366</v>
-      </c>
-      <c r="C164" t="s">
-        <v>338</v>
-      </c>
-      <c r="E164" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>364</v>
-      </c>
-      <c r="B165" t="s">
-        <v>366</v>
-      </c>
-      <c r="C165" t="s">
-        <v>340</v>
-      </c>
-      <c r="E165" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>364</v>
-      </c>
-      <c r="B166" t="s">
-        <v>366</v>
-      </c>
-      <c r="C166" t="s">
-        <v>342</v>
-      </c>
-      <c r="E166" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>364</v>
-      </c>
-      <c r="B167" t="s">
-        <v>366</v>
-      </c>
-      <c r="C167" t="s">
-        <v>344</v>
-      </c>
-      <c r="E167" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>364</v>
-      </c>
-      <c r="B168" t="s">
-        <v>366</v>
-      </c>
-      <c r="C168" t="s">
-        <v>346</v>
-      </c>
-      <c r="E168" t="s">
+      <c r="E176" t="s">
         <v>347</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>365</v>
-      </c>
-      <c r="B169" t="s">
-        <v>1</v>
-      </c>
-      <c r="C169" t="s">
-        <v>2</v>
-      </c>
-      <c r="E169" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>365</v>
-      </c>
-      <c r="B170" t="s">
-        <v>1</v>
-      </c>
-      <c r="C170" t="s">
-        <v>370</v>
-      </c>
-      <c r="E170" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>365</v>
-      </c>
-      <c r="B171" t="s">
-        <v>1</v>
-      </c>
-      <c r="C171" t="s">
-        <v>218</v>
-      </c>
-      <c r="E171" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>365</v>
-      </c>
-      <c r="B172" t="s">
-        <v>1</v>
-      </c>
-      <c r="C172" t="s">
-        <v>22</v>
-      </c>
-      <c r="E172" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>365</v>
-      </c>
-      <c r="B173" t="s">
-        <v>1</v>
-      </c>
-      <c r="C173" t="s">
-        <v>371</v>
-      </c>
-      <c r="E173" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>365</v>
-      </c>
-      <c r="B174" t="s">
-        <v>1</v>
-      </c>
-      <c r="C174" t="s">
-        <v>372</v>
-      </c>
-      <c r="E174" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>365</v>
-      </c>
-      <c r="B175" t="s">
-        <v>308</v>
-      </c>
-      <c r="C175" t="s">
-        <v>115</v>
-      </c>
-      <c r="E175" t="s">
-        <v>395</v>
-      </c>
-      <c r="F175" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>365</v>
-      </c>
-      <c r="B176" t="s">
-        <v>308</v>
-      </c>
-      <c r="C176" t="s">
-        <v>57</v>
-      </c>
-      <c r="E176" t="s">
-        <v>397</v>
-      </c>
-      <c r="F176" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B177" t="s">
-        <v>308</v>
+        <v>1</v>
       </c>
       <c r="C177" t="s">
-        <v>59</v>
+        <v>217</v>
       </c>
       <c r="E177" t="s">
-        <v>399</v>
-      </c>
-      <c r="F177" t="s">
-        <v>400</v>
+        <v>348</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B178" t="s">
-        <v>308</v>
+        <v>1</v>
       </c>
       <c r="C178" t="s">
-        <v>434</v>
+        <v>22</v>
       </c>
       <c r="E178" t="s">
-        <v>401</v>
-      </c>
-      <c r="F178" t="s">
-        <v>402</v>
+        <v>349</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B179" t="s">
-        <v>308</v>
+        <v>1</v>
       </c>
       <c r="C179" t="s">
-        <v>61</v>
+        <v>369</v>
       </c>
       <c r="E179" t="s">
-        <v>403</v>
-      </c>
-      <c r="F179" t="s">
-        <v>404</v>
+        <v>350</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B180" t="s">
-        <v>308</v>
+        <v>1</v>
       </c>
       <c r="C180" t="s">
-        <v>436</v>
+        <v>370</v>
       </c>
       <c r="E180" t="s">
-        <v>405</v>
-      </c>
-      <c r="F180" t="s">
-        <v>406</v>
+        <v>351</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B181" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C181" t="s">
-        <v>435</v>
+        <v>114</v>
       </c>
       <c r="E181" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="F181" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B182" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C182" t="s">
-        <v>177</v>
+        <v>56</v>
       </c>
       <c r="E182" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="F182" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B183" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C183" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="E183" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="F183" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B184" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C184" t="s">
-        <v>93</v>
+        <v>432</v>
       </c>
       <c r="E184" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="F184" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B185" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C185" t="s">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="E185" t="s">
-        <v>373</v>
+        <v>401</v>
       </c>
       <c r="F185" t="s">
-        <v>374</v>
+        <v>402</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B186" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C186" t="s">
-        <v>57</v>
+        <v>434</v>
       </c>
       <c r="E186" t="s">
-        <v>375</v>
+        <v>403</v>
       </c>
       <c r="F186" t="s">
-        <v>376</v>
+        <v>404</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B187" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C187" t="s">
-        <v>118</v>
+        <v>433</v>
       </c>
       <c r="E187" t="s">
-        <v>377</v>
+        <v>405</v>
       </c>
       <c r="F187" t="s">
-        <v>378</v>
+        <v>406</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B188" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C188" t="s">
-        <v>435</v>
+        <v>176</v>
       </c>
       <c r="E188" t="s">
-        <v>379</v>
+        <v>407</v>
       </c>
       <c r="F188" t="s">
-        <v>380</v>
+        <v>408</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B189" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C189" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
       <c r="E189" t="s">
-        <v>381</v>
+        <v>409</v>
       </c>
       <c r="F189" t="s">
-        <v>382</v>
+        <v>410</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B190" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C190" t="s">
-        <v>144</v>
+        <v>92</v>
       </c>
       <c r="E190" t="s">
-        <v>383</v>
+        <v>411</v>
       </c>
       <c r="F190" t="s">
-        <v>384</v>
+        <v>412</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B191" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C191" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="E191" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="F191" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B192" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C192" t="s">
-        <v>165</v>
+        <v>56</v>
       </c>
       <c r="E192" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="F192" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B193" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C193" t="s">
-        <v>169</v>
+        <v>117</v>
       </c>
       <c r="E193" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="F193" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B194" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C194" t="s">
-        <v>177</v>
+        <v>433</v>
       </c>
       <c r="E194" t="s">
-        <v>391</v>
+        <v>377</v>
       </c>
       <c r="F194" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B195" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C195" t="s">
-        <v>180</v>
+        <v>133</v>
       </c>
       <c r="E195" t="s">
-        <v>393</v>
+        <v>379</v>
       </c>
       <c r="F195" t="s">
-        <v>394</v>
+        <v>380</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B196" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C196" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="E196" t="s">
-        <v>354</v>
+        <v>381</v>
       </c>
       <c r="F196" t="s">
-        <v>447</v>
+        <v>382</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B197" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C197" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="E197" t="s">
-        <v>355</v>
+        <v>383</v>
       </c>
       <c r="F197" t="s">
-        <v>446</v>
+        <v>384</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B198" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C198" t="s">
-        <v>208</v>
+        <v>164</v>
       </c>
       <c r="E198" t="s">
-        <v>356</v>
+        <v>385</v>
       </c>
       <c r="F198" t="s">
-        <v>445</v>
+        <v>386</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B199" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C199" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
       <c r="E199" t="s">
-        <v>357</v>
+        <v>387</v>
       </c>
       <c r="F199" t="s">
-        <v>444</v>
+        <v>388</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B200" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C200" t="s">
-        <v>220</v>
+        <v>176</v>
       </c>
       <c r="E200" t="s">
-        <v>358</v>
+        <v>389</v>
       </c>
       <c r="F200" t="s">
-        <v>443</v>
+        <v>390</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B201" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C201" t="s">
-        <v>229</v>
+        <v>179</v>
       </c>
       <c r="E201" t="s">
-        <v>359</v>
+        <v>391</v>
       </c>
       <c r="F201" t="s">
-        <v>442</v>
+        <v>392</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B202" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C202" t="s">
-        <v>237</v>
+        <v>192</v>
       </c>
       <c r="E202" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="F202" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B203" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C203" t="s">
-        <v>233</v>
+        <v>114</v>
       </c>
       <c r="E203" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="F203" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B204" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C204" t="s">
-        <v>265</v>
+        <v>207</v>
       </c>
       <c r="E204" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="F204" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>431</v>
+        <v>363</v>
       </c>
       <c r="B205" t="s">
-        <v>433</v>
+        <v>308</v>
       </c>
       <c r="C205" t="s">
-        <v>281</v>
+        <v>215</v>
       </c>
       <c r="E205" t="s">
-        <v>417</v>
+        <v>355</v>
       </c>
       <c r="F205" t="s">
-        <v>418</v>
+        <v>442</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>431</v>
+        <v>363</v>
       </c>
       <c r="B206" t="s">
-        <v>433</v>
+        <v>308</v>
       </c>
       <c r="C206" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="E206" t="s">
-        <v>419</v>
+        <v>356</v>
       </c>
       <c r="F206" t="s">
-        <v>420</v>
+        <v>441</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>431</v>
+        <v>363</v>
       </c>
       <c r="B207" t="s">
-        <v>433</v>
+        <v>308</v>
       </c>
       <c r="C207" t="s">
-        <v>284</v>
+        <v>228</v>
       </c>
       <c r="E207" t="s">
-        <v>421</v>
+        <v>357</v>
       </c>
       <c r="F207" t="s">
-        <v>422</v>
+        <v>440</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>431</v>
+        <v>363</v>
       </c>
       <c r="B208" t="s">
-        <v>433</v>
+        <v>308</v>
       </c>
       <c r="C208" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="E208" t="s">
-        <v>423</v>
+        <v>358</v>
       </c>
       <c r="F208" t="s">
-        <v>424</v>
+        <v>439</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>431</v>
+        <v>363</v>
       </c>
       <c r="B209" t="s">
-        <v>433</v>
+        <v>308</v>
       </c>
       <c r="C209" t="s">
-        <v>293</v>
+        <v>232</v>
       </c>
       <c r="E209" t="s">
-        <v>425</v>
+        <v>359</v>
       </c>
       <c r="F209" t="s">
-        <v>426</v>
+        <v>438</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>431</v>
+        <v>363</v>
       </c>
       <c r="B210" t="s">
-        <v>433</v>
+        <v>308</v>
       </c>
       <c r="C210" t="s">
-        <v>438</v>
+        <v>264</v>
       </c>
       <c r="E210" t="s">
-        <v>427</v>
+        <v>360</v>
       </c>
       <c r="F210" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
+        <v>429</v>
+      </c>
+      <c r="B211" t="s">
         <v>431</v>
       </c>
-      <c r="B211" t="s">
-        <v>311</v>
-      </c>
       <c r="C211" t="s">
-        <v>311</v>
+        <v>280</v>
       </c>
       <c r="E211" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
       <c r="F211" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B212" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="C212" t="s">
-        <v>437</v>
+        <v>207</v>
       </c>
       <c r="E212" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="F212" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B213" t="s">
-        <v>450</v>
+        <v>431</v>
       </c>
       <c r="C213" t="s">
-        <v>451</v>
+        <v>283</v>
       </c>
       <c r="E213" t="s">
-        <v>452</v>
+        <v>419</v>
       </c>
       <c r="F213" t="s">
-        <v>453</v>
+        <v>420</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B214" t="s">
-        <v>450</v>
+        <v>431</v>
       </c>
       <c r="C214" t="s">
-        <v>456</v>
+        <v>285</v>
       </c>
       <c r="E214" t="s">
-        <v>454</v>
+        <v>421</v>
       </c>
       <c r="F214" t="s">
-        <v>455</v>
+        <v>422</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B215" t="s">
-        <v>450</v>
+        <v>431</v>
       </c>
       <c r="C215" t="s">
-        <v>457</v>
+        <v>292</v>
       </c>
       <c r="E215" t="s">
-        <v>458</v>
+        <v>423</v>
       </c>
       <c r="F215" t="s">
-        <v>459</v>
+        <v>424</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B216" t="s">
+        <v>431</v>
+      </c>
+      <c r="C216" t="s">
+        <v>436</v>
+      </c>
+      <c r="E216" t="s">
+        <v>425</v>
+      </c>
+      <c r="F216" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>429</v>
+      </c>
+      <c r="B217" t="s">
+        <v>309</v>
+      </c>
+      <c r="C217" t="s">
+        <v>309</v>
+      </c>
+      <c r="E217" t="s">
+        <v>427</v>
+      </c>
+      <c r="F217" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>430</v>
+      </c>
+      <c r="B218" t="s">
+        <v>435</v>
+      </c>
+      <c r="C218" t="s">
+        <v>435</v>
+      </c>
+      <c r="E218" t="s">
+        <v>413</v>
+      </c>
+      <c r="F218" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>430</v>
+      </c>
+      <c r="B219" t="s">
+        <v>448</v>
+      </c>
+      <c r="C219" t="s">
+        <v>449</v>
+      </c>
+      <c r="E219" t="s">
         <v>450</v>
       </c>
-      <c r="C216" t="s">
+      <c r="F219" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>430</v>
+      </c>
+      <c r="B220" t="s">
+        <v>448</v>
+      </c>
+      <c r="C220" t="s">
+        <v>454</v>
+      </c>
+      <c r="E220" t="s">
+        <v>452</v>
+      </c>
+      <c r="F220" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>430</v>
+      </c>
+      <c r="B221" t="s">
+        <v>448</v>
+      </c>
+      <c r="C221" t="s">
+        <v>455</v>
+      </c>
+      <c r="E221" t="s">
+        <v>456</v>
+      </c>
+      <c r="F221" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>430</v>
+      </c>
+      <c r="B222" t="s">
+        <v>448</v>
+      </c>
+      <c r="C222" t="s">
+        <v>458</v>
+      </c>
+      <c r="E222" t="s">
+        <v>459</v>
+      </c>
+      <c r="F222" t="s">
         <v>460</v>
       </c>
-      <c r="E216" t="s">
-        <v>461</v>
-      </c>
-      <c r="F216" t="s">
-        <v>462</v>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>473</v>
+      </c>
+      <c r="B223" t="s">
+        <v>471</v>
+      </c>
+      <c r="C223" t="s">
+        <v>472</v>
+      </c>
+      <c r="E223" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B224" t="s">
+        <v>471</v>
+      </c>
+      <c r="C224" t="s">
+        <v>477</v>
+      </c>
+      <c r="E224" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B225" t="s">
+        <v>471</v>
+      </c>
+      <c r="C225" t="s">
+        <v>472</v>
+      </c>
+      <c r="E225" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B226" t="s">
+        <v>471</v>
+      </c>
+      <c r="C226" t="s">
+        <v>477</v>
+      </c>
+      <c r="E226" t="s">
+        <v>478</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated icons and now all the file-icons show a +/- correct symbol like word, pdf etc.
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -1437,75 +1437,75 @@
     <t>Basics</t>
   </si>
   <si>
+    <t>foreach loop</t>
+  </si>
+  <si>
+    <t>Resources</t>
+  </si>
+  <si>
+    <t>script</t>
+  </si>
+  <si>
+    <t>[Html</t>
+  </si>
+  <si>
+    <t>&lt;script src="[App:Path]/dist/${1:myscripts}.js" type="text/javascript" data-enableoptimizations="100"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>@Html</t>
+  </si>
+  <si>
+    <t>&lt;script src="@App.Path/dist/${1:myscripts}.js" type="text/javascript" data-enableoptimizations="100"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>css, style-sheet</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" href="@App.Path/assets/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" href="[App:Path]/assets/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
+  </si>
+  <si>
+    <t>comment, server-side</t>
+  </si>
+  <si>
+    <t>@* 
+server side multi-line comment
+*@</t>
+  </si>
+  <si>
+    <t>using</t>
+  </si>
+  <si>
+    <t>@using ${1:System.Data.Linq}</t>
+  </si>
+  <si>
+    <t>functions block server-side</t>
+  </si>
+  <si>
+    <t>@functions{
+}</t>
+  </si>
+  <si>
+    <t>Permissions</t>
+  </si>
+  <si>
+    <t>IsEditMode</t>
+  </si>
+  <si>
+    <t>@if (DotNetNuke.Common.Globals.IsEditMode())
+{
+        &lt;div&gt; stuff here which only appears in edit mode &lt;/div&gt;
+}</t>
+  </si>
+  <si>
     <t>@foreach(var ${1:cont} in AsDynamic(Data["${2:Default}"])){
     &lt;div class="sc-element"&gt;
         @${1}.EntityTitle
         @${1}.Toolbar
     &lt;/div&gt;
-}</t>
-  </si>
-  <si>
-    <t>foreach loop</t>
-  </si>
-  <si>
-    <t>Resources</t>
-  </si>
-  <si>
-    <t>script</t>
-  </si>
-  <si>
-    <t>[Html</t>
-  </si>
-  <si>
-    <t>&lt;script src="[App:Path]/dist/${1:myscripts}.js" type="text/javascript" data-enableoptimizations="100"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>@Html</t>
-  </si>
-  <si>
-    <t>&lt;script src="@App.Path/dist/${1:myscripts}.js" type="text/javascript" data-enableoptimizations="100"&gt;&lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>css, style-sheet</t>
-  </si>
-  <si>
-    <t>&lt;link rel="stylesheet" href="@App.Path/assets/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;link rel="stylesheet" href="[App:Path]/assets/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
-  </si>
-  <si>
-    <t>comment, server-side</t>
-  </si>
-  <si>
-    <t>@* 
-server side multi-line comment
-*@</t>
-  </si>
-  <si>
-    <t>using</t>
-  </si>
-  <si>
-    <t>@using ${1:System.Data.Linq}</t>
-  </si>
-  <si>
-    <t>functions block server-side</t>
-  </si>
-  <si>
-    <t>@functions{
-}</t>
-  </si>
-  <si>
-    <t>Permissions</t>
-  </si>
-  <si>
-    <t>IsEditMode</t>
-  </si>
-  <si>
-    <t>@if (DotNetNuke.Common.Globals.IsEditMode())
-{
-        &lt;div&gt; stuff here which only appears in edit mode &lt;/div&gt;
-}</t>
+}…</t>
   </si>
 </sst>
 </file>
@@ -1847,8 +1847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="E157" sqref="E157"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2071,10 +2071,10 @@
         <v>326</v>
       </c>
       <c r="C12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>469</v>
+        <v>488</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -4111,13 +4111,13 @@
         <v>447</v>
       </c>
       <c r="B156" t="s">
+        <v>485</v>
+      </c>
+      <c r="C156" t="s">
         <v>486</v>
       </c>
-      <c r="C156" t="s">
+      <c r="E156" s="3" t="s">
         <v>487</v>
-      </c>
-      <c r="E156" s="3" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -4128,10 +4128,10 @@
         <v>468</v>
       </c>
       <c r="C157" t="s">
+        <v>481</v>
+      </c>
+      <c r="E157" s="1" t="s">
         <v>482</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -4142,10 +4142,10 @@
         <v>468</v>
       </c>
       <c r="C158" t="s">
+        <v>479</v>
+      </c>
+      <c r="E158" s="3" t="s">
         <v>480</v>
-      </c>
-      <c r="E158" s="3" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4156,10 +4156,10 @@
         <v>468</v>
       </c>
       <c r="C159" t="s">
+        <v>483</v>
+      </c>
+      <c r="E159" s="3" t="s">
         <v>484</v>
-      </c>
-      <c r="E159" s="3" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -5166,58 +5166,58 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
+        <v>472</v>
+      </c>
+      <c r="B223" t="s">
+        <v>470</v>
+      </c>
+      <c r="C223" t="s">
+        <v>471</v>
+      </c>
+      <c r="E223" t="s">
         <v>473</v>
-      </c>
-      <c r="B223" t="s">
-        <v>471</v>
-      </c>
-      <c r="C223" t="s">
-        <v>472</v>
-      </c>
-      <c r="E223" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B224" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C224" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E224" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B225" t="s">
+        <v>470</v>
+      </c>
+      <c r="C225" t="s">
+        <v>471</v>
+      </c>
+      <c r="E225" t="s">
         <v>475</v>
-      </c>
-      <c r="B225" t="s">
-        <v>471</v>
-      </c>
-      <c r="C225" t="s">
-        <v>472</v>
-      </c>
-      <c r="E225" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B226" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C226" t="s">
+        <v>476</v>
+      </c>
+      <c r="E226" t="s">
         <v>477</v>
-      </c>
-      <c r="E226" t="s">
-        <v>478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now supports generic, input-type snippets
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="506">
   <si>
     <t>set</t>
   </si>
@@ -1506,6 +1506,64 @@
         @${1}.Toolbar
     &lt;/div&gt;
 }…</t>
+  </si>
+  <si>
+    <t>@App</t>
+  </si>
+  <si>
+    <t>[App</t>
+  </si>
+  <si>
+    <t>@\InputType</t>
+  </si>
+  <si>
+    <t>hyperlink-library</t>
+  </si>
+  <si>
+    <t>hyperlink-default</t>
+  </si>
+  <si>
+    <t>thumbnail url</t>
+  </si>
+  <si>
+    <t>thumbnail IMG tag</t>
+  </si>
+  <si>
+    <t>[\InputType</t>
+  </si>
+  <si>
+    <t>@$101{var}.$102{prop}?w=${1:200}&amp;h=${2:200}&amp;mode=${3:crop}</t>
+  </si>
+  <si>
+    <t>[$101{var}:$102{prop}]?w=${1:200}&amp;h=${2:200}&amp;mode=${3:crop}</t>
+  </si>
+  <si>
+    <t>&lt;img src="@$101{var}.$102{prop}?w=${1:200}&amp;h=${2:200}&amp;mode=${3:crop}"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src="[$101{var}:$102{prop}]?w=${1:200}&amp;h=${2:200}&amp;mode=${3:crop}"&gt;</t>
+  </si>
+  <si>
+    <t>Thumbnail URL with crop-mode</t>
+  </si>
+  <si>
+    <t>Thumbnail IMG tag with crop-mode</t>
+  </si>
+  <si>
+    <t>loop across assets</t>
+  </si>
+  <si>
+    <t>Large example with looping ADAM assets</t>
+  </si>
+  <si>
+    <t>@foreach(var ${3:pic} in Adam(${1:Content}, "${2:Screenshots}").Files){
+ &lt;div style="clear: both"&gt;
+  &lt;img src="@${3:pic}.Url?w=200&amp;h=200&amp;mode=crop" title="@${3:pic}.FileName" style="float: right"&gt;
+  &lt;h3&gt;@${3:pic}.Metadata.${10:Title}&lt;/h3&gt;
+  Has Meta: @${3:pic}.HasMetadata 
+  &lt;div&gt;Description: @Html.Raw(${3:pic}.Metadata.${11:Description})&lt;/div&gt;
+ &lt;/div&gt;
+}</t>
   </si>
 </sst>
 </file>
@@ -1568,8 +1626,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F228" totalsRowShown="0">
-  <autoFilter ref="A1:F228"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F231" totalsRowShown="0">
+  <autoFilter ref="A1:F231"/>
   <tableColumns count="6">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -1845,16 +1903,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F226"/>
+  <dimension ref="A1:F231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="E228" sqref="E228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61.7109375" customWidth="1"/>
@@ -1883,7 +1941,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>320</v>
+        <v>489</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1903,7 +1961,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>320</v>
+        <v>489</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1923,7 +1981,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>320</v>
+        <v>489</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -1943,7 +2001,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>320</v>
+        <v>489</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1963,7 +2021,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>320</v>
+        <v>489</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1983,7 +2041,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>320</v>
+        <v>489</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -4170,7 +4228,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>361</v>
       </c>
@@ -4184,7 +4242,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>361</v>
       </c>
@@ -4198,7 +4256,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>362</v>
       </c>
@@ -4212,7 +4270,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>362</v>
       </c>
@@ -4226,7 +4284,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>362</v>
       </c>
@@ -4240,7 +4298,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>362</v>
       </c>
@@ -4254,7 +4312,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>362</v>
       </c>
@@ -4268,7 +4326,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>362</v>
       </c>
@@ -4282,7 +4340,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>362</v>
       </c>
@@ -4296,7 +4354,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>362</v>
       </c>
@@ -4310,7 +4368,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>362</v>
       </c>
@@ -4324,7 +4382,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>362</v>
       </c>
@@ -4338,7 +4396,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>362</v>
       </c>
@@ -4352,7 +4410,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>362</v>
       </c>
@@ -4366,9 +4424,9 @@
         <v>345</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>363</v>
+        <v>490</v>
       </c>
       <c r="B175" t="s">
         <v>1</v>
@@ -4379,10 +4437,13 @@
       <c r="E175" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F175" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>363</v>
+        <v>490</v>
       </c>
       <c r="B176" t="s">
         <v>1</v>
@@ -4393,10 +4454,13 @@
       <c r="E176" t="s">
         <v>347</v>
       </c>
+      <c r="F176" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>363</v>
+        <v>490</v>
       </c>
       <c r="B177" t="s">
         <v>1</v>
@@ -4407,10 +4471,13 @@
       <c r="E177" t="s">
         <v>348</v>
       </c>
+      <c r="F177" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>363</v>
+        <v>490</v>
       </c>
       <c r="B178" t="s">
         <v>1</v>
@@ -4421,10 +4488,13 @@
       <c r="E178" t="s">
         <v>349</v>
       </c>
+      <c r="F178" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>363</v>
+        <v>490</v>
       </c>
       <c r="B179" t="s">
         <v>1</v>
@@ -4435,10 +4505,13 @@
       <c r="E179" t="s">
         <v>350</v>
       </c>
+      <c r="F179" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>363</v>
+        <v>490</v>
       </c>
       <c r="B180" t="s">
         <v>1</v>
@@ -4448,6 +4521,9 @@
       </c>
       <c r="E180" t="s">
         <v>351</v>
+      </c>
+      <c r="F180" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
@@ -5192,7 +5268,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>474</v>
       </c>
@@ -5206,7 +5282,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>474</v>
       </c>
@@ -5218,6 +5294,91 @@
       </c>
       <c r="E226" t="s">
         <v>477</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A227" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B227" t="s">
+        <v>492</v>
+      </c>
+      <c r="C227" t="s">
+        <v>503</v>
+      </c>
+      <c r="E227" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="F227" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B228" t="s">
+        <v>493</v>
+      </c>
+      <c r="C228" t="s">
+        <v>494</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="F228" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B229" t="s">
+        <v>493</v>
+      </c>
+      <c r="C229" t="s">
+        <v>495</v>
+      </c>
+      <c r="E229" t="s">
+        <v>499</v>
+      </c>
+      <c r="F229" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B230" t="s">
+        <v>493</v>
+      </c>
+      <c r="C230" t="s">
+        <v>494</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="F230" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>496</v>
+      </c>
+      <c r="B231" t="s">
+        <v>493</v>
+      </c>
+      <c r="C231" t="s">
+        <v>495</v>
+      </c>
+      <c r="E231" t="s">
+        <v>500</v>
+      </c>
+      <c r="F231" t="s">
+        <v>502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now input type snippets in separated code, and show a +more button if more templates exist
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -1553,9 +1553,6 @@
     <t>loop across assets</t>
   </si>
   <si>
-    <t>Large example with looping ADAM assets</t>
-  </si>
-  <si>
     <t>@foreach(var ${3:pic} in Adam(${1:Content}, "${2:Screenshots}").Files){
  &lt;div style="clear: both"&gt;
   &lt;img src="@${3:pic}.Url?w=200&amp;h=200&amp;mode=crop" title="@${3:pic}.FileName" style="float: right"&gt;
@@ -1564,6 +1561,9 @@
   &lt;div&gt;Description: @Html.Raw(${3:pic}.Metadata.${11:Description})&lt;/div&gt;
  &lt;/div&gt;
 }</t>
+  </si>
+  <si>
+    <t>Adam: Large example with looping ADAM assets</t>
   </si>
 </sst>
 </file>
@@ -1906,7 +1906,7 @@
   <dimension ref="A1:F231"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
-      <selection activeCell="E228" sqref="E228"/>
+      <selection activeCell="F228" sqref="F228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5307,10 +5307,10 @@
         <v>503</v>
       </c>
       <c r="E227" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="F227" t="s">
         <v>505</v>
-      </c>
-      <c r="F227" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adam improved + more snippets
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="511">
   <si>
     <t>set</t>
   </si>
@@ -1550,10 +1550,7 @@
     <t>Thumbnail IMG tag with crop-mode</t>
   </si>
   <si>
-    <t>loop across assets</t>
-  </si>
-  <si>
-    <t>@foreach(var ${3:pic} in Adam(${1:Content}, "${2:Screenshots}").Files){
+    <t>@foreach(var ${3:pic} in Adam(${1:var}, "${2:prop}").Files){
  &lt;div style="clear: both"&gt;
   &lt;img src="@${3:pic}.Url?w=200&amp;h=200&amp;mode=crop" title="@${3:pic}.FileName" style="float: right"&gt;
   &lt;h3&gt;@${3:pic}.Metadata.${10:Title}&lt;/h3&gt;
@@ -1564,6 +1561,28 @@
   </si>
   <si>
     <t>Adam: Large example with looping ADAM assets</t>
+  </si>
+  <si>
+    <t>simple loop for assets</t>
+  </si>
+  <si>
+    <t>loop with metadata assets</t>
+  </si>
+  <si>
+    <t>@foreach(var ${3:pic} in Adam(${1:var}, "${2:prop}").Files){
+ &lt;span&gt;@${3:pic}.Url, @${3:pic}.FileName &lt;/span&gt;
+}</t>
+  </si>
+  <si>
+    <t>Adam: simple example with looping ADAM assets</t>
+  </si>
+  <si>
+    <t>loop with type filter</t>
+  </si>
+  <si>
+    <t>@foreach(var ${3:pic} in (AsAdam(${1:var}, "${2:prop}").Files as IEnumerable&lt;ToSic.SexyContent.Adam.AdamFile&gt;).Where(f =&gt; f.Type == "${4:image}")){
+ &lt;span&gt;@${3:pic}.Url, @${3:pic}.FileName &lt;/span&gt;
+}</t>
   </si>
 </sst>
 </file>
@@ -1626,8 +1645,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F231" totalsRowShown="0">
-  <autoFilter ref="A1:F231"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F233" totalsRowShown="0">
+  <autoFilter ref="A1:F233"/>
   <tableColumns count="6">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -1903,10 +1922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F231"/>
+  <dimension ref="A1:F233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
-      <selection activeCell="F228" sqref="F228"/>
+    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
+      <selection activeCell="C230" sqref="C230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5296,7 +5315,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="227" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>491</v>
       </c>
@@ -5304,52 +5323,49 @@
         <v>492</v>
       </c>
       <c r="C227" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="E227" s="3" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="F227" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>491</v>
       </c>
       <c r="B228" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C228" t="s">
-        <v>494</v>
-      </c>
-      <c r="E228" s="1" t="s">
-        <v>497</v>
+        <v>506</v>
+      </c>
+      <c r="E228" s="3" t="s">
+        <v>503</v>
       </c>
       <c r="F228" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>491</v>
       </c>
       <c r="B229" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C229" t="s">
-        <v>495</v>
-      </c>
-      <c r="E229" t="s">
-        <v>499</v>
-      </c>
-      <c r="F229" t="s">
-        <v>502</v>
+        <v>509</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="B230" t="s">
         <v>493</v>
@@ -5358,15 +5374,15 @@
         <v>494</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F230" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
-        <v>496</v>
+      <c r="A231" s="1" t="s">
+        <v>491</v>
       </c>
       <c r="B231" t="s">
         <v>493</v>
@@ -5375,9 +5391,43 @@
         <v>495</v>
       </c>
       <c r="E231" t="s">
+        <v>499</v>
+      </c>
+      <c r="F231" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B232" t="s">
+        <v>493</v>
+      </c>
+      <c r="C232" t="s">
+        <v>494</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="F232" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>496</v>
+      </c>
+      <c r="B233" t="s">
+        <v>493</v>
+      </c>
+      <c r="C233" t="s">
+        <v>495</v>
+      </c>
+      <c r="E233" t="s">
         <v>500</v>
       </c>
-      <c r="F231" t="s">
+      <c r="F233" t="s">
         <v>502</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix list snippet availability for list and toolbar - fix #608
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="510">
   <si>
     <t>set</t>
   </si>
@@ -939,9 +939,6 @@
   </si>
   <si>
     <t>@Dnn.User.Profile.GetPropertyValue(\${1:City}\)</t>
-  </si>
-  <si>
-    <t>Content</t>
   </si>
   <si>
     <t>Module</t>
@@ -1646,7 +1643,14 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F233" totalsRowShown="0">
-  <autoFilter ref="A1:F233"/>
+  <autoFilter ref="A1:F233">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="@Content"/>
+        <filter val="[Content"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -1924,8 +1928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="E234" sqref="E234"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B161" sqref="B161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,7 +1950,7 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D1" t="s">
         <v>20</v>
@@ -1958,9 +1962,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1978,9 +1982,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1998,9 +2002,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -2018,9 +2022,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -2038,9 +2042,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -2058,9 +2062,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -2080,13 +2084,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B8" t="s">
-        <v>305</v>
+        <v>364</v>
       </c>
       <c r="C8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E8" t="s">
         <v>30</v>
@@ -2094,72 +2098,72 @@
     </row>
     <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B9" t="s">
+        <v>364</v>
+      </c>
+      <c r="C9" t="s">
+        <v>366</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>463</v>
-      </c>
-      <c r="B9" t="s">
-        <v>305</v>
-      </c>
-      <c r="C9" t="s">
-        <v>367</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>464</v>
       </c>
       <c r="B10" t="s">
         <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E10" t="s">
         <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B11" t="s">
         <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C13" t="s">
         <v>32</v>
@@ -2168,12 +2172,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C14" t="s">
         <v>34</v>
@@ -2182,12 +2186,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
@@ -2196,12 +2200,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B16" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
@@ -2210,12 +2214,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C17" t="s">
         <v>40</v>
@@ -2224,12 +2228,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C18" t="s">
         <v>42</v>
@@ -2238,12 +2242,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C19" t="s">
         <v>44</v>
@@ -2252,12 +2256,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B20" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C20" t="s">
         <v>46</v>
@@ -2266,12 +2270,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B21" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C21" t="s">
         <v>48</v>
@@ -2280,12 +2284,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B22" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C22" t="s">
         <v>50</v>
@@ -2294,12 +2298,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B23" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C23" t="s">
         <v>52</v>
@@ -2308,12 +2312,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C24" t="s">
         <v>54</v>
@@ -2322,12 +2326,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B25" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C25" t="s">
         <v>56</v>
@@ -2336,12 +2340,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C26" t="s">
         <v>58</v>
@@ -2350,12 +2354,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B27" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C27" t="s">
         <v>60</v>
@@ -2364,12 +2368,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B28" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C28" t="s">
         <v>62</v>
@@ -2378,12 +2382,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B29" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C29" t="s">
         <v>64</v>
@@ -2392,12 +2396,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C30" t="s">
         <v>66</v>
@@ -2406,12 +2410,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B31" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C31" t="s">
         <v>68</v>
@@ -2420,12 +2424,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B32" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C32" t="s">
         <v>70</v>
@@ -2434,12 +2438,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B33" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C33" t="s">
         <v>72</v>
@@ -2448,12 +2452,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B34" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C34" t="s">
         <v>74</v>
@@ -2462,12 +2466,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B35" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C35" t="s">
         <v>76</v>
@@ -2476,12 +2480,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B36" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C36" t="s">
         <v>78</v>
@@ -2490,12 +2494,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B37" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C37" t="s">
         <v>80</v>
@@ -2504,12 +2508,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B38" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C38" t="s">
         <v>82</v>
@@ -2518,12 +2522,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B39" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C39" t="s">
         <v>84</v>
@@ -2532,12 +2536,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B40" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C40" t="s">
         <v>86</v>
@@ -2546,12 +2550,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B41" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C41" t="s">
         <v>88</v>
@@ -2560,12 +2564,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B42" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C42" t="s">
         <v>90</v>
@@ -2574,12 +2578,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B43" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C43" t="s">
         <v>92</v>
@@ -2588,12 +2592,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B44" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C44" t="s">
         <v>94</v>
@@ -2602,12 +2606,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B45" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C45" t="s">
         <v>96</v>
@@ -2616,12 +2620,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B46" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C46" t="s">
         <v>98</v>
@@ -2630,12 +2634,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B47" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C47" t="s">
         <v>100</v>
@@ -2644,12 +2648,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B48" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C48" t="s">
         <v>102</v>
@@ -2658,12 +2662,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B49" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C49" t="s">
         <v>104</v>
@@ -2672,12 +2676,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B50" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C50" t="s">
         <v>44</v>
@@ -2686,12 +2690,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B51" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C51" t="s">
         <v>46</v>
@@ -2700,12 +2704,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B52" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C52" t="s">
         <v>108</v>
@@ -2714,12 +2718,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B53" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C53" t="s">
         <v>110</v>
@@ -2728,12 +2732,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B54" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C54" t="s">
         <v>112</v>
@@ -2742,12 +2746,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B55" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C55" t="s">
         <v>114</v>
@@ -2756,12 +2760,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B56" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C56" t="s">
         <v>56</v>
@@ -2770,15 +2774,15 @@
         <v>116</v>
       </c>
       <c r="F56" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B57" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C57" t="s">
         <v>117</v>
@@ -2787,12 +2791,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B58" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C58" t="s">
         <v>119</v>
@@ -2801,12 +2805,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B59" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C59" t="s">
         <v>121</v>
@@ -2815,12 +2819,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B60" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C60" t="s">
         <v>123</v>
@@ -2829,12 +2833,12 @@
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B61" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C61" t="s">
         <v>125</v>
@@ -2843,12 +2847,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B62" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C62" t="s">
         <v>127</v>
@@ -2857,12 +2861,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B63" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C63" t="s">
         <v>129</v>
@@ -2871,12 +2875,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B64" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C64" t="s">
         <v>131</v>
@@ -2885,12 +2889,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C65" t="s">
         <v>133</v>
@@ -2899,12 +2903,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B66" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C66" t="s">
         <v>135</v>
@@ -2913,12 +2917,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B67" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C67" t="s">
         <v>137</v>
@@ -2927,12 +2931,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B68" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C68" t="s">
         <v>139</v>
@@ -2941,12 +2945,12 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B69" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C69" t="s">
         <v>141</v>
@@ -2955,12 +2959,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B70" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C70" t="s">
         <v>143</v>
@@ -2969,12 +2973,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B71" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C71" t="s">
         <v>145</v>
@@ -2983,12 +2987,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B72" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C72" t="s">
         <v>147</v>
@@ -2997,12 +3001,12 @@
         <v>148</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B73" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C73" t="s">
         <v>149</v>
@@ -3011,12 +3015,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B74" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C74" t="s">
         <v>90</v>
@@ -3025,12 +3029,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B75" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C75" t="s">
         <v>152</v>
@@ -3039,12 +3043,12 @@
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B76" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C76" t="s">
         <v>154</v>
@@ -3053,12 +3057,12 @@
         <v>155</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B77" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C77" t="s">
         <v>156</v>
@@ -3067,12 +3071,12 @@
         <v>157</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B78" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C78" t="s">
         <v>158</v>
@@ -3081,12 +3085,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B79" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C79" t="s">
         <v>160</v>
@@ -3095,12 +3099,12 @@
         <v>161</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B80" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C80" t="s">
         <v>92</v>
@@ -3109,12 +3113,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B81" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C81" t="s">
         <v>94</v>
@@ -3123,12 +3127,12 @@
         <v>163</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B82" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C82" t="s">
         <v>164</v>
@@ -3137,12 +3141,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B83" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C83" t="s">
         <v>166</v>
@@ -3151,12 +3155,12 @@
         <v>167</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B84" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C84" t="s">
         <v>168</v>
@@ -3165,12 +3169,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B85" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C85" t="s">
         <v>170</v>
@@ -3179,12 +3183,12 @@
         <v>171</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B86" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C86" t="s">
         <v>172</v>
@@ -3193,12 +3197,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B87" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C87" t="s">
         <v>174</v>
@@ -3207,12 +3211,12 @@
         <v>175</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B88" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C88" t="s">
         <v>176</v>
@@ -3221,12 +3225,12 @@
         <v>177</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B89" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C89" t="s">
         <v>100</v>
@@ -3235,12 +3239,12 @@
         <v>178</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B90" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C90" t="s">
         <v>179</v>
@@ -3249,12 +3253,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B91" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C91" t="s">
         <v>181</v>
@@ -3263,12 +3267,12 @@
         <v>182</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B92" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C92" t="s">
         <v>183</v>
@@ -3277,12 +3281,12 @@
         <v>184</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B93" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C93" t="s">
         <v>185</v>
@@ -3291,12 +3295,12 @@
         <v>186</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B94" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C94" t="s">
         <v>187</v>
@@ -3305,12 +3309,12 @@
         <v>188</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B95" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C95" t="s">
         <v>189</v>
@@ -3319,12 +3323,12 @@
         <v>190</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B96" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C96" t="s">
         <v>108</v>
@@ -3333,12 +3337,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B97" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C97" t="s">
         <v>192</v>
@@ -3347,12 +3351,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B98" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C98" t="s">
         <v>194</v>
@@ -3361,15 +3365,15 @@
         <v>195</v>
       </c>
       <c r="F98" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B99" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C99" t="s">
         <v>196</v>
@@ -3378,15 +3382,15 @@
         <v>197</v>
       </c>
       <c r="F99" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B100" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C100" t="s">
         <v>198</v>
@@ -3395,12 +3399,12 @@
         <v>199</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B101" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C101" t="s">
         <v>200</v>
@@ -3409,12 +3413,12 @@
         <v>201</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B102" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C102" t="s">
         <v>202</v>
@@ -3423,12 +3427,12 @@
         <v>203</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B103" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C103" t="s">
         <v>204</v>
@@ -3437,12 +3441,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B104" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C104" t="s">
         <v>114</v>
@@ -3451,12 +3455,12 @@
         <v>206</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B105" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C105" t="s">
         <v>207</v>
@@ -3465,12 +3469,12 @@
         <v>208</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B106" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C106" t="s">
         <v>209</v>
@@ -3479,12 +3483,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B107" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C107" t="s">
         <v>211</v>
@@ -3493,12 +3497,12 @@
         <v>212</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B108" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C108" t="s">
         <v>213</v>
@@ -3507,12 +3511,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B109" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C109" t="s">
         <v>215</v>
@@ -3521,12 +3525,12 @@
         <v>216</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B110" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C110" t="s">
         <v>217</v>
@@ -3535,12 +3539,12 @@
         <v>218</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B111" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C111" t="s">
         <v>219</v>
@@ -3549,12 +3553,12 @@
         <v>220</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B112" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C112" t="s">
         <v>221</v>
@@ -3563,12 +3567,12 @@
         <v>222</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B113" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C113" t="s">
         <v>223</v>
@@ -3577,15 +3581,15 @@
         <v>224</v>
       </c>
       <c r="F113" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B114" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C114" t="s">
         <v>133</v>
@@ -3594,12 +3598,12 @@
         <v>225</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B115" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C115" t="s">
         <v>226</v>
@@ -3608,15 +3612,15 @@
         <v>227</v>
       </c>
       <c r="F115" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B116" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C116" t="s">
         <v>228</v>
@@ -3625,12 +3629,12 @@
         <v>229</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B117" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C117" t="s">
         <v>230</v>
@@ -3639,12 +3643,12 @@
         <v>231</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B118" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C118" t="s">
         <v>232</v>
@@ -3653,12 +3657,12 @@
         <v>233</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B119" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C119" t="s">
         <v>234</v>
@@ -3667,12 +3671,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B120" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C120" t="s">
         <v>236</v>
@@ -3681,12 +3685,12 @@
         <v>237</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B121" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C121" t="s">
         <v>238</v>
@@ -3695,12 +3699,12 @@
         <v>239</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B122" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C122" t="s">
         <v>240</v>
@@ -3709,12 +3713,12 @@
         <v>241</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B123" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C123" t="s">
         <v>242</v>
@@ -3723,12 +3727,12 @@
         <v>243</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B124" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C124" t="s">
         <v>244</v>
@@ -3737,12 +3741,12 @@
         <v>245</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B125" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C125" t="s">
         <v>246</v>
@@ -3751,15 +3755,15 @@
         <v>247</v>
       </c>
       <c r="F125" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B126" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C126" t="s">
         <v>248</v>
@@ -3768,12 +3772,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B127" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C127" t="s">
         <v>250</v>
@@ -3782,12 +3786,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B128" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C128" t="s">
         <v>252</v>
@@ -3796,12 +3800,12 @@
         <v>253</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B129" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C129" t="s">
         <v>254</v>
@@ -3810,12 +3814,12 @@
         <v>255</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B130" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C130" t="s">
         <v>256</v>
@@ -3824,12 +3828,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B131" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C131" t="s">
         <v>258</v>
@@ -3838,12 +3842,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B132" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C132" t="s">
         <v>260</v>
@@ -3852,12 +3856,12 @@
         <v>261</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B133" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C133" t="s">
         <v>262</v>
@@ -3866,12 +3870,12 @@
         <v>263</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B134" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C134" t="s">
         <v>264</v>
@@ -3880,12 +3884,12 @@
         <v>265</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B135" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C135" t="s">
         <v>266</v>
@@ -3894,12 +3898,12 @@
         <v>267</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B136" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C136" t="s">
         <v>268</v>
@@ -3908,12 +3912,12 @@
         <v>269</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B137" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C137" t="s">
         <v>270</v>
@@ -3922,12 +3926,12 @@
         <v>271</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B138" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C138" t="s">
         <v>272</v>
@@ -3936,12 +3940,12 @@
         <v>273</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B139" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C139" t="s">
         <v>274</v>
@@ -3950,12 +3954,12 @@
         <v>275</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B140" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C140" t="s">
         <v>276</v>
@@ -3964,12 +3968,12 @@
         <v>277</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B141" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C141" t="s">
         <v>278</v>
@@ -3978,12 +3982,12 @@
         <v>279</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B142" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C142" t="s">
         <v>280</v>
@@ -3992,12 +3996,12 @@
         <v>281</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B143" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C143" t="s">
         <v>207</v>
@@ -4006,12 +4010,12 @@
         <v>282</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B144" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C144" t="s">
         <v>283</v>
@@ -4020,12 +4024,12 @@
         <v>284</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B145" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C145" t="s">
         <v>285</v>
@@ -4034,12 +4038,12 @@
         <v>286</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B146" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C146" t="s">
         <v>123</v>
@@ -4048,12 +4052,12 @@
         <v>287</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B147" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C147" t="s">
         <v>288</v>
@@ -4062,12 +4066,12 @@
         <v>289</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B148" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C148" t="s">
         <v>290</v>
@@ -4076,12 +4080,12 @@
         <v>291</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B149" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C149" t="s">
         <v>292</v>
@@ -4090,12 +4094,12 @@
         <v>293</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B150" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C150" t="s">
         <v>294</v>
@@ -4104,15 +4108,15 @@
         <v>295</v>
       </c>
       <c r="F150" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B151" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C151" t="s">
         <v>234</v>
@@ -4121,12 +4125,12 @@
         <v>296</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B152" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C152" t="s">
         <v>297</v>
@@ -4135,15 +4139,15 @@
         <v>298</v>
       </c>
       <c r="F152" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B153" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C153" t="s">
         <v>299</v>
@@ -4152,12 +4156,12 @@
         <v>300</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B154" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C154" t="s">
         <v>301</v>
@@ -4166,12 +4170,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B155" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C155" t="s">
         <v>303</v>
@@ -4180,272 +4184,272 @@
         <v>304</v>
       </c>
       <c r="F155" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B156" t="s">
+        <v>484</v>
+      </c>
+      <c r="C156" t="s">
         <v>485</v>
       </c>
-      <c r="C156" t="s">
+      <c r="E156" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="E156" s="3" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B157" t="s">
         <v>467</v>
       </c>
-      <c r="B157" t="s">
-        <v>468</v>
-      </c>
       <c r="C157" t="s">
+        <v>480</v>
+      </c>
+      <c r="E157" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="E157" s="1" t="s">
+    </row>
+    <row r="158" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B158" t="s">
+        <v>467</v>
+      </c>
+      <c r="C158" t="s">
+        <v>478</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B159" t="s">
+        <v>467</v>
+      </c>
+      <c r="C159" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
+      <c r="E159" s="3" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B160" t="s">
         <v>467</v>
-      </c>
-      <c r="B158" t="s">
-        <v>468</v>
-      </c>
-      <c r="C158" t="s">
-        <v>479</v>
-      </c>
-      <c r="E158" s="3" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A159" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="B159" t="s">
-        <v>468</v>
-      </c>
-      <c r="C159" t="s">
-        <v>483</v>
-      </c>
-      <c r="E159" s="3" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="B160" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B161" t="s">
+        <v>364</v>
+      </c>
+      <c r="C161" t="s">
         <v>365</v>
       </c>
-      <c r="C161" t="s">
-        <v>366</v>
-      </c>
       <c r="E161" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
+        <v>360</v>
+      </c>
+      <c r="B162" t="s">
+        <v>364</v>
+      </c>
+      <c r="C162" t="s">
+        <v>366</v>
+      </c>
+      <c r="E162" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>361</v>
-      </c>
-      <c r="B162" t="s">
-        <v>365</v>
-      </c>
-      <c r="C162" t="s">
-        <v>367</v>
-      </c>
-      <c r="E162" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>362</v>
       </c>
       <c r="B163" t="s">
         <v>60</v>
       </c>
       <c r="C163" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E163" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B164" t="s">
         <v>60</v>
       </c>
       <c r="C164" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E164" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>361</v>
+      </c>
+      <c r="B165" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>362</v>
-      </c>
-      <c r="B165" t="s">
+      <c r="C165" t="s">
+        <v>325</v>
+      </c>
+      <c r="E165" t="s">
         <v>326</v>
       </c>
-      <c r="C165" t="s">
-        <v>326</v>
-      </c>
-      <c r="E165" t="s">
+    </row>
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>361</v>
+      </c>
+      <c r="B166" t="s">
+        <v>363</v>
+      </c>
+      <c r="C166" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>362</v>
-      </c>
-      <c r="B166" t="s">
-        <v>364</v>
-      </c>
-      <c r="C166" t="s">
+      <c r="E166" t="s">
         <v>328</v>
       </c>
-      <c r="E166" t="s">
+    </row>
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>361</v>
+      </c>
+      <c r="B167" t="s">
+        <v>363</v>
+      </c>
+      <c r="C167" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>362</v>
-      </c>
-      <c r="B167" t="s">
-        <v>364</v>
-      </c>
-      <c r="C167" t="s">
+      <c r="E167" t="s">
         <v>330</v>
       </c>
-      <c r="E167" t="s">
+    </row>
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>361</v>
+      </c>
+      <c r="B168" t="s">
+        <v>363</v>
+      </c>
+      <c r="C168" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>362</v>
-      </c>
-      <c r="B168" t="s">
-        <v>364</v>
-      </c>
-      <c r="C168" t="s">
+      <c r="E168" t="s">
         <v>332</v>
       </c>
-      <c r="E168" t="s">
+    </row>
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>361</v>
+      </c>
+      <c r="B169" t="s">
+        <v>363</v>
+      </c>
+      <c r="C169" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>362</v>
-      </c>
-      <c r="B169" t="s">
-        <v>364</v>
-      </c>
-      <c r="C169" t="s">
+      <c r="E169" t="s">
         <v>334</v>
       </c>
-      <c r="E169" t="s">
+    </row>
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>361</v>
+      </c>
+      <c r="B170" t="s">
+        <v>363</v>
+      </c>
+      <c r="C170" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>362</v>
-      </c>
-      <c r="B170" t="s">
-        <v>364</v>
-      </c>
-      <c r="C170" t="s">
+      <c r="E170" t="s">
         <v>336</v>
       </c>
-      <c r="E170" t="s">
+    </row>
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>361</v>
+      </c>
+      <c r="B171" t="s">
+        <v>363</v>
+      </c>
+      <c r="C171" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>362</v>
-      </c>
-      <c r="B171" t="s">
-        <v>364</v>
-      </c>
-      <c r="C171" t="s">
+      <c r="E171" t="s">
         <v>338</v>
       </c>
-      <c r="E171" t="s">
+    </row>
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>361</v>
+      </c>
+      <c r="B172" t="s">
+        <v>363</v>
+      </c>
+      <c r="C172" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>362</v>
-      </c>
-      <c r="B172" t="s">
-        <v>364</v>
-      </c>
-      <c r="C172" t="s">
+      <c r="E172" t="s">
         <v>340</v>
       </c>
-      <c r="E172" t="s">
+    </row>
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>361</v>
+      </c>
+      <c r="B173" t="s">
+        <v>363</v>
+      </c>
+      <c r="C173" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>362</v>
-      </c>
-      <c r="B173" t="s">
-        <v>364</v>
-      </c>
-      <c r="C173" t="s">
+      <c r="E173" t="s">
         <v>342</v>
       </c>
-      <c r="E173" t="s">
+    </row>
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>361</v>
+      </c>
+      <c r="B174" t="s">
+        <v>363</v>
+      </c>
+      <c r="C174" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>362</v>
-      </c>
-      <c r="B174" t="s">
-        <v>364</v>
-      </c>
-      <c r="C174" t="s">
+      <c r="E174" t="s">
         <v>344</v>
       </c>
-      <c r="E174" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B175" t="s">
         <v>1</v>
@@ -4454,32 +4458,32 @@
         <v>2</v>
       </c>
       <c r="E175" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F175" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B176" t="s">
         <v>1</v>
       </c>
       <c r="C176" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E176" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F176" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B177" t="s">
         <v>1</v>
@@ -4488,15 +4492,15 @@
         <v>217</v>
       </c>
       <c r="E177" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F177" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B178" t="s">
         <v>1</v>
@@ -4505,930 +4509,930 @@
         <v>22</v>
       </c>
       <c r="E178" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F178" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B179" t="s">
         <v>1</v>
       </c>
       <c r="C179" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E179" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F179" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B180" t="s">
         <v>1</v>
       </c>
       <c r="C180" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E180" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F180" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B181" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C181" t="s">
         <v>114</v>
       </c>
       <c r="E181" t="s">
+        <v>392</v>
+      </c>
+      <c r="F181" t="s">
         <v>393</v>
       </c>
-      <c r="F181" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B182" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C182" t="s">
         <v>56</v>
       </c>
       <c r="E182" t="s">
+        <v>394</v>
+      </c>
+      <c r="F182" t="s">
         <v>395</v>
       </c>
-      <c r="F182" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B183" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C183" t="s">
         <v>58</v>
       </c>
       <c r="E183" t="s">
+        <v>396</v>
+      </c>
+      <c r="F183" t="s">
         <v>397</v>
       </c>
-      <c r="F183" t="s">
+    </row>
+    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>362</v>
+      </c>
+      <c r="B184" t="s">
+        <v>305</v>
+      </c>
+      <c r="C184" t="s">
+        <v>431</v>
+      </c>
+      <c r="E184" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>363</v>
-      </c>
-      <c r="B184" t="s">
-        <v>306</v>
-      </c>
-      <c r="C184" t="s">
-        <v>432</v>
-      </c>
-      <c r="E184" t="s">
+      <c r="F184" t="s">
         <v>399</v>
       </c>
-      <c r="F184" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B185" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C185" t="s">
         <v>60</v>
       </c>
       <c r="E185" t="s">
+        <v>400</v>
+      </c>
+      <c r="F185" t="s">
         <v>401</v>
       </c>
-      <c r="F185" t="s">
+    </row>
+    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>362</v>
+      </c>
+      <c r="B186" t="s">
+        <v>305</v>
+      </c>
+      <c r="C186" t="s">
+        <v>433</v>
+      </c>
+      <c r="E186" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>363</v>
-      </c>
-      <c r="B186" t="s">
-        <v>306</v>
-      </c>
-      <c r="C186" t="s">
-        <v>434</v>
-      </c>
-      <c r="E186" t="s">
+      <c r="F186" t="s">
         <v>403</v>
       </c>
-      <c r="F186" t="s">
+    </row>
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>362</v>
+      </c>
+      <c r="B187" t="s">
+        <v>305</v>
+      </c>
+      <c r="C187" t="s">
+        <v>432</v>
+      </c>
+      <c r="E187" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>363</v>
-      </c>
-      <c r="B187" t="s">
-        <v>306</v>
-      </c>
-      <c r="C187" t="s">
-        <v>433</v>
-      </c>
-      <c r="E187" t="s">
+      <c r="F187" t="s">
         <v>405</v>
       </c>
-      <c r="F187" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B188" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C188" t="s">
         <v>176</v>
       </c>
       <c r="E188" t="s">
+        <v>406</v>
+      </c>
+      <c r="F188" t="s">
         <v>407</v>
       </c>
-      <c r="F188" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B189" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C189" t="s">
         <v>86</v>
       </c>
       <c r="E189" t="s">
+        <v>408</v>
+      </c>
+      <c r="F189" t="s">
         <v>409</v>
       </c>
-      <c r="F189" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B190" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C190" t="s">
         <v>92</v>
       </c>
       <c r="E190" t="s">
+        <v>410</v>
+      </c>
+      <c r="F190" t="s">
         <v>411</v>
       </c>
-      <c r="F190" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B191" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C191" t="s">
         <v>114</v>
       </c>
       <c r="E191" t="s">
+        <v>370</v>
+      </c>
+      <c r="F191" t="s">
         <v>371</v>
       </c>
-      <c r="F191" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B192" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C192" t="s">
         <v>56</v>
       </c>
       <c r="E192" t="s">
+        <v>372</v>
+      </c>
+      <c r="F192" t="s">
         <v>373</v>
       </c>
-      <c r="F192" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B193" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C193" t="s">
         <v>117</v>
       </c>
       <c r="E193" t="s">
+        <v>374</v>
+      </c>
+      <c r="F193" t="s">
         <v>375</v>
       </c>
-      <c r="F193" t="s">
+    </row>
+    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>362</v>
+      </c>
+      <c r="B194" t="s">
+        <v>306</v>
+      </c>
+      <c r="C194" t="s">
+        <v>432</v>
+      </c>
+      <c r="E194" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>363</v>
-      </c>
-      <c r="B194" t="s">
-        <v>307</v>
-      </c>
-      <c r="C194" t="s">
-        <v>433</v>
-      </c>
-      <c r="E194" t="s">
+      <c r="F194" t="s">
         <v>377</v>
       </c>
-      <c r="F194" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B195" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C195" t="s">
         <v>133</v>
       </c>
       <c r="E195" t="s">
+        <v>378</v>
+      </c>
+      <c r="F195" t="s">
         <v>379</v>
       </c>
-      <c r="F195" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B196" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C196" t="s">
         <v>143</v>
       </c>
       <c r="E196" t="s">
+        <v>380</v>
+      </c>
+      <c r="F196" t="s">
         <v>381</v>
       </c>
-      <c r="F196" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B197" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C197" t="s">
         <v>92</v>
       </c>
       <c r="E197" t="s">
+        <v>382</v>
+      </c>
+      <c r="F197" t="s">
         <v>383</v>
       </c>
-      <c r="F197" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B198" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C198" t="s">
         <v>164</v>
       </c>
       <c r="E198" t="s">
+        <v>384</v>
+      </c>
+      <c r="F198" t="s">
         <v>385</v>
       </c>
-      <c r="F198" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B199" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C199" t="s">
         <v>168</v>
       </c>
       <c r="E199" t="s">
+        <v>386</v>
+      </c>
+      <c r="F199" t="s">
         <v>387</v>
       </c>
-      <c r="F199" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B200" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C200" t="s">
         <v>176</v>
       </c>
       <c r="E200" t="s">
+        <v>388</v>
+      </c>
+      <c r="F200" t="s">
         <v>389</v>
       </c>
-      <c r="F200" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B201" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C201" t="s">
         <v>179</v>
       </c>
       <c r="E201" t="s">
+        <v>390</v>
+      </c>
+      <c r="F201" t="s">
         <v>391</v>
       </c>
-      <c r="F201" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B202" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C202" t="s">
         <v>192</v>
       </c>
       <c r="E202" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F202" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B203" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C203" t="s">
         <v>114</v>
       </c>
       <c r="E203" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F203" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B204" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C204" t="s">
         <v>207</v>
       </c>
       <c r="E204" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F204" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B205" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C205" t="s">
         <v>215</v>
       </c>
       <c r="E205" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F205" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B206" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C206" t="s">
         <v>219</v>
       </c>
       <c r="E206" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F206" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B207" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C207" t="s">
         <v>228</v>
       </c>
       <c r="E207" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F207" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B208" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C208" t="s">
         <v>236</v>
       </c>
       <c r="E208" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F208" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B209" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C209" t="s">
         <v>232</v>
       </c>
       <c r="E209" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F209" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B210" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C210" t="s">
         <v>264</v>
       </c>
       <c r="E210" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F210" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B211" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C211" t="s">
         <v>280</v>
       </c>
       <c r="E211" t="s">
+        <v>414</v>
+      </c>
+      <c r="F211" t="s">
         <v>415</v>
       </c>
-      <c r="F211" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B212" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C212" t="s">
         <v>207</v>
       </c>
       <c r="E212" t="s">
+        <v>416</v>
+      </c>
+      <c r="F212" t="s">
         <v>417</v>
       </c>
-      <c r="F212" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B213" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C213" t="s">
         <v>283</v>
       </c>
       <c r="E213" t="s">
+        <v>418</v>
+      </c>
+      <c r="F213" t="s">
         <v>419</v>
       </c>
-      <c r="F213" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B214" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C214" t="s">
         <v>285</v>
       </c>
       <c r="E214" t="s">
+        <v>420</v>
+      </c>
+      <c r="F214" t="s">
         <v>421</v>
       </c>
-      <c r="F214" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B215" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C215" t="s">
         <v>292</v>
       </c>
       <c r="E215" t="s">
+        <v>422</v>
+      </c>
+      <c r="F215" t="s">
         <v>423</v>
       </c>
-      <c r="F215" t="s">
+    </row>
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>428</v>
+      </c>
+      <c r="B216" t="s">
+        <v>430</v>
+      </c>
+      <c r="C216" t="s">
+        <v>435</v>
+      </c>
+      <c r="E216" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
+      <c r="F216" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>428</v>
+      </c>
+      <c r="B217" t="s">
+        <v>308</v>
+      </c>
+      <c r="C217" t="s">
+        <v>308</v>
+      </c>
+      <c r="E217" t="s">
+        <v>426</v>
+      </c>
+      <c r="F217" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
         <v>429</v>
       </c>
-      <c r="B216" t="s">
-        <v>431</v>
-      </c>
-      <c r="C216" t="s">
-        <v>436</v>
-      </c>
-      <c r="E216" t="s">
-        <v>425</v>
-      </c>
-      <c r="F216" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
+      <c r="B218" t="s">
+        <v>434</v>
+      </c>
+      <c r="C218" t="s">
+        <v>434</v>
+      </c>
+      <c r="E218" t="s">
+        <v>412</v>
+      </c>
+      <c r="F218" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
         <v>429</v>
       </c>
-      <c r="B217" t="s">
-        <v>309</v>
-      </c>
-      <c r="C217" t="s">
-        <v>309</v>
-      </c>
-      <c r="E217" t="s">
-        <v>427</v>
-      </c>
-      <c r="F217" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>430</v>
-      </c>
-      <c r="B218" t="s">
-        <v>435</v>
-      </c>
-      <c r="C218" t="s">
-        <v>435</v>
-      </c>
-      <c r="E218" t="s">
-        <v>413</v>
-      </c>
-      <c r="F218" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>430</v>
-      </c>
       <c r="B219" t="s">
+        <v>447</v>
+      </c>
+      <c r="C219" t="s">
         <v>448</v>
       </c>
-      <c r="C219" t="s">
+      <c r="E219" t="s">
         <v>449</v>
       </c>
-      <c r="E219" t="s">
+      <c r="F219" t="s">
         <v>450</v>
       </c>
-      <c r="F219" t="s">
+    </row>
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>429</v>
+      </c>
+      <c r="B220" t="s">
+        <v>447</v>
+      </c>
+      <c r="C220" t="s">
+        <v>453</v>
+      </c>
+      <c r="E220" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
-        <v>430</v>
-      </c>
-      <c r="B220" t="s">
-        <v>448</v>
-      </c>
-      <c r="C220" t="s">
+      <c r="F220" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>429</v>
+      </c>
+      <c r="B221" t="s">
+        <v>447</v>
+      </c>
+      <c r="C221" t="s">
         <v>454</v>
       </c>
-      <c r="E220" t="s">
-        <v>452</v>
-      </c>
-      <c r="F220" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>430</v>
-      </c>
-      <c r="B221" t="s">
-        <v>448</v>
-      </c>
-      <c r="C221" t="s">
+      <c r="E221" t="s">
         <v>455</v>
       </c>
-      <c r="E221" t="s">
+      <c r="F221" t="s">
         <v>456</v>
       </c>
-      <c r="F221" t="s">
+    </row>
+    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>429</v>
+      </c>
+      <c r="B222" t="s">
+        <v>447</v>
+      </c>
+      <c r="C222" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
-        <v>430</v>
-      </c>
-      <c r="B222" t="s">
-        <v>448</v>
-      </c>
-      <c r="C222" t="s">
+      <c r="E222" t="s">
         <v>458</v>
       </c>
-      <c r="E222" t="s">
+      <c r="F222" t="s">
         <v>459</v>
       </c>
-      <c r="F222" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
+        <v>471</v>
+      </c>
+      <c r="B223" t="s">
+        <v>469</v>
+      </c>
+      <c r="C223" t="s">
+        <v>470</v>
+      </c>
+      <c r="E223" t="s">
         <v>472</v>
       </c>
-      <c r="B223" t="s">
+    </row>
+    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A224" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B224" t="s">
+        <v>469</v>
+      </c>
+      <c r="C224" t="s">
+        <v>475</v>
+      </c>
+      <c r="E224" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B225" t="s">
+        <v>469</v>
+      </c>
+      <c r="C225" t="s">
         <v>470</v>
       </c>
-      <c r="C223" t="s">
-        <v>471</v>
-      </c>
-      <c r="E223" t="s">
+      <c r="E225" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A224" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="B224" t="s">
-        <v>470</v>
-      </c>
-      <c r="C224" t="s">
+      <c r="B226" t="s">
+        <v>469</v>
+      </c>
+      <c r="C226" t="s">
+        <v>475</v>
+      </c>
+      <c r="E226" t="s">
         <v>476</v>
       </c>
-      <c r="E224" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A225" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="B225" t="s">
-        <v>470</v>
-      </c>
-      <c r="C225" t="s">
-        <v>471</v>
-      </c>
-      <c r="E225" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A226" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="B226" t="s">
-        <v>470</v>
-      </c>
-      <c r="C226" t="s">
-        <v>476</v>
-      </c>
-      <c r="E226" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="227" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B227" t="s">
         <v>491</v>
       </c>
-      <c r="B227" t="s">
+      <c r="C227" t="s">
+        <v>500</v>
+      </c>
+      <c r="E227" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="F227" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B228" t="s">
+        <v>491</v>
+      </c>
+      <c r="C228" t="s">
+        <v>501</v>
+      </c>
+      <c r="E228" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="F228" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B229" t="s">
+        <v>491</v>
+      </c>
+      <c r="C229" t="s">
+        <v>504</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B230" t="s">
         <v>492</v>
       </c>
-      <c r="C227" t="s">
-        <v>501</v>
-      </c>
-      <c r="E227" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="F227" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A228" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="B228" t="s">
+      <c r="C230" t="s">
+        <v>493</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="F230" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B231" t="s">
         <v>492</v>
       </c>
-      <c r="C228" t="s">
-        <v>502</v>
-      </c>
-      <c r="E228" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="F228" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A229" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="B229" t="s">
+      <c r="C231" t="s">
+        <v>494</v>
+      </c>
+      <c r="E231" t="s">
+        <v>507</v>
+      </c>
+      <c r="F231" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B232" t="s">
         <v>492</v>
       </c>
-      <c r="C229" t="s">
-        <v>505</v>
-      </c>
-      <c r="E229" s="3" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A230" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="B230" t="s">
+      <c r="C232" t="s">
         <v>493</v>
       </c>
-      <c r="C230" t="s">
+      <c r="E232" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="F232" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>495</v>
+      </c>
+      <c r="B233" t="s">
+        <v>492</v>
+      </c>
+      <c r="C233" t="s">
         <v>494</v>
       </c>
-      <c r="E230" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="F230" t="s">
+      <c r="E233" t="s">
+        <v>509</v>
+      </c>
+      <c r="F233" t="s">
         <v>497</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A231" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="B231" t="s">
-        <v>493</v>
-      </c>
-      <c r="C231" t="s">
-        <v>495</v>
-      </c>
-      <c r="E231" t="s">
-        <v>508</v>
-      </c>
-      <c r="F231" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A232" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="B232" t="s">
-        <v>493</v>
-      </c>
-      <c r="C232" t="s">
-        <v>494</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="F232" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
-        <v>496</v>
-      </c>
-      <c r="B233" t="s">
-        <v>493</v>
-      </c>
-      <c r="C233" t="s">
-        <v>495</v>
-      </c>
-      <c r="E233" t="s">
-        <v>510</v>
-      </c>
-      <c r="F233" t="s">
-        <v>498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix snippen close #667
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -1535,7 +1535,44 @@
     <t>Thumbnail IMG tag with crop-mode</t>
   </si>
   <si>
-    <t>@foreach(var ${3:pic} in Adam(${1:var}, "${2:prop}").Files){
+    <t>Adam: Large example with looping ADAM assets</t>
+  </si>
+  <si>
+    <t>simple loop for assets</t>
+  </si>
+  <si>
+    <t>loop with metadata assets</t>
+  </si>
+  <si>
+    <t>Adam: simple example with looping ADAM assets</t>
+  </si>
+  <si>
+    <t>loop with type filter</t>
+  </si>
+  <si>
+    <t>@foreach(var ${3:pic} in (AsAdam(${1:var}, "${2:prop}").Files as IEnumerable&lt;ToSic.SexyContent.Adam.AdamFile&gt;).Where(f =&gt; f.Type == "${4:image}")){
+ &lt;span&gt;@${3:pic}.Url, @${3:pic}.FileName &lt;/span&gt;
+}</t>
+  </si>
+  <si>
+    <t>@${101:var}.${102:prop}?w=${1:200}&amp;h=${2:200}&amp;mode=${3:crop}</t>
+  </si>
+  <si>
+    <t>&lt;img src="@${101:var}.${102:prop}?w=${1:200}&amp;h=${2:200}&amp;mode=${3:crop}"&gt;</t>
+  </si>
+  <si>
+    <t>[${101:var}:${102:prop}]?w=${1:200}&amp;h=${2:200}&amp;mode=${3:crop}</t>
+  </si>
+  <si>
+    <t>&lt;img src="[${101:var}:${102:prop}]?w=${1:200}&amp;h=${2:200}&amp;mode=${3:crop}"&gt;</t>
+  </si>
+  <si>
+    <t>@foreach(var ${3:pic} in AsAdam(${1:var}, "${2:prop}").Files){
+ &lt;span&gt;@${3:pic}.Url, @${3:pic}.FileName &lt;/span&gt;
+}</t>
+  </si>
+  <si>
+    <t>@foreach(var ${3:pic} in AsAdam(${1:var}, "${2:prop}").Files){
  &lt;div style="clear: both"&gt;
   &lt;img src="@${3:pic}.Url?w=200&amp;h=200&amp;mode=crop" title="@${3:pic}.FileName" style="float: right"&gt;
   &lt;h3&gt;@${3:pic}.Metadata.${10:Title}&lt;/h3&gt;
@@ -1543,43 +1580,6 @@
   &lt;div&gt;Description: @Html.Raw(${3:pic}.Metadata.${11:Description})&lt;/div&gt;
  &lt;/div&gt;
 }</t>
-  </si>
-  <si>
-    <t>Adam: Large example with looping ADAM assets</t>
-  </si>
-  <si>
-    <t>simple loop for assets</t>
-  </si>
-  <si>
-    <t>loop with metadata assets</t>
-  </si>
-  <si>
-    <t>@foreach(var ${3:pic} in Adam(${1:var}, "${2:prop}").Files){
- &lt;span&gt;@${3:pic}.Url, @${3:pic}.FileName &lt;/span&gt;
-}</t>
-  </si>
-  <si>
-    <t>Adam: simple example with looping ADAM assets</t>
-  </si>
-  <si>
-    <t>loop with type filter</t>
-  </si>
-  <si>
-    <t>@foreach(var ${3:pic} in (AsAdam(${1:var}, "${2:prop}").Files as IEnumerable&lt;ToSic.SexyContent.Adam.AdamFile&gt;).Where(f =&gt; f.Type == "${4:image}")){
- &lt;span&gt;@${3:pic}.Url, @${3:pic}.FileName &lt;/span&gt;
-}</t>
-  </si>
-  <si>
-    <t>@${101:var}.${102:prop}?w=${1:200}&amp;h=${2:200}&amp;mode=${3:crop}</t>
-  </si>
-  <si>
-    <t>&lt;img src="@${101:var}.${102:prop}?w=${1:200}&amp;h=${2:200}&amp;mode=${3:crop}"&gt;</t>
-  </si>
-  <si>
-    <t>[${101:var}:${102:prop}]?w=${1:200}&amp;h=${2:200}&amp;mode=${3:crop}</t>
-  </si>
-  <si>
-    <t>&lt;img src="[${101:var}:${102:prop}]?w=${1:200}&amp;h=${2:200}&amp;mode=${3:crop}"&gt;</t>
   </si>
 </sst>
 </file>
@@ -1921,8 +1921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F233"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="E229" sqref="E229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5320,13 +5320,13 @@
         <v>491</v>
       </c>
       <c r="C227" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E227" s="3" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="F227" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="228" spans="1:6" ht="150" x14ac:dyDescent="0.25">
@@ -5337,13 +5337,13 @@
         <v>491</v>
       </c>
       <c r="C228" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E228" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="F228" t="s">
         <v>498</v>
-      </c>
-      <c r="F228" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="229" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -5354,10 +5354,10 @@
         <v>491</v>
       </c>
       <c r="C229" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E229" s="3" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -5371,7 +5371,7 @@
         <v>493</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="F230" t="s">
         <v>496</v>
@@ -5388,7 +5388,7 @@
         <v>494</v>
       </c>
       <c r="E231" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F231" t="s">
         <v>497</v>
@@ -5405,7 +5405,7 @@
         <v>493</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F232" t="s">
         <v>496</v>
@@ -5422,7 +5422,7 @@
         <v>494</v>
       </c>
       <c r="E233" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="F233" t="s">
         <v>497</v>

</xml_diff>

<commit_message>
added @Html.Raw snippet - close #672
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="514">
   <si>
     <t>set</t>
   </si>
@@ -1580,6 +1580,18 @@
   &lt;div&gt;Description: @Html.Raw(${3:pic}.Metadata.${11:Description})&lt;/div&gt;
  &lt;/div&gt;
 }</t>
+  </si>
+  <si>
+    <t>string-wysiwyg</t>
+  </si>
+  <si>
+    <t>raw html</t>
+  </si>
+  <si>
+    <t>@Html.Raw(${101:var}.${102:prop})</t>
+  </si>
+  <si>
+    <t>Output the html as html, not as text</t>
   </si>
 </sst>
 </file>
@@ -1642,8 +1654,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F233" totalsRowShown="0">
-  <autoFilter ref="A1:F233"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F234" totalsRowShown="0">
+  <autoFilter ref="A1:F234"/>
   <tableColumns count="6">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -1919,15 +1931,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F233"/>
+  <dimension ref="A1:F234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="E229" sqref="E229"/>
+    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="D229" sqref="D229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="32.28515625" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
@@ -5396,35 +5408,52 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="B232" t="s">
-        <v>492</v>
+        <v>510</v>
       </c>
       <c r="C232" t="s">
-        <v>493</v>
+        <v>511</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="F232" t="s">
-        <v>496</v>
+        <v>513</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
+      <c r="A233" s="1" t="s">
         <v>495</v>
       </c>
       <c r="B233" t="s">
         <v>492</v>
       </c>
       <c r="C233" t="s">
+        <v>493</v>
+      </c>
+      <c r="E233" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="F233" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>495</v>
+      </c>
+      <c r="B234" t="s">
+        <v>492</v>
+      </c>
+      <c r="C234" t="s">
         <v>494</v>
       </c>
-      <c r="E233" t="s">
+      <c r="E234" t="s">
         <v>507</v>
       </c>
-      <c r="F233" t="s">
+      <c r="F234" t="s">
         <v>497</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Provide a quick command to see if user has edit-permissions - usually for creating toolbars... - close #674
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="516">
   <si>
     <t>set</t>
   </si>
@@ -1592,6 +1592,16 @@
   </si>
   <si>
     <t>Output the html as html, not as text</t>
+  </si>
+  <si>
+    <t>UserMayEditContent</t>
+  </si>
+  <si>
+    <t>@if(Environment.Permissions.UserMayEditContent)
+{
+       &lt;!-- stuff, like a custom edit toolbar - here an example --&gt;
+       &lt;ul class="sc-menu" data-toolbar='{ "action": "new", "contentType": "Gallery Image", "prefill": { "File": "File:@c.Image.FileId" } }'&gt;&lt;/ul&gt;
+}</t>
   </si>
 </sst>
 </file>
@@ -1654,8 +1664,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F234" totalsRowShown="0">
-  <autoFilter ref="A1:F234"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F235" totalsRowShown="0">
+  <autoFilter ref="A1:F235">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="@\InputType"/>
+        <filter val="@App"/>
+        <filter val="@C#"/>
+        <filter val="@Content"/>
+        <filter val="@DnnRazor"/>
+        <filter val="@Html"/>
+        <filter val="@List"/>
+        <filter val="@User"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -1931,10 +1954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F234"/>
+  <dimension ref="A1:F235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="D229" sqref="D229"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="E158" sqref="E158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4206,21 +4229,21 @@
         <v>486</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>466</v>
+        <v>446</v>
       </c>
       <c r="B157" t="s">
-        <v>467</v>
+        <v>484</v>
       </c>
       <c r="C157" t="s">
-        <v>480</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>466</v>
       </c>
@@ -4228,13 +4251,13 @@
         <v>467</v>
       </c>
       <c r="C158" t="s">
-        <v>478</v>
-      </c>
-      <c r="E158" s="3" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>466</v>
       </c>
@@ -4242,35 +4265,35 @@
         <v>467</v>
       </c>
       <c r="C159" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>466</v>
       </c>
       <c r="B160" t="s">
         <v>467</v>
       </c>
+      <c r="C160" t="s">
+        <v>482</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>360</v>
+      <c r="A161" s="1" t="s">
+        <v>466</v>
       </c>
       <c r="B161" t="s">
-        <v>364</v>
-      </c>
-      <c r="C161" t="s">
-        <v>365</v>
-      </c>
-      <c r="E161" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>360</v>
       </c>
@@ -4278,27 +4301,27 @@
         <v>364</v>
       </c>
       <c r="C162" t="s">
+        <v>365</v>
+      </c>
+      <c r="E162" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>360</v>
+      </c>
+      <c r="B163" t="s">
+        <v>364</v>
+      </c>
+      <c r="C163" t="s">
         <v>366</v>
       </c>
-      <c r="E162" t="s">
+      <c r="E163" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>361</v>
-      </c>
-      <c r="B163" t="s">
-        <v>60</v>
-      </c>
-      <c r="C163" t="s">
-        <v>460</v>
-      </c>
-      <c r="E163" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>361</v>
       </c>
@@ -4306,41 +4329,41 @@
         <v>60</v>
       </c>
       <c r="C164" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E164" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>361</v>
       </c>
       <c r="B165" t="s">
-        <v>325</v>
+        <v>60</v>
       </c>
       <c r="C165" t="s">
-        <v>325</v>
+        <v>461</v>
       </c>
       <c r="E165" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>361</v>
       </c>
       <c r="B166" t="s">
-        <v>363</v>
+        <v>325</v>
       </c>
       <c r="C166" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E166" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>361</v>
       </c>
@@ -4348,13 +4371,13 @@
         <v>363</v>
       </c>
       <c r="C167" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E167" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>361</v>
       </c>
@@ -4362,13 +4385,13 @@
         <v>363</v>
       </c>
       <c r="C168" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E168" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>361</v>
       </c>
@@ -4376,13 +4399,13 @@
         <v>363</v>
       </c>
       <c r="C169" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E169" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>361</v>
       </c>
@@ -4390,13 +4413,13 @@
         <v>363</v>
       </c>
       <c r="C170" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E170" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>361</v>
       </c>
@@ -4404,13 +4427,13 @@
         <v>363</v>
       </c>
       <c r="C171" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E171" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>361</v>
       </c>
@@ -4418,13 +4441,13 @@
         <v>363</v>
       </c>
       <c r="C172" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E172" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>361</v>
       </c>
@@ -4432,13 +4455,13 @@
         <v>363</v>
       </c>
       <c r="C173" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E173" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>361</v>
       </c>
@@ -4446,30 +4469,27 @@
         <v>363</v>
       </c>
       <c r="C174" t="s">
+        <v>341</v>
+      </c>
+      <c r="E174" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>361</v>
+      </c>
+      <c r="B175" t="s">
+        <v>363</v>
+      </c>
+      <c r="C175" t="s">
         <v>343</v>
       </c>
-      <c r="E174" t="s">
+      <c r="E175" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>489</v>
-      </c>
-      <c r="B175" t="s">
-        <v>1</v>
-      </c>
-      <c r="C175" t="s">
-        <v>2</v>
-      </c>
-      <c r="E175" t="s">
-        <v>345</v>
-      </c>
-      <c r="F175" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>489</v>
       </c>
@@ -4477,16 +4497,16 @@
         <v>1</v>
       </c>
       <c r="C176" t="s">
-        <v>367</v>
+        <v>2</v>
       </c>
       <c r="E176" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F176" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>489</v>
       </c>
@@ -4494,16 +4514,16 @@
         <v>1</v>
       </c>
       <c r="C177" t="s">
-        <v>217</v>
+        <v>367</v>
       </c>
       <c r="E177" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F177" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>489</v>
       </c>
@@ -4511,16 +4531,16 @@
         <v>1</v>
       </c>
       <c r="C178" t="s">
-        <v>22</v>
+        <v>217</v>
       </c>
       <c r="E178" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F178" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>489</v>
       </c>
@@ -4528,16 +4548,16 @@
         <v>1</v>
       </c>
       <c r="C179" t="s">
-        <v>368</v>
+        <v>22</v>
       </c>
       <c r="E179" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F179" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>489</v>
       </c>
@@ -4545,33 +4565,33 @@
         <v>1</v>
       </c>
       <c r="C180" t="s">
+        <v>368</v>
+      </c>
+      <c r="E180" t="s">
+        <v>349</v>
+      </c>
+      <c r="F180" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>489</v>
+      </c>
+      <c r="B181" t="s">
+        <v>1</v>
+      </c>
+      <c r="C181" t="s">
         <v>369</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E181" t="s">
         <v>350</v>
       </c>
-      <c r="F180" t="s">
+      <c r="F181" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>362</v>
-      </c>
-      <c r="B181" t="s">
-        <v>305</v>
-      </c>
-      <c r="C181" t="s">
-        <v>114</v>
-      </c>
-      <c r="E181" t="s">
-        <v>392</v>
-      </c>
-      <c r="F181" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>362</v>
       </c>
@@ -4579,16 +4599,16 @@
         <v>305</v>
       </c>
       <c r="C182" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
       <c r="E182" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F182" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>362</v>
       </c>
@@ -4596,16 +4616,16 @@
         <v>305</v>
       </c>
       <c r="C183" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E183" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F183" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>362</v>
       </c>
@@ -4613,16 +4633,16 @@
         <v>305</v>
       </c>
       <c r="C184" t="s">
-        <v>431</v>
+        <v>58</v>
       </c>
       <c r="E184" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F184" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>362</v>
       </c>
@@ -4630,16 +4650,16 @@
         <v>305</v>
       </c>
       <c r="C185" t="s">
-        <v>60</v>
+        <v>431</v>
       </c>
       <c r="E185" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F185" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>362</v>
       </c>
@@ -4647,16 +4667,16 @@
         <v>305</v>
       </c>
       <c r="C186" t="s">
-        <v>433</v>
+        <v>60</v>
       </c>
       <c r="E186" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F186" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>362</v>
       </c>
@@ -4664,16 +4684,16 @@
         <v>305</v>
       </c>
       <c r="C187" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E187" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F187" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>362</v>
       </c>
@@ -4681,16 +4701,16 @@
         <v>305</v>
       </c>
       <c r="C188" t="s">
-        <v>176</v>
+        <v>432</v>
       </c>
       <c r="E188" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F188" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>362</v>
       </c>
@@ -4698,16 +4718,16 @@
         <v>305</v>
       </c>
       <c r="C189" t="s">
-        <v>86</v>
+        <v>176</v>
       </c>
       <c r="E189" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F189" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>362</v>
       </c>
@@ -4715,33 +4735,33 @@
         <v>305</v>
       </c>
       <c r="C190" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E190" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F190" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>362</v>
       </c>
       <c r="B191" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C191" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="E191" t="s">
-        <v>370</v>
+        <v>410</v>
       </c>
       <c r="F191" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>362</v>
       </c>
@@ -4749,16 +4769,16 @@
         <v>306</v>
       </c>
       <c r="C192" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
       <c r="E192" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F192" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>362</v>
       </c>
@@ -4766,16 +4786,16 @@
         <v>306</v>
       </c>
       <c r="C193" t="s">
-        <v>117</v>
+        <v>56</v>
       </c>
       <c r="E193" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F193" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>362</v>
       </c>
@@ -4783,16 +4803,16 @@
         <v>306</v>
       </c>
       <c r="C194" t="s">
-        <v>432</v>
+        <v>117</v>
       </c>
       <c r="E194" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F194" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>362</v>
       </c>
@@ -4800,16 +4820,16 @@
         <v>306</v>
       </c>
       <c r="C195" t="s">
-        <v>133</v>
+        <v>432</v>
       </c>
       <c r="E195" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F195" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>362</v>
       </c>
@@ -4817,16 +4837,16 @@
         <v>306</v>
       </c>
       <c r="C196" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="E196" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F196" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>362</v>
       </c>
@@ -4834,16 +4854,16 @@
         <v>306</v>
       </c>
       <c r="C197" t="s">
-        <v>92</v>
+        <v>143</v>
       </c>
       <c r="E197" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F197" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>362</v>
       </c>
@@ -4851,16 +4871,16 @@
         <v>306</v>
       </c>
       <c r="C198" t="s">
-        <v>164</v>
+        <v>92</v>
       </c>
       <c r="E198" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F198" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>362</v>
       </c>
@@ -4868,16 +4888,16 @@
         <v>306</v>
       </c>
       <c r="C199" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E199" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F199" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>362</v>
       </c>
@@ -4885,16 +4905,16 @@
         <v>306</v>
       </c>
       <c r="C200" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E200" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F200" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>362</v>
       </c>
@@ -4902,33 +4922,33 @@
         <v>306</v>
       </c>
       <c r="C201" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E201" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F201" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>362</v>
       </c>
       <c r="B202" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C202" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="E202" t="s">
-        <v>351</v>
+        <v>390</v>
       </c>
       <c r="F202" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>362</v>
       </c>
@@ -4936,16 +4956,16 @@
         <v>307</v>
       </c>
       <c r="C203" t="s">
-        <v>114</v>
+        <v>192</v>
       </c>
       <c r="E203" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F203" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>362</v>
       </c>
@@ -4953,16 +4973,16 @@
         <v>307</v>
       </c>
       <c r="C204" t="s">
-        <v>207</v>
+        <v>114</v>
       </c>
       <c r="E204" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F204" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>362</v>
       </c>
@@ -4970,16 +4990,16 @@
         <v>307</v>
       </c>
       <c r="C205" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="E205" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F205" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>362</v>
       </c>
@@ -4987,16 +5007,16 @@
         <v>307</v>
       </c>
       <c r="C206" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E206" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F206" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>362</v>
       </c>
@@ -5004,16 +5024,16 @@
         <v>307</v>
       </c>
       <c r="C207" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="E207" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F207" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>362</v>
       </c>
@@ -5021,16 +5041,16 @@
         <v>307</v>
       </c>
       <c r="C208" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E208" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F208" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>362</v>
       </c>
@@ -5038,16 +5058,16 @@
         <v>307</v>
       </c>
       <c r="C209" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="E209" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F209" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>362</v>
       </c>
@@ -5055,33 +5075,33 @@
         <v>307</v>
       </c>
       <c r="C210" t="s">
+        <v>232</v>
+      </c>
+      <c r="E210" t="s">
+        <v>358</v>
+      </c>
+      <c r="F210" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>362</v>
+      </c>
+      <c r="B211" t="s">
+        <v>307</v>
+      </c>
+      <c r="C211" t="s">
         <v>264</v>
       </c>
-      <c r="E210" t="s">
+      <c r="E211" t="s">
         <v>359</v>
       </c>
-      <c r="F210" t="s">
+      <c r="F211" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>428</v>
-      </c>
-      <c r="B211" t="s">
-        <v>430</v>
-      </c>
-      <c r="C211" t="s">
-        <v>280</v>
-      </c>
-      <c r="E211" t="s">
-        <v>414</v>
-      </c>
-      <c r="F211" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>428</v>
       </c>
@@ -5089,16 +5109,16 @@
         <v>430</v>
       </c>
       <c r="C212" t="s">
-        <v>207</v>
+        <v>280</v>
       </c>
       <c r="E212" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F212" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>428</v>
       </c>
@@ -5106,16 +5126,16 @@
         <v>430</v>
       </c>
       <c r="C213" t="s">
-        <v>283</v>
+        <v>207</v>
       </c>
       <c r="E213" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F213" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>428</v>
       </c>
@@ -5123,16 +5143,16 @@
         <v>430</v>
       </c>
       <c r="C214" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E214" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F214" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>428</v>
       </c>
@@ -5140,16 +5160,16 @@
         <v>430</v>
       </c>
       <c r="C215" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="E215" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F215" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>428</v>
       </c>
@@ -5157,67 +5177,67 @@
         <v>430</v>
       </c>
       <c r="C216" t="s">
-        <v>435</v>
+        <v>292</v>
       </c>
       <c r="E216" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F216" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>428</v>
       </c>
       <c r="B217" t="s">
+        <v>430</v>
+      </c>
+      <c r="C217" t="s">
+        <v>435</v>
+      </c>
+      <c r="E217" t="s">
+        <v>424</v>
+      </c>
+      <c r="F217" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>428</v>
+      </c>
+      <c r="B218" t="s">
         <v>308</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C218" t="s">
         <v>308</v>
       </c>
-      <c r="E217" t="s">
+      <c r="E218" t="s">
         <v>426</v>
       </c>
-      <c r="F217" t="s">
+      <c r="F218" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>429</v>
-      </c>
-      <c r="B218" t="s">
-        <v>434</v>
-      </c>
-      <c r="C218" t="s">
-        <v>434</v>
-      </c>
-      <c r="E218" t="s">
-        <v>412</v>
-      </c>
-      <c r="F218" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>429</v>
       </c>
       <c r="B219" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="C219" t="s">
-        <v>448</v>
+        <v>434</v>
       </c>
       <c r="E219" t="s">
-        <v>449</v>
+        <v>412</v>
       </c>
       <c r="F219" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>429</v>
       </c>
@@ -5225,16 +5245,16 @@
         <v>447</v>
       </c>
       <c r="C220" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="E220" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F220" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>429</v>
       </c>
@@ -5242,16 +5262,16 @@
         <v>447</v>
       </c>
       <c r="C221" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E221" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="F221" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>429</v>
       </c>
@@ -5259,55 +5279,58 @@
         <v>447</v>
       </c>
       <c r="C222" t="s">
+        <v>454</v>
+      </c>
+      <c r="E222" t="s">
+        <v>455</v>
+      </c>
+      <c r="F222" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>429</v>
+      </c>
+      <c r="B223" t="s">
+        <v>447</v>
+      </c>
+      <c r="C223" t="s">
         <v>457</v>
       </c>
-      <c r="E222" t="s">
+      <c r="E223" t="s">
         <v>458</v>
       </c>
-      <c r="F222" t="s">
+      <c r="F223" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
-        <v>471</v>
-      </c>
-      <c r="B223" t="s">
-        <v>469</v>
-      </c>
-      <c r="C223" t="s">
-        <v>470</v>
-      </c>
-      <c r="E223" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A224" s="1" t="s">
+    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
         <v>471</v>
       </c>
       <c r="B224" t="s">
         <v>469</v>
       </c>
       <c r="C224" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="E224" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B225" t="s">
         <v>469</v>
       </c>
       <c r="C225" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="E225" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -5318,30 +5341,27 @@
         <v>469</v>
       </c>
       <c r="C226" t="s">
+        <v>470</v>
+      </c>
+      <c r="E226" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B227" t="s">
+        <v>469</v>
+      </c>
+      <c r="C227" t="s">
         <v>475</v>
       </c>
-      <c r="E226" t="s">
+      <c r="E227" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="227" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A227" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="B227" t="s">
-        <v>491</v>
-      </c>
-      <c r="C227" t="s">
-        <v>499</v>
-      </c>
-      <c r="E227" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="F227" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>490</v>
       </c>
@@ -5349,16 +5369,16 @@
         <v>491</v>
       </c>
       <c r="C228" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F228" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>490</v>
       </c>
@@ -5366,27 +5386,27 @@
         <v>491</v>
       </c>
       <c r="C229" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E229" s="3" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+      <c r="F229" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>490</v>
       </c>
       <c r="B230" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C230" t="s">
-        <v>493</v>
-      </c>
-      <c r="E230" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="F230" t="s">
-        <v>496</v>
+        <v>502</v>
+      </c>
+      <c r="E230" s="3" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
@@ -5397,13 +5417,13 @@
         <v>492</v>
       </c>
       <c r="C231" t="s">
-        <v>494</v>
-      </c>
-      <c r="E231" t="s">
-        <v>505</v>
+        <v>493</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>504</v>
       </c>
       <c r="F231" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
@@ -5411,49 +5431,66 @@
         <v>490</v>
       </c>
       <c r="B232" t="s">
-        <v>510</v>
+        <v>492</v>
       </c>
       <c r="C232" t="s">
-        <v>511</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>512</v>
+        <v>494</v>
+      </c>
+      <c r="E232" t="s">
+        <v>505</v>
       </c>
       <c r="F232" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="B233" t="s">
-        <v>492</v>
+        <v>510</v>
       </c>
       <c r="C233" t="s">
-        <v>493</v>
+        <v>511</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="F233" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
         <v>495</v>
       </c>
       <c r="B234" t="s">
         <v>492</v>
       </c>
       <c r="C234" t="s">
+        <v>493</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="F234" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>495</v>
+      </c>
+      <c r="B235" t="s">
+        <v>492</v>
+      </c>
+      <c r="C235" t="s">
         <v>494</v>
       </c>
-      <c r="E234" t="s">
+      <c r="E235" t="s">
         <v>507</v>
       </c>
-      <c r="F234" t="s">
+      <c r="F235" t="s">
         <v>497</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added many more snippets, incl. the new content-block snippets
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="545">
   <si>
     <t>set</t>
   </si>
@@ -1473,9 +1473,6 @@
   </si>
   <si>
     <t>using</t>
-  </si>
-  <si>
-    <t>@using ${1:System.Data.Linq}</t>
   </si>
   <si>
     <t>functions block server-side</t>
@@ -1603,11 +1600,111 @@
        &lt;ul class="sc-menu" data-toolbar='{ "action": "new", "contentType": "Gallery Image", "prefill": { "File": "File:@c.Image.FileId" } }'&gt;&lt;/ul&gt;
 }</t>
   </si>
+  <si>
+    <t>entity</t>
+  </si>
+  <si>
+    <t>entity-content-blocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div class="sc-content-block-list" @${101:var}.${102:prop}.EditContext()&gt;
+    @foreach(var contentBlock in ${101:var}.${102:prop}){
+        @contentBlock.Render()
+    }
+&lt;/div&gt;
+</t>
+  </si>
+  <si>
+    <t>Content blocks with in-page editing</t>
+  </si>
+  <si>
+    <t>content block with inpage editing</t>
+  </si>
+  <si>
+    <t>render entity</t>
+  </si>
+  <si>
+    <t>@${101:var}.render()</t>
+  </si>
+  <si>
+    <t>loop through items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@foreach(var ${103:item} in ${101:var}.${102:prop}){
+    @${103:item}.Render()
+}
+</t>
+  </si>
+  <si>
+    <t>Render a content-block entity (remember that you can't render the list, this only renders one item).
+Note that if you try to render any kind of entity, this will not throw an error, but just render an HTML comment as there is no definition for how to render other types of entities as of now.</t>
+  </si>
+  <si>
+    <t>edit context</t>
+  </si>
+  <si>
+    <t>@${101:var}.${102:prop}.EditContext()</t>
+  </si>
+  <si>
+    <t>This should be used inside a &lt;div&gt; tag to provide additional information to the in-page editing ui</t>
+  </si>
+  <si>
+    <t>item count</t>
+  </si>
+  <si>
+    <t>@${101:var}.${102:prop}.Count</t>
+  </si>
+  <si>
+    <t>get first item</t>
+  </si>
+  <si>
+    <t>@${101:var}.${102:prop}[0]</t>
+  </si>
+  <si>
+    <t>using 2sxc namespace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@using ToSic.SexyContent;
+</t>
+  </si>
+  <si>
+    <t>using Linq</t>
+  </si>
+  <si>
+    <t>@using System.Linq;</t>
+  </si>
+  <si>
+    <t>@using ${1:System.Linq}</t>
+  </si>
+  <si>
+    <t>The 2sxc namespace, in case you explicitly want to work with 2sxc objects</t>
+  </si>
+  <si>
+    <t>get item number 0</t>
+  </si>
+  <si>
+    <t>This will give you the count of items</t>
+  </si>
+  <si>
+    <t>Note that this only works, if there are items, otherwise you'll get an error</t>
+  </si>
+  <si>
+    <t>This also requires a @using Tosic.SexyContent; at the beginning of your cshtml</t>
+  </si>
+  <si>
+    <t>show title of first item if exists</t>
+  </si>
+  <si>
+    <t>@(${1:var}.${2:prop} as ToSic.SexyContent.DynamicEntityList).FirstOrDefault()?.Title</t>
+  </si>
+  <si>
+    <t>This is a shorthand for try-to-get-and-if-null-don’t-show</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1664,21 +1761,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F235" totalsRowShown="0">
-  <autoFilter ref="A1:F235">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="@\InputType"/>
-        <filter val="@App"/>
-        <filter val="@C#"/>
-        <filter val="@Content"/>
-        <filter val="@DnnRazor"/>
-        <filter val="@Html"/>
-        <filter val="@List"/>
-        <filter val="@User"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F245" totalsRowShown="0">
+  <autoFilter ref="A1:F245"/>
   <tableColumns count="6">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -1954,10 +2038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F235"/>
+  <dimension ref="A1:F245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="E158" sqref="E158"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="C246" sqref="C246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1992,7 +2076,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2012,7 +2096,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -2032,7 +2116,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -2052,7 +2136,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -2072,7 +2156,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -2092,7 +2176,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -2183,7 +2267,7 @@
         <v>468</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -4220,13 +4304,13 @@
         <v>446</v>
       </c>
       <c r="B156" t="s">
+        <v>483</v>
+      </c>
+      <c r="C156" t="s">
         <v>484</v>
       </c>
-      <c r="C156" t="s">
+      <c r="E156" s="3" t="s">
         <v>485</v>
-      </c>
-      <c r="E156" s="3" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -4234,13 +4318,13 @@
         <v>446</v>
       </c>
       <c r="B157" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C157" t="s">
+        <v>513</v>
+      </c>
+      <c r="E157" s="3" t="s">
         <v>514</v>
-      </c>
-      <c r="E157" s="3" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -4254,10 +4338,10 @@
         <v>480</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>466</v>
       </c>
@@ -4265,13 +4349,16 @@
         <v>467</v>
       </c>
       <c r="C159" t="s">
-        <v>478</v>
+        <v>532</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>533</v>
+      </c>
+      <c r="F159" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>466</v>
       </c>
@@ -4279,119 +4366,119 @@
         <v>467</v>
       </c>
       <c r="C160" t="s">
-        <v>482</v>
+        <v>534</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>466</v>
       </c>
       <c r="B161" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+      <c r="C161" t="s">
+        <v>478</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B162" t="s">
+        <v>467</v>
+      </c>
+      <c r="C162" t="s">
+        <v>481</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B163" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>360</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B164" t="s">
         <v>364</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C164" t="s">
         <v>365</v>
       </c>
-      <c r="E162" t="s">
+      <c r="E164" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>360</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B165" t="s">
         <v>364</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C165" t="s">
         <v>366</v>
       </c>
-      <c r="E163" t="s">
+      <c r="E165" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>361</v>
-      </c>
-      <c r="B164" t="s">
-        <v>60</v>
-      </c>
-      <c r="C164" t="s">
-        <v>460</v>
-      </c>
-      <c r="E164" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>361</v>
-      </c>
-      <c r="B165" t="s">
-        <v>60</v>
-      </c>
-      <c r="C165" t="s">
-        <v>461</v>
-      </c>
-      <c r="E165" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>361</v>
       </c>
       <c r="B166" t="s">
-        <v>325</v>
+        <v>60</v>
       </c>
       <c r="C166" t="s">
-        <v>325</v>
+        <v>460</v>
       </c>
       <c r="E166" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>361</v>
       </c>
       <c r="B167" t="s">
-        <v>363</v>
+        <v>60</v>
       </c>
       <c r="C167" t="s">
-        <v>327</v>
+        <v>461</v>
       </c>
       <c r="E167" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>361</v>
       </c>
       <c r="B168" t="s">
-        <v>363</v>
+        <v>325</v>
       </c>
       <c r="C168" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E168" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>361</v>
       </c>
@@ -4399,13 +4486,13 @@
         <v>363</v>
       </c>
       <c r="C169" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E169" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>361</v>
       </c>
@@ -4413,13 +4500,13 @@
         <v>363</v>
       </c>
       <c r="C170" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E170" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>361</v>
       </c>
@@ -4427,13 +4514,13 @@
         <v>363</v>
       </c>
       <c r="C171" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E171" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>361</v>
       </c>
@@ -4441,13 +4528,13 @@
         <v>363</v>
       </c>
       <c r="C172" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E172" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>361</v>
       </c>
@@ -4455,13 +4542,13 @@
         <v>363</v>
       </c>
       <c r="C173" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E173" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>361</v>
       </c>
@@ -4469,13 +4556,13 @@
         <v>363</v>
       </c>
       <c r="C174" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E174" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>361</v>
       </c>
@@ -4483,149 +4570,143 @@
         <v>363</v>
       </c>
       <c r="C175" t="s">
+        <v>339</v>
+      </c>
+      <c r="E175" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>361</v>
+      </c>
+      <c r="B176" t="s">
+        <v>363</v>
+      </c>
+      <c r="C176" t="s">
+        <v>341</v>
+      </c>
+      <c r="E176" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>361</v>
+      </c>
+      <c r="B177" t="s">
+        <v>363</v>
+      </c>
+      <c r="C177" t="s">
         <v>343</v>
       </c>
-      <c r="E175" t="s">
+      <c r="E177" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>489</v>
-      </c>
-      <c r="B176" t="s">
-        <v>1</v>
-      </c>
-      <c r="C176" t="s">
-        <v>2</v>
-      </c>
-      <c r="E176" t="s">
-        <v>345</v>
-      </c>
-      <c r="F176" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>489</v>
-      </c>
-      <c r="B177" t="s">
-        <v>1</v>
-      </c>
-      <c r="C177" t="s">
-        <v>367</v>
-      </c>
-      <c r="E177" t="s">
-        <v>346</v>
-      </c>
-      <c r="F177" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B178" t="s">
         <v>1</v>
       </c>
       <c r="C178" t="s">
-        <v>217</v>
+        <v>2</v>
       </c>
       <c r="E178" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F178" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B179" t="s">
         <v>1</v>
       </c>
       <c r="C179" t="s">
-        <v>22</v>
+        <v>367</v>
       </c>
       <c r="E179" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F179" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B180" t="s">
         <v>1</v>
       </c>
       <c r="C180" t="s">
-        <v>368</v>
+        <v>217</v>
       </c>
       <c r="E180" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F180" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B181" t="s">
         <v>1</v>
       </c>
       <c r="C181" t="s">
+        <v>22</v>
+      </c>
+      <c r="E181" t="s">
+        <v>348</v>
+      </c>
+      <c r="F181" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>488</v>
+      </c>
+      <c r="B182" t="s">
+        <v>1</v>
+      </c>
+      <c r="C182" t="s">
+        <v>368</v>
+      </c>
+      <c r="E182" t="s">
+        <v>349</v>
+      </c>
+      <c r="F182" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>488</v>
+      </c>
+      <c r="B183" t="s">
+        <v>1</v>
+      </c>
+      <c r="C183" t="s">
         <v>369</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E183" t="s">
         <v>350</v>
       </c>
-      <c r="F181" t="s">
+      <c r="F183" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>362</v>
-      </c>
-      <c r="B182" t="s">
-        <v>305</v>
-      </c>
-      <c r="C182" t="s">
-        <v>114</v>
-      </c>
-      <c r="E182" t="s">
-        <v>392</v>
-      </c>
-      <c r="F182" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>362</v>
-      </c>
-      <c r="B183" t="s">
-        <v>305</v>
-      </c>
-      <c r="C183" t="s">
-        <v>56</v>
-      </c>
-      <c r="E183" t="s">
-        <v>394</v>
-      </c>
-      <c r="F183" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>362</v>
       </c>
@@ -4633,16 +4714,16 @@
         <v>305</v>
       </c>
       <c r="C184" t="s">
-        <v>58</v>
+        <v>114</v>
       </c>
       <c r="E184" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="F184" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>362</v>
       </c>
@@ -4650,16 +4731,16 @@
         <v>305</v>
       </c>
       <c r="C185" t="s">
-        <v>431</v>
+        <v>56</v>
       </c>
       <c r="E185" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="F185" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>362</v>
       </c>
@@ -4667,16 +4748,16 @@
         <v>305</v>
       </c>
       <c r="C186" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E186" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="F186" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>362</v>
       </c>
@@ -4684,16 +4765,16 @@
         <v>305</v>
       </c>
       <c r="C187" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E187" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="F187" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>362</v>
       </c>
@@ -4701,16 +4782,16 @@
         <v>305</v>
       </c>
       <c r="C188" t="s">
-        <v>432</v>
+        <v>60</v>
       </c>
       <c r="E188" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="F188" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>362</v>
       </c>
@@ -4718,16 +4799,16 @@
         <v>305</v>
       </c>
       <c r="C189" t="s">
-        <v>176</v>
+        <v>433</v>
       </c>
       <c r="E189" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="F189" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>362</v>
       </c>
@@ -4735,16 +4816,16 @@
         <v>305</v>
       </c>
       <c r="C190" t="s">
-        <v>86</v>
+        <v>432</v>
       </c>
       <c r="E190" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="F190" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>362</v>
       </c>
@@ -4752,50 +4833,50 @@
         <v>305</v>
       </c>
       <c r="C191" t="s">
-        <v>92</v>
+        <v>176</v>
       </c>
       <c r="E191" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="F191" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>362</v>
       </c>
       <c r="B192" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C192" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="E192" t="s">
-        <v>370</v>
+        <v>408</v>
       </c>
       <c r="F192" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>362</v>
       </c>
       <c r="B193" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C193" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="E193" t="s">
-        <v>372</v>
+        <v>410</v>
       </c>
       <c r="F193" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>362</v>
       </c>
@@ -4803,16 +4884,16 @@
         <v>306</v>
       </c>
       <c r="C194" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E194" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F194" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>362</v>
       </c>
@@ -4820,16 +4901,16 @@
         <v>306</v>
       </c>
       <c r="C195" t="s">
-        <v>432</v>
+        <v>56</v>
       </c>
       <c r="E195" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="F195" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>362</v>
       </c>
@@ -4837,16 +4918,16 @@
         <v>306</v>
       </c>
       <c r="C196" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="E196" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F196" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>362</v>
       </c>
@@ -4854,16 +4935,16 @@
         <v>306</v>
       </c>
       <c r="C197" t="s">
-        <v>143</v>
+        <v>432</v>
       </c>
       <c r="E197" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="F197" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>362</v>
       </c>
@@ -4871,16 +4952,16 @@
         <v>306</v>
       </c>
       <c r="C198" t="s">
-        <v>92</v>
+        <v>133</v>
       </c>
       <c r="E198" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F198" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>362</v>
       </c>
@@ -4888,16 +4969,16 @@
         <v>306</v>
       </c>
       <c r="C199" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="E199" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="F199" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>362</v>
       </c>
@@ -4905,16 +4986,16 @@
         <v>306</v>
       </c>
       <c r="C200" t="s">
-        <v>168</v>
+        <v>92</v>
       </c>
       <c r="E200" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="F200" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>362</v>
       </c>
@@ -4922,16 +5003,16 @@
         <v>306</v>
       </c>
       <c r="C201" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="E201" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="F201" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>362</v>
       </c>
@@ -4939,50 +5020,50 @@
         <v>306</v>
       </c>
       <c r="C202" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="E202" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="F202" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>362</v>
       </c>
       <c r="B203" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C203" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="E203" t="s">
-        <v>351</v>
+        <v>388</v>
       </c>
       <c r="F203" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>362</v>
       </c>
       <c r="B204" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C204" t="s">
-        <v>114</v>
+        <v>179</v>
       </c>
       <c r="E204" t="s">
-        <v>352</v>
+        <v>390</v>
       </c>
       <c r="F204" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>362</v>
       </c>
@@ -4990,16 +5071,16 @@
         <v>307</v>
       </c>
       <c r="C205" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="E205" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F205" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>362</v>
       </c>
@@ -5007,16 +5088,16 @@
         <v>307</v>
       </c>
       <c r="C206" t="s">
-        <v>215</v>
+        <v>114</v>
       </c>
       <c r="E206" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F206" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>362</v>
       </c>
@@ -5024,16 +5105,16 @@
         <v>307</v>
       </c>
       <c r="C207" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="E207" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F207" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>362</v>
       </c>
@@ -5041,16 +5122,16 @@
         <v>307</v>
       </c>
       <c r="C208" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="E208" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F208" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>362</v>
       </c>
@@ -5058,16 +5139,16 @@
         <v>307</v>
       </c>
       <c r="C209" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="E209" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F209" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>362</v>
       </c>
@@ -5075,16 +5156,16 @@
         <v>307</v>
       </c>
       <c r="C210" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E210" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F210" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>362</v>
       </c>
@@ -5092,50 +5173,50 @@
         <v>307</v>
       </c>
       <c r="C211" t="s">
+        <v>236</v>
+      </c>
+      <c r="E211" t="s">
+        <v>357</v>
+      </c>
+      <c r="F211" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>362</v>
+      </c>
+      <c r="B212" t="s">
+        <v>307</v>
+      </c>
+      <c r="C212" t="s">
+        <v>232</v>
+      </c>
+      <c r="E212" t="s">
+        <v>358</v>
+      </c>
+      <c r="F212" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>362</v>
+      </c>
+      <c r="B213" t="s">
+        <v>307</v>
+      </c>
+      <c r="C213" t="s">
         <v>264</v>
       </c>
-      <c r="E211" t="s">
+      <c r="E213" t="s">
         <v>359</v>
       </c>
-      <c r="F211" t="s">
+      <c r="F213" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>428</v>
-      </c>
-      <c r="B212" t="s">
-        <v>430</v>
-      </c>
-      <c r="C212" t="s">
-        <v>280</v>
-      </c>
-      <c r="E212" t="s">
-        <v>414</v>
-      </c>
-      <c r="F212" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
-        <v>428</v>
-      </c>
-      <c r="B213" t="s">
-        <v>430</v>
-      </c>
-      <c r="C213" t="s">
-        <v>207</v>
-      </c>
-      <c r="E213" t="s">
-        <v>416</v>
-      </c>
-      <c r="F213" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>428</v>
       </c>
@@ -5143,16 +5224,16 @@
         <v>430</v>
       </c>
       <c r="C214" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E214" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="F214" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>428</v>
       </c>
@@ -5160,16 +5241,16 @@
         <v>430</v>
       </c>
       <c r="C215" t="s">
-        <v>285</v>
+        <v>207</v>
       </c>
       <c r="E215" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="F215" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>428</v>
       </c>
@@ -5177,16 +5258,16 @@
         <v>430</v>
       </c>
       <c r="C216" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="E216" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="F216" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>428</v>
       </c>
@@ -5194,84 +5275,84 @@
         <v>430</v>
       </c>
       <c r="C217" t="s">
-        <v>435</v>
+        <v>285</v>
       </c>
       <c r="E217" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F217" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>428</v>
       </c>
       <c r="B218" t="s">
+        <v>430</v>
+      </c>
+      <c r="C218" t="s">
+        <v>292</v>
+      </c>
+      <c r="E218" t="s">
+        <v>422</v>
+      </c>
+      <c r="F218" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>428</v>
+      </c>
+      <c r="B219" t="s">
+        <v>430</v>
+      </c>
+      <c r="C219" t="s">
+        <v>435</v>
+      </c>
+      <c r="E219" t="s">
+        <v>424</v>
+      </c>
+      <c r="F219" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>428</v>
+      </c>
+      <c r="B220" t="s">
         <v>308</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C220" t="s">
         <v>308</v>
       </c>
-      <c r="E218" t="s">
+      <c r="E220" t="s">
         <v>426</v>
       </c>
-      <c r="F218" t="s">
+      <c r="F220" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>429</v>
-      </c>
-      <c r="B219" t="s">
-        <v>434</v>
-      </c>
-      <c r="C219" t="s">
-        <v>434</v>
-      </c>
-      <c r="E219" t="s">
-        <v>412</v>
-      </c>
-      <c r="F219" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
-        <v>429</v>
-      </c>
-      <c r="B220" t="s">
-        <v>447</v>
-      </c>
-      <c r="C220" t="s">
-        <v>448</v>
-      </c>
-      <c r="E220" t="s">
-        <v>449</v>
-      </c>
-      <c r="F220" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>429</v>
       </c>
       <c r="B221" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="C221" t="s">
-        <v>453</v>
+        <v>434</v>
       </c>
       <c r="E221" t="s">
-        <v>451</v>
+        <v>412</v>
       </c>
       <c r="F221" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>429</v>
       </c>
@@ -5279,16 +5360,16 @@
         <v>447</v>
       </c>
       <c r="C222" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="E222" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="F222" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>429</v>
       </c>
@@ -5296,46 +5377,52 @@
         <v>447</v>
       </c>
       <c r="C223" t="s">
+        <v>453</v>
+      </c>
+      <c r="E223" t="s">
+        <v>451</v>
+      </c>
+      <c r="F223" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>429</v>
+      </c>
+      <c r="B224" t="s">
+        <v>447</v>
+      </c>
+      <c r="C224" t="s">
+        <v>454</v>
+      </c>
+      <c r="E224" t="s">
+        <v>455</v>
+      </c>
+      <c r="F224" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>429</v>
+      </c>
+      <c r="B225" t="s">
+        <v>447</v>
+      </c>
+      <c r="C225" t="s">
         <v>457</v>
       </c>
-      <c r="E223" t="s">
+      <c r="E225" t="s">
         <v>458</v>
       </c>
-      <c r="F223" t="s">
+      <c r="F225" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
         <v>471</v>
-      </c>
-      <c r="B224" t="s">
-        <v>469</v>
-      </c>
-      <c r="C224" t="s">
-        <v>470</v>
-      </c>
-      <c r="E224" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="B225" t="s">
-        <v>469</v>
-      </c>
-      <c r="C225" t="s">
-        <v>475</v>
-      </c>
-      <c r="E225" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A226" s="1" t="s">
-        <v>473</v>
       </c>
       <c r="B226" t="s">
         <v>469</v>
@@ -5344,12 +5431,12 @@
         <v>470</v>
       </c>
       <c r="E226" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B227" t="s">
         <v>469</v>
@@ -5358,140 +5445,301 @@
         <v>475</v>
       </c>
       <c r="E227" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B228" t="s">
+        <v>469</v>
+      </c>
+      <c r="C228" t="s">
+        <v>470</v>
+      </c>
+      <c r="E228" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B229" t="s">
+        <v>469</v>
+      </c>
+      <c r="C229" t="s">
+        <v>475</v>
+      </c>
+      <c r="E229" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="228" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A228" s="1" t="s">
+    <row r="230" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B230" t="s">
         <v>490</v>
       </c>
-      <c r="B228" t="s">
-        <v>491</v>
-      </c>
-      <c r="C228" t="s">
+      <c r="C230" t="s">
+        <v>498</v>
+      </c>
+      <c r="E230" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="F230" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B231" t="s">
+        <v>490</v>
+      </c>
+      <c r="C231" t="s">
         <v>499</v>
       </c>
-      <c r="E228" s="3" t="s">
+      <c r="E231" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F228" t="s">
+      <c r="F231" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B232" t="s">
+        <v>490</v>
+      </c>
+      <c r="C232" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="229" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A229" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="B229" t="s">
-        <v>491</v>
-      </c>
-      <c r="C229" t="s">
-        <v>500</v>
-      </c>
-      <c r="E229" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="F229" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A230" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="B230" t="s">
-        <v>491</v>
-      </c>
-      <c r="C230" t="s">
+      <c r="E232" s="3" t="s">
         <v>502</v>
-      </c>
-      <c r="E230" s="3" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A231" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="B231" t="s">
-        <v>492</v>
-      </c>
-      <c r="C231" t="s">
-        <v>493</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="F231" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A232" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="B232" t="s">
-        <v>492</v>
-      </c>
-      <c r="C232" t="s">
-        <v>494</v>
-      </c>
-      <c r="E232" t="s">
-        <v>505</v>
-      </c>
-      <c r="F232" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B233" t="s">
-        <v>510</v>
+        <v>491</v>
       </c>
       <c r="C233" t="s">
-        <v>511</v>
+        <v>492</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="F233" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="B234" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C234" t="s">
         <v>493</v>
       </c>
-      <c r="E234" s="1" t="s">
-        <v>506</v>
+      <c r="E234" t="s">
+        <v>504</v>
       </c>
       <c r="F234" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A235" t="s">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B235" t="s">
+        <v>509</v>
+      </c>
+      <c r="C235" t="s">
+        <v>510</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="F235" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B236" t="s">
+        <v>491</v>
+      </c>
+      <c r="C236" t="s">
+        <v>492</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="F236" t="s">
         <v>495</v>
       </c>
-      <c r="B235" t="s">
-        <v>492</v>
-      </c>
-      <c r="C235" t="s">
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
         <v>494</v>
       </c>
-      <c r="E235" t="s">
-        <v>507</v>
-      </c>
-      <c r="F235" t="s">
-        <v>497</v>
+      <c r="B237" t="s">
+        <v>491</v>
+      </c>
+      <c r="C237" t="s">
+        <v>493</v>
+      </c>
+      <c r="E237" t="s">
+        <v>506</v>
+      </c>
+      <c r="F237" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B238" t="s">
+        <v>516</v>
+      </c>
+      <c r="C238" t="s">
+        <v>519</v>
+      </c>
+      <c r="E238" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="F238" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A239" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B239" t="s">
+        <v>516</v>
+      </c>
+      <c r="C239" t="s">
+        <v>520</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="F239" s="2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A240" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B240" t="s">
+        <v>515</v>
+      </c>
+      <c r="C240" t="s">
+        <v>522</v>
+      </c>
+      <c r="E240" s="3" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B241" t="s">
+        <v>516</v>
+      </c>
+      <c r="C241" t="s">
+        <v>525</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="F241" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B242" t="s">
+        <v>515</v>
+      </c>
+      <c r="C242" t="s">
+        <v>528</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="F242" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B243" t="s">
+        <v>515</v>
+      </c>
+      <c r="C243" t="s">
+        <v>538</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="F243" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B244" t="s">
+        <v>515</v>
+      </c>
+      <c r="C244" t="s">
+        <v>530</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="F244" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A245" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B245" t="s">
+        <v>515</v>
+      </c>
+      <c r="C245" t="s">
+        <v>542</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="F245" t="s">
+        <v>544</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Snippet update to mirror changes in the edit-api
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -1590,7 +1590,146 @@
     <t>entity-content-blocks</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;div class="sc-content-block-list" @${101:var}.${102:prop}.EditContext()&gt;
+    <t>Content blocks with in-page editing</t>
+  </si>
+  <si>
+    <t>content block with inpage editing</t>
+  </si>
+  <si>
+    <t>render entity</t>
+  </si>
+  <si>
+    <t>@${101:var}.render()</t>
+  </si>
+  <si>
+    <t>loop through items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@foreach(var ${103:item} in ${101:var}.${102:prop}){
+    @${103:item}.Render()
+}
+</t>
+  </si>
+  <si>
+    <t>Render a content-block entity (remember that you can't render the list, this only renders one item).
+Note that if you try to render any kind of entity, this will not throw an error, but just render an HTML comment as there is no definition for how to render other types of entities as of now.</t>
+  </si>
+  <si>
+    <t>edit context</t>
+  </si>
+  <si>
+    <t>This should be used inside a &lt;div&gt; tag to provide additional information to the in-page editing ui</t>
+  </si>
+  <si>
+    <t>item count</t>
+  </si>
+  <si>
+    <t>@${101:var}.${102:prop}.Count</t>
+  </si>
+  <si>
+    <t>get first item</t>
+  </si>
+  <si>
+    <t>@${101:var}.${102:prop}[0]</t>
+  </si>
+  <si>
+    <t>using 2sxc namespace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@using ToSic.SexyContent;
+</t>
+  </si>
+  <si>
+    <t>using Linq</t>
+  </si>
+  <si>
+    <t>@using System.Linq;</t>
+  </si>
+  <si>
+    <t>@using ${1:System.Linq}</t>
+  </si>
+  <si>
+    <t>The 2sxc namespace, in case you explicitly want to work with 2sxc objects</t>
+  </si>
+  <si>
+    <t>get item number 0</t>
+  </si>
+  <si>
+    <t>This will give you the count of items</t>
+  </si>
+  <si>
+    <t>Note that this only works, if there are items, otherwise you'll get an error</t>
+  </si>
+  <si>
+    <t>This also requires a @using Tosic.SexyContent; at the beginning of your cshtml</t>
+  </si>
+  <si>
+    <t>show title of first item if exists</t>
+  </si>
+  <si>
+    <t>This is a shorthand for try-to-get-and-if-null-don’t-show</t>
+  </si>
+  <si>
+    <t>render first if it exists</t>
+  </si>
+  <si>
+    <t>This is a shorthand for try-to-render-first-and-if-null-don’t-show</t>
+  </si>
+  <si>
+    <t>@(${1:var}.${2:prop}.Count &gt; 0 ? ${1:var}.${2:prop}[0].Render() : "")</t>
+  </si>
+  <si>
+    <t>@(${1:var}.${2:prop}.Count &gt; 0 ? ${1:var}.${2:prop}[0].Title : "")</t>
+  </si>
+  <si>
+    <t>&lt;repeat repeat="${1:Employee} in Data:${2:Default}"&gt;...[${1}:Title]...&lt;/repeat&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sc-element"&gt;[${1:Content}:Toolbar]&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="sc-element"&gt;[List:Toolbar]&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Loop over a list of items in one of the input streams. The first value is the token-name inside the loop, the value after Data: is the stream name. Common use is Repeat="Item in Data:Default"</t>
+  </si>
+  <si>
+    <t>Get the count</t>
+  </si>
+  <si>
+    <t>Find out if this is the first item</t>
+  </si>
+  <si>
+    <t>Find out if this is the last item</t>
+  </si>
+  <si>
+    <t>Get the index of the current item, one based. So the number start with 1, 2, 3, …</t>
+  </si>
+  <si>
+    <t>Get the index of the current item, zero based. So the number start with 0, 1, 2, …</t>
+  </si>
+  <si>
+    <t>Show an inline-toolbar. If you wat it hovering, make sure you have an HTML-element around it with the class sc-element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show an inline toolbar, floating. Note that this is just an example, the div with the class sc-element can be further away, it doesn't have to be the direct container. </t>
+  </si>
+  <si>
+    <t>Use this to alternate between 0, 1 - often used to color table rows</t>
+  </si>
+  <si>
+    <t>Use this to alternate between 0, 1 and 2 - often used to have 3 items side-by side, followed by a new line</t>
+  </si>
+  <si>
+    <t>@ListContent.Toolbar</t>
+  </si>
+  <si>
+    <t>&lt;div class="sc-element"&gt;
+    @ListContent.Toolbar
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div class="sc-content-block-list" @Edit.ContextAttributes(${101:var}, "${102:prop}")&gt;
     @foreach(var contentBlock in ${101:var}.${102:prop}){
         @contentBlock.Render()
     }
@@ -1598,146 +1737,7 @@
 </t>
   </si>
   <si>
-    <t>Content blocks with in-page editing</t>
-  </si>
-  <si>
-    <t>content block with inpage editing</t>
-  </si>
-  <si>
-    <t>render entity</t>
-  </si>
-  <si>
-    <t>@${101:var}.render()</t>
-  </si>
-  <si>
-    <t>loop through items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@foreach(var ${103:item} in ${101:var}.${102:prop}){
-    @${103:item}.Render()
-}
-</t>
-  </si>
-  <si>
-    <t>Render a content-block entity (remember that you can't render the list, this only renders one item).
-Note that if you try to render any kind of entity, this will not throw an error, but just render an HTML comment as there is no definition for how to render other types of entities as of now.</t>
-  </si>
-  <si>
-    <t>edit context</t>
-  </si>
-  <si>
-    <t>@${101:var}.${102:prop}.EditContext()</t>
-  </si>
-  <si>
-    <t>This should be used inside a &lt;div&gt; tag to provide additional information to the in-page editing ui</t>
-  </si>
-  <si>
-    <t>item count</t>
-  </si>
-  <si>
-    <t>@${101:var}.${102:prop}.Count</t>
-  </si>
-  <si>
-    <t>get first item</t>
-  </si>
-  <si>
-    <t>@${101:var}.${102:prop}[0]</t>
-  </si>
-  <si>
-    <t>using 2sxc namespace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@using ToSic.SexyContent;
-</t>
-  </si>
-  <si>
-    <t>using Linq</t>
-  </si>
-  <si>
-    <t>@using System.Linq;</t>
-  </si>
-  <si>
-    <t>@using ${1:System.Linq}</t>
-  </si>
-  <si>
-    <t>The 2sxc namespace, in case you explicitly want to work with 2sxc objects</t>
-  </si>
-  <si>
-    <t>get item number 0</t>
-  </si>
-  <si>
-    <t>This will give you the count of items</t>
-  </si>
-  <si>
-    <t>Note that this only works, if there are items, otherwise you'll get an error</t>
-  </si>
-  <si>
-    <t>This also requires a @using Tosic.SexyContent; at the beginning of your cshtml</t>
-  </si>
-  <si>
-    <t>show title of first item if exists</t>
-  </si>
-  <si>
-    <t>This is a shorthand for try-to-get-and-if-null-don’t-show</t>
-  </si>
-  <si>
-    <t>render first if it exists</t>
-  </si>
-  <si>
-    <t>This is a shorthand for try-to-render-first-and-if-null-don’t-show</t>
-  </si>
-  <si>
-    <t>@(${1:var}.${2:prop}.Count &gt; 0 ? ${1:var}.${2:prop}[0].Render() : "")</t>
-  </si>
-  <si>
-    <t>@(${1:var}.${2:prop}.Count &gt; 0 ? ${1:var}.${2:prop}[0].Title : "")</t>
-  </si>
-  <si>
-    <t>&lt;repeat repeat="${1:Employee} in Data:${2:Default}"&gt;...[${1}:Title]...&lt;/repeat&gt;</t>
-  </si>
-  <si>
-    <t>&lt;div class="sc-element"&gt;[${1:Content}:Toolbar]&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>&lt;div class="sc-element"&gt;[List:Toolbar]&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>Loop over a list of items in one of the input streams. The first value is the token-name inside the loop, the value after Data: is the stream name. Common use is Repeat="Item in Data:Default"</t>
-  </si>
-  <si>
-    <t>Get the count</t>
-  </si>
-  <si>
-    <t>Find out if this is the first item</t>
-  </si>
-  <si>
-    <t>Find out if this is the last item</t>
-  </si>
-  <si>
-    <t>Get the index of the current item, one based. So the number start with 1, 2, 3, …</t>
-  </si>
-  <si>
-    <t>Get the index of the current item, zero based. So the number start with 0, 1, 2, …</t>
-  </si>
-  <si>
-    <t>Show an inline-toolbar. If you wat it hovering, make sure you have an HTML-element around it with the class sc-element</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show an inline toolbar, floating. Note that this is just an example, the div with the class sc-element can be further away, it doesn't have to be the direct container. </t>
-  </si>
-  <si>
-    <t>Use this to alternate between 0, 1 - often used to color table rows</t>
-  </si>
-  <si>
-    <t>Use this to alternate between 0, 1 and 2 - often used to have 3 items side-by side, followed by a new line</t>
-  </si>
-  <si>
-    <t>@ListContent.Toolbar</t>
-  </si>
-  <si>
-    <t>&lt;div class="sc-element"&gt;
-    @ListContent.Toolbar
-&lt;/div&gt;</t>
+    <t>@Edit.ContextAttributes(${101:var}, "${102:prop}")</t>
   </si>
 </sst>
 </file>
@@ -1802,10 +1802,10 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F246" totalsRowShown="0">
   <autoFilter ref="A1:F246">
-    <filterColumn colId="0">
+    <filterColumn colId="4">
       <filters>
-        <filter val="@List"/>
-        <filter val="[List"/>
+        <filter val="@${101:var}.${102:prop}.EditContext()"/>
+        <filter val="&lt;div class=&quot;sc-content-block-list&quot; @${101:var}.${102:prop}.EditContext()&gt;_x000a_    @foreach(var contentBlock in ${101:var}.${102:prop}){_x000a_        @contentBlock.Render()_x000a_    }_x000a_&lt;/div&gt;_x000a_"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2087,7 +2087,7 @@
   <dimension ref="A1:F246"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E241" sqref="E241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2254,7 +2254,7 @@
         <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -2271,10 +2271,10 @@
         <v>460</v>
       </c>
       <c r="F9" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>459</v>
       </c>
@@ -2288,13 +2288,13 @@
         <v>308</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F10" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>459</v>
       </c>
@@ -2305,10 +2305,10 @@
         <v>457</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>459</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>475</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -4401,13 +4401,13 @@
         <v>462</v>
       </c>
       <c r="C159" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="F159" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4418,10 +4418,10 @@
         <v>462</v>
       </c>
       <c r="C160" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -4474,7 +4474,7 @@
         <v>320</v>
       </c>
       <c r="F164" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4488,13 +4488,13 @@
         <v>362</v>
       </c>
       <c r="E165" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="F165" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>357</v>
       </c>
@@ -4508,7 +4508,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>357</v>
       </c>
@@ -4519,10 +4519,10 @@
         <v>457</v>
       </c>
       <c r="E167" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>357</v>
       </c>
@@ -4533,13 +4533,13 @@
         <v>322</v>
       </c>
       <c r="E168" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F168" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>357</v>
       </c>
@@ -4553,10 +4553,10 @@
         <v>324</v>
       </c>
       <c r="F169" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>357</v>
       </c>
@@ -4570,10 +4570,10 @@
         <v>326</v>
       </c>
       <c r="F170" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>357</v>
       </c>
@@ -4587,10 +4587,10 @@
         <v>328</v>
       </c>
       <c r="F171" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>357</v>
       </c>
@@ -4604,10 +4604,10 @@
         <v>330</v>
       </c>
       <c r="F172" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>357</v>
       </c>
@@ -4621,10 +4621,10 @@
         <v>332</v>
       </c>
       <c r="F173" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>357</v>
       </c>
@@ -4638,10 +4638,10 @@
         <v>334</v>
       </c>
       <c r="F174" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>357</v>
       </c>
@@ -4655,10 +4655,10 @@
         <v>336</v>
       </c>
       <c r="F175" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>357</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>357</v>
       </c>
@@ -5691,7 +5691,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>484</v>
       </c>
@@ -5699,13 +5699,13 @@
         <v>511</v>
       </c>
       <c r="C238" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E238" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="F238" t="s">
         <v>512</v>
-      </c>
-      <c r="F238" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="239" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
@@ -5716,13 +5716,13 @@
         <v>511</v>
       </c>
       <c r="C239" t="s">
+        <v>514</v>
+      </c>
+      <c r="E239" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="E239" s="1" t="s">
-        <v>516</v>
-      </c>
       <c r="F239" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="240" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -5733,13 +5733,13 @@
         <v>510</v>
       </c>
       <c r="C240" t="s">
+        <v>516</v>
+      </c>
+      <c r="E240" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="E240" s="3" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="241" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>484</v>
       </c>
@@ -5747,13 +5747,13 @@
         <v>511</v>
       </c>
       <c r="C241" t="s">
+        <v>519</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="F241" t="s">
         <v>520</v>
-      </c>
-      <c r="E241" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="F241" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="242" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5764,13 +5764,13 @@
         <v>510</v>
       </c>
       <c r="C242" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="F242" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="243" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5781,13 +5781,13 @@
         <v>510</v>
       </c>
       <c r="C243" t="s">
+        <v>531</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="F243" t="s">
         <v>533</v>
-      </c>
-      <c r="E243" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="F243" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5798,13 +5798,13 @@
         <v>510</v>
       </c>
       <c r="C244" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F244" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5815,13 +5815,13 @@
         <v>510</v>
       </c>
       <c r="C245" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="F245" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5832,13 +5832,13 @@
         <v>511</v>
       </c>
       <c r="C246" t="s">
+        <v>537</v>
+      </c>
+      <c r="E246" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="E246" s="1" t="s">
-        <v>541</v>
-      </c>
       <c r="F246" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix sherlock snippets close #853
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="571">
   <si>
     <t>set</t>
   </si>
@@ -1431,12 +1431,6 @@
   </si>
   <si>
     <t>css, style-sheet</t>
-  </si>
-  <si>
-    <t>&lt;link rel="stylesheet" href="@App.Path/assets/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;link rel="stylesheet" href="[App:Path]/assets/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
   </si>
   <si>
     <t>comment, server-side</t>
@@ -1589,12 +1583,6 @@
     <t>loop through items</t>
   </si>
   <si>
-    <t xml:space="preserve">@foreach(var ${103:item} in ${101:var}.${102:prop}){
-    @${103:item}.Render()
-}
-</t>
-  </si>
-  <si>
     <t>Render a content-block entity (remember that you can't render the list, this only renders one item).
 Note that if you try to render any kind of entity, this will not throw an error, but just render an HTML comment as there is no definition for how to render other types of entities as of now.</t>
   </si>
@@ -1719,6 +1707,53 @@
     <t>&lt;div class="sc-element"&gt;
     @Edit.Toolbar(ListContent)
 &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Toolbar with edit and replace buttons only</t>
+  </si>
+  <si>
+    <t>@Edit.Toolbar(actions: "new", contentType: "${10:BlogPost}")</t>
+  </si>
+  <si>
+    <t>@Edit.Toolbar(${1:Content}, actions: "edit,replace")</t>
+  </si>
+  <si>
+    <t>@Edit.Toolbar(actions: "new", contentType: "${10:BlogPost}", prefill: new { Title = "Hello", Color = "red" } )</t>
+  </si>
+  <si>
+    <t>Toolbar with new and prefill example</t>
+  </si>
+  <si>
+    <t>Toolbar for an item</t>
+  </si>
+  <si>
+    <t>ToolbarFloat for an item</t>
+  </si>
+  <si>
+    <t>Toolbar for item with edit / replace only</t>
+  </si>
+  <si>
+    <t>Toolbar to create new only</t>
+  </si>
+  <si>
+    <t>Toolbar to create new and prefill</t>
+  </si>
+  <si>
+    <t>@Edit.ContextAttributes(${101:var}, field: "${102:prop}")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div class="sc-content-block-list" @Edit.ContextAttributes(${101:var}, field: "${102:prop}")&gt;
+    @foreach(var contentBlock in AsDynamic(${101:var}.${102:prop})){
+        @contentBlock.Render()
+    }
+&lt;/div&gt;
+</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" href="[App:Path]/dist/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" href="@App.Path/dist/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
   </si>
   <si>
     <t>@foreach(var ${1:cont} in AsDynamic(Data["${2:Default}"])){
@@ -1726,48 +1761,22 @@
         @${1}.EntityTitle
         @$Edit.Toolbar({1})
     &lt;/div&gt;
-}…</t>
-  </si>
-  <si>
-    <t>Toolbar with edit and replace buttons only</t>
-  </si>
-  <si>
-    <t>@Edit.Toolbar(actions: "new", contentType: "${10:BlogPost}")</t>
-  </si>
-  <si>
-    <t>@Edit.Toolbar(${1:Content}, actions: "edit,replace")</t>
-  </si>
-  <si>
-    <t>@Edit.Toolbar(actions: "new", contentType: "${10:BlogPost}", prefill: new { Title = "Hello", Color = "red" } )</t>
-  </si>
-  <si>
-    <t>Toolbar with new and prefill example</t>
-  </si>
-  <si>
-    <t>Toolbar for an item</t>
-  </si>
-  <si>
-    <t>ToolbarFloat for an item</t>
-  </si>
-  <si>
-    <t>Toolbar for item with edit / replace only</t>
-  </si>
-  <si>
-    <t>Toolbar to create new only</t>
-  </si>
-  <si>
-    <t>Toolbar to create new and prefill</t>
-  </si>
-  <si>
-    <t>@Edit.ContextAttributes(${101:var}, field: "${102:prop}")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div class="sc-content-block-list" @Edit.ContextAttributes(${101:var}, field: "${102:prop}")&gt;
-    @foreach(var contentBlock in ${101:var}.${102:prop}){
-        @contentBlock.Render()
-    }
-&lt;/div&gt;
+}</t>
+  </si>
+  <si>
+    <t>simple loop to show all items in the default list</t>
+  </si>
+  <si>
+    <t>for-each on the default list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@foreach(var ${103:item} in AsDynamic(${101:var}.${102:prop})){
+    @${103:item}.EntityId
+}
 </t>
+  </si>
+  <si>
+    <t>loop over a list of sub-items</t>
   </si>
 </sst>
 </file>
@@ -1834,8 +1843,10 @@
   <autoFilter ref="A1:F249">
     <filterColumn colId="4">
       <filters>
-        <filter val="@Edit.ContextAttributes(${101:var}, &quot;${102:prop}&quot;)"/>
-        <filter val="&lt;div class=&quot;sc-content-block-list&quot; @Edit.ContextAttributes(${101:var}, &quot;${102:prop}&quot;)&gt;_x000a_    @foreach(var contentBlock in ${101:var}.${102:prop}){_x000a_        @contentBlock.Render()_x000a_    }_x000a_&lt;/div&gt;_x000a_"/>
+        <filter val="@${101:var}.render()"/>
+        <filter val="@(${1:var}.${2:prop}.Count &gt; 0 ? ${1:var}.${2:prop}[0].Render() : &quot;&quot;)"/>
+        <filter val="@foreach(var ${103:item} in ${101:var}.${102:prop}){_x000a_    @${103:item}.Render()_x000a_}_x000a_"/>
+        <filter val="&lt;div class=&quot;sc-content-block-list&quot; @Edit.ContextAttributes(${101:var}, field: &quot;${102:prop}&quot;)&gt;_x000a_    @foreach(var contentBlock in AsDynamic(${101:var}.${102:prop})){_x000a_        @contentBlock.Render()_x000a_    }_x000a_&lt;/div&gt;_x000a_"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2117,7 +2128,7 @@
   <dimension ref="A1:F249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E244" sqref="E244"/>
+      <selection activeCell="F249" sqref="F249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2126,7 +2137,7 @@
     <col min="2" max="2" width="32.28515625" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.7109375" customWidth="1"/>
+    <col min="5" max="5" width="71.85546875" customWidth="1"/>
     <col min="6" max="6" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2152,7 +2163,7 @@
     </row>
     <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2172,7 +2183,7 @@
     </row>
     <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -2192,7 +2203,7 @@
     </row>
     <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -2212,7 +2223,7 @@
     </row>
     <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -2232,7 +2243,7 @@
     </row>
     <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -2252,7 +2263,7 @@
     </row>
     <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -2278,13 +2289,13 @@
         <v>359</v>
       </c>
       <c r="C8" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F8" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -2295,13 +2306,13 @@
         <v>359</v>
       </c>
       <c r="C9" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="F9" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2312,13 +2323,13 @@
         <v>359</v>
       </c>
       <c r="C10" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="F10" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2329,13 +2340,13 @@
         <v>359</v>
       </c>
       <c r="C11" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="F11" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2346,13 +2357,13 @@
         <v>359</v>
       </c>
       <c r="C12" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="F12" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2369,7 +2380,7 @@
         <v>307</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="F13" t="s">
         <v>308</v>
@@ -2386,7 +2397,7 @@
         <v>456</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
@@ -2399,8 +2410,14 @@
       <c r="C15" t="s">
         <v>461</v>
       </c>
+      <c r="D15" t="s">
+        <v>568</v>
+      </c>
       <c r="E15" s="3" t="s">
-        <v>555</v>
+        <v>566</v>
+      </c>
+      <c r="F15" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4437,13 +4454,13 @@
         <v>441</v>
       </c>
       <c r="B159" t="s">
+        <v>474</v>
+      </c>
+      <c r="C159" t="s">
+        <v>475</v>
+      </c>
+      <c r="E159" s="3" t="s">
         <v>476</v>
-      </c>
-      <c r="C159" t="s">
-        <v>477</v>
-      </c>
-      <c r="E159" s="3" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="105" hidden="1" x14ac:dyDescent="0.25">
@@ -4451,13 +4468,13 @@
         <v>441</v>
       </c>
       <c r="B160" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C160" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4468,10 +4485,10 @@
         <v>460</v>
       </c>
       <c r="C161" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -4482,13 +4499,13 @@
         <v>460</v>
       </c>
       <c r="C162" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="F162" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4499,10 +4516,10 @@
         <v>460</v>
       </c>
       <c r="C163" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -4513,10 +4530,10 @@
         <v>460</v>
       </c>
       <c r="C164" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -4527,10 +4544,10 @@
         <v>460</v>
       </c>
       <c r="C165" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4555,7 +4572,7 @@
         <v>319</v>
       </c>
       <c r="F167" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4569,10 +4586,10 @@
         <v>361</v>
       </c>
       <c r="E168" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F168" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4600,7 +4617,7 @@
         <v>456</v>
       </c>
       <c r="E170" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4614,10 +4631,10 @@
         <v>321</v>
       </c>
       <c r="E171" t="s">
+        <v>535</v>
+      </c>
+      <c r="F171" t="s">
         <v>538</v>
-      </c>
-      <c r="F171" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4634,7 +4651,7 @@
         <v>323</v>
       </c>
       <c r="F172" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4651,7 +4668,7 @@
         <v>325</v>
       </c>
       <c r="F173" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4668,7 +4685,7 @@
         <v>327</v>
       </c>
       <c r="F174" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4685,7 +4702,7 @@
         <v>329</v>
       </c>
       <c r="F175" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4702,7 +4719,7 @@
         <v>331</v>
       </c>
       <c r="F176" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4719,7 +4736,7 @@
         <v>333</v>
       </c>
       <c r="F177" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4736,7 +4753,7 @@
         <v>335</v>
       </c>
       <c r="F178" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4769,7 +4786,7 @@
     </row>
     <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B181" t="s">
         <v>1</v>
@@ -4786,7 +4803,7 @@
     </row>
     <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B182" t="s">
         <v>1</v>
@@ -4803,7 +4820,7 @@
     </row>
     <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B183" t="s">
         <v>1</v>
@@ -4820,7 +4837,7 @@
     </row>
     <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B184" t="s">
         <v>1</v>
@@ -4837,7 +4854,7 @@
     </row>
     <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B185" t="s">
         <v>1</v>
@@ -4854,7 +4871,7 @@
     </row>
     <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B186" t="s">
         <v>1</v>
@@ -5608,7 +5625,7 @@
         <v>468</v>
       </c>
       <c r="E230" t="s">
-        <v>470</v>
+        <v>564</v>
       </c>
     </row>
     <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5636,290 +5653,293 @@
         <v>468</v>
       </c>
       <c r="E232" t="s">
-        <v>469</v>
+        <v>565</v>
       </c>
     </row>
     <row r="233" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B233" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C233" t="s">
+        <v>488</v>
+      </c>
+      <c r="E233" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="F233" t="s">
         <v>490</v>
-      </c>
-      <c r="E233" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="F233" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="234" spans="1:6" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B234" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C234" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E234" s="3" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="F234" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="235" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B235" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C235" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E235" s="3" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B236" t="s">
         <v>481</v>
       </c>
-      <c r="B236" t="s">
-        <v>483</v>
-      </c>
       <c r="C236" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F236" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B237" t="s">
         <v>481</v>
       </c>
-      <c r="B237" t="s">
+      <c r="C237" t="s">
         <v>483</v>
       </c>
-      <c r="C237" t="s">
-        <v>485</v>
-      </c>
       <c r="E237" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F237" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B238" t="s">
+        <v>499</v>
+      </c>
+      <c r="C238" t="s">
+        <v>500</v>
+      </c>
+      <c r="E238" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="C238" t="s">
+      <c r="F238" t="s">
         <v>502</v>
-      </c>
-      <c r="E238" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="F238" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B239" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C239" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="F239" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="240" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
+        <v>484</v>
+      </c>
+      <c r="B240" t="s">
+        <v>481</v>
+      </c>
+      <c r="C240" t="s">
+        <v>483</v>
+      </c>
+      <c r="E240" t="s">
+        <v>496</v>
+      </c>
+      <c r="F240" t="s">
         <v>486</v>
       </c>
-      <c r="B240" t="s">
-        <v>483</v>
-      </c>
-      <c r="C240" t="s">
-        <v>485</v>
-      </c>
-      <c r="E240" t="s">
-        <v>498</v>
-      </c>
-      <c r="F240" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="241" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="241" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B241" t="s">
+        <v>506</v>
+      </c>
+      <c r="C241" t="s">
         <v>508</v>
       </c>
-      <c r="C241" t="s">
+      <c r="E241" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="F241" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B242" t="s">
+        <v>506</v>
+      </c>
+      <c r="C242" t="s">
+        <v>509</v>
+      </c>
+      <c r="E242" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="E241" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="F241" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="242" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B242" t="s">
-        <v>508</v>
-      </c>
-      <c r="C242" t="s">
+      <c r="F242" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A243" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B243" t="s">
+        <v>505</v>
+      </c>
+      <c r="C243" t="s">
         <v>511</v>
       </c>
-      <c r="E242" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="F242" s="2" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="243" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A243" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B243" t="s">
-        <v>507</v>
-      </c>
-      <c r="C243" t="s">
+      <c r="E243" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="F243" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B244" t="s">
+        <v>506</v>
+      </c>
+      <c r="C244" t="s">
         <v>513</v>
       </c>
-      <c r="E243" s="3" t="s">
+      <c r="E244" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="F244" t="s">
         <v>514</v>
-      </c>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A244" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B244" t="s">
-        <v>508</v>
-      </c>
-      <c r="C244" t="s">
-        <v>516</v>
-      </c>
-      <c r="E244" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="F244" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B245" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C245" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="F245" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B246" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C246" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F246" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B247" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C247" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F247" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="248" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B248" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C248" t="s">
+        <v>529</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="F248" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B249" t="s">
+        <v>506</v>
+      </c>
+      <c r="C249" t="s">
+        <v>531</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="F249" t="s">
         <v>532</v>
-      </c>
-      <c r="E248" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="F248" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A249" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B249" t="s">
-        <v>508</v>
-      </c>
-      <c r="C249" t="s">
-        <v>534</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="F249" t="s">
-        <v>535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reset Master to currently released code base
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="568">
   <si>
     <t>set</t>
   </si>
@@ -1431,6 +1431,12 @@
   </si>
   <si>
     <t>css, style-sheet</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" href="@App.Path/assets/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" href="[App:Path]/assets/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
   </si>
   <si>
     <t>comment, server-side</t>
@@ -1583,6 +1589,12 @@
     <t>loop through items</t>
   </si>
   <si>
+    <t xml:space="preserve">@foreach(var ${103:item} in ${101:var}.${102:prop}){
+    @${103:item}.Render()
+}
+</t>
+  </si>
+  <si>
     <t>Render a content-block entity (remember that you can't render the list, this only renders one item).
 Note that if you try to render any kind of entity, this will not throw an error, but just render an HTML comment as there is no definition for how to render other types of entities as of now.</t>
   </si>
@@ -1707,53 +1719,6 @@
     <t>&lt;div class="sc-element"&gt;
     @Edit.Toolbar(ListContent)
 &lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>Toolbar with edit and replace buttons only</t>
-  </si>
-  <si>
-    <t>@Edit.Toolbar(actions: "new", contentType: "${10:BlogPost}")</t>
-  </si>
-  <si>
-    <t>@Edit.Toolbar(${1:Content}, actions: "edit,replace")</t>
-  </si>
-  <si>
-    <t>@Edit.Toolbar(actions: "new", contentType: "${10:BlogPost}", prefill: new { Title = "Hello", Color = "red" } )</t>
-  </si>
-  <si>
-    <t>Toolbar with new and prefill example</t>
-  </si>
-  <si>
-    <t>Toolbar for an item</t>
-  </si>
-  <si>
-    <t>ToolbarFloat for an item</t>
-  </si>
-  <si>
-    <t>Toolbar for item with edit / replace only</t>
-  </si>
-  <si>
-    <t>Toolbar to create new only</t>
-  </si>
-  <si>
-    <t>Toolbar to create new and prefill</t>
-  </si>
-  <si>
-    <t>@Edit.ContextAttributes(${101:var}, field: "${102:prop}")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div class="sc-content-block-list" @Edit.ContextAttributes(${101:var}, field: "${102:prop}")&gt;
-    @foreach(var contentBlock in AsDynamic(${101:var}.${102:prop})){
-        @contentBlock.Render()
-    }
-&lt;/div&gt;
-</t>
-  </si>
-  <si>
-    <t>&lt;link rel="stylesheet" href="[App:Path]/dist/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;link rel="stylesheet" href="@App.Path/dist/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
   </si>
   <si>
     <t>@foreach(var ${1:cont} in AsDynamic(Data["${2:Default}"])){
@@ -1761,46 +1726,48 @@
         @${1}.EntityTitle
         @$Edit.Toolbar({1})
     &lt;/div&gt;
-}</t>
-  </si>
-  <si>
-    <t>simple loop to show all items in the default list</t>
-  </si>
-  <si>
-    <t>for-each on the default list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@foreach(var ${103:item} in AsDynamic(${101:var}.${102:prop})){
-    @${103:item}.EntityId
-}
+}…</t>
+  </si>
+  <si>
+    <t>Toolbar with edit and replace buttons only</t>
+  </si>
+  <si>
+    <t>@Edit.Toolbar(actions: "new", contentType: "${10:BlogPost}")</t>
+  </si>
+  <si>
+    <t>@Edit.Toolbar(${1:Content}, actions: "edit,replace")</t>
+  </si>
+  <si>
+    <t>@Edit.Toolbar(actions: "new", contentType: "${10:BlogPost}", prefill: new { Title = "Hello", Color = "red" } )</t>
+  </si>
+  <si>
+    <t>Toolbar with new and prefill example</t>
+  </si>
+  <si>
+    <t>Toolbar for an item</t>
+  </si>
+  <si>
+    <t>ToolbarFloat for an item</t>
+  </si>
+  <si>
+    <t>Toolbar for item with edit / replace only</t>
+  </si>
+  <si>
+    <t>Toolbar to create new only</t>
+  </si>
+  <si>
+    <t>Toolbar to create new and prefill</t>
+  </si>
+  <si>
+    <t>@Edit.ContextAttributes(${101:var}, field: "${102:prop}")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div class="sc-content-block-list" @Edit.ContextAttributes(${101:var}, field: "${102:prop}")&gt;
+    @foreach(var contentBlock in ${101:var}.${102:prop}){
+        @contentBlock.Render()
+    }
+&lt;/div&gt;
 </t>
-  </si>
-  <si>
-    <t>loop over a list of sub-items</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>yyyy-MM-dd</t>
-  </si>
-  <si>
-    <t>@${1:var}.${2:prop}.ToString("yyyy-MM-dd")</t>
-  </si>
-  <si>
-    <t>format date with yyyy-MM-dd</t>
-  </si>
-  <si>
-    <t>link to url as parameter</t>
-  </si>
-  <si>
-    <t>Link to the same page but use this value as a url parameter</t>
-  </si>
-  <si>
-    <t>@Link.To(parameters: "${10:id}=" + ${1:var}.${2:prop})</t>
-  </si>
-  <si>
-    <t>string-url-path</t>
   </si>
 </sst>
 </file>
@@ -1863,8 +1830,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F251" totalsRowShown="0">
-  <autoFilter ref="A1:F251"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F249" totalsRowShown="0">
+  <autoFilter ref="A1:F249">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="@Edit.ContextAttributes(${101:var}, &quot;${102:prop}&quot;)"/>
+        <filter val="&lt;div class=&quot;sc-content-block-list&quot; @Edit.ContextAttributes(${101:var}, &quot;${102:prop}&quot;)&gt;_x000a_    @foreach(var contentBlock in ${101:var}.${102:prop}){_x000a_        @contentBlock.Render()_x000a_    }_x000a_&lt;/div&gt;_x000a_"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -2140,10 +2114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F251"/>
+  <dimension ref="A1:F249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="C241" sqref="C241"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E244" sqref="E244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2152,7 +2126,7 @@
     <col min="2" max="2" width="32.28515625" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.85546875" customWidth="1"/>
+    <col min="5" max="5" width="61.7109375" customWidth="1"/>
     <col min="6" max="6" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2176,9 +2150,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2196,9 +2170,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -2216,9 +2190,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -2236,9 +2210,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -2256,9 +2230,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -2276,9 +2250,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -2296,7 +2270,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>457</v>
       </c>
@@ -2304,16 +2278,16 @@
         <v>359</v>
       </c>
       <c r="C8" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="F8" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>457</v>
       </c>
@@ -2321,16 +2295,16 @@
         <v>359</v>
       </c>
       <c r="C9" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="F9" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>457</v>
       </c>
@@ -2338,16 +2312,16 @@
         <v>359</v>
       </c>
       <c r="C10" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
       <c r="F10" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>457</v>
       </c>
@@ -2355,16 +2329,16 @@
         <v>359</v>
       </c>
       <c r="C11" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
       <c r="F11" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>457</v>
       </c>
@@ -2372,16 +2346,16 @@
         <v>359</v>
       </c>
       <c r="C12" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="F12" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>458</v>
       </c>
@@ -2395,13 +2369,13 @@
         <v>307</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="F13" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>458</v>
       </c>
@@ -2412,10 +2386,10 @@
         <v>456</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>458</v>
       </c>
@@ -2425,17 +2399,11 @@
       <c r="C15" t="s">
         <v>461</v>
       </c>
-      <c r="D15" t="s">
-        <v>568</v>
-      </c>
       <c r="E15" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F15" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>317</v>
       </c>
@@ -2449,7 +2417,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>317</v>
       </c>
@@ -2463,7 +2431,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>317</v>
       </c>
@@ -2477,7 +2445,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>317</v>
       </c>
@@ -2491,7 +2459,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>317</v>
       </c>
@@ -2505,7 +2473,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>317</v>
       </c>
@@ -2519,7 +2487,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>317</v>
       </c>
@@ -2533,7 +2501,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>317</v>
       </c>
@@ -2547,7 +2515,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>317</v>
       </c>
@@ -2561,7 +2529,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>317</v>
       </c>
@@ -2575,7 +2543,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>317</v>
       </c>
@@ -2589,7 +2557,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>317</v>
       </c>
@@ -2603,7 +2571,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>317</v>
       </c>
@@ -2617,7 +2585,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>317</v>
       </c>
@@ -2631,7 +2599,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>317</v>
       </c>
@@ -2645,7 +2613,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>317</v>
       </c>
@@ -2659,7 +2627,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>317</v>
       </c>
@@ -2673,7 +2641,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>317</v>
       </c>
@@ -2687,7 +2655,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>317</v>
       </c>
@@ -2701,7 +2669,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>317</v>
       </c>
@@ -2715,7 +2683,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>317</v>
       </c>
@@ -2729,7 +2697,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>317</v>
       </c>
@@ -2743,7 +2711,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>317</v>
       </c>
@@ -2757,7 +2725,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>317</v>
       </c>
@@ -2771,7 +2739,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>317</v>
       </c>
@@ -2785,7 +2753,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>317</v>
       </c>
@@ -2799,7 +2767,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>317</v>
       </c>
@@ -2813,7 +2781,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>317</v>
       </c>
@@ -2827,7 +2795,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>317</v>
       </c>
@@ -2841,7 +2809,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>317</v>
       </c>
@@ -2855,7 +2823,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>317</v>
       </c>
@@ -2869,7 +2837,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>317</v>
       </c>
@@ -2883,7 +2851,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>317</v>
       </c>
@@ -2897,7 +2865,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>317</v>
       </c>
@@ -2911,7 +2879,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>317</v>
       </c>
@@ -2925,7 +2893,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>317</v>
       </c>
@@ -2939,7 +2907,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>317</v>
       </c>
@@ -2953,7 +2921,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>317</v>
       </c>
@@ -2967,7 +2935,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>317</v>
       </c>
@@ -2981,7 +2949,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>317</v>
       </c>
@@ -2995,7 +2963,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>317</v>
       </c>
@@ -3009,7 +2977,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>317</v>
       </c>
@@ -3023,7 +2991,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>317</v>
       </c>
@@ -3037,7 +3005,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>317</v>
       </c>
@@ -3054,7 +3022,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>317</v>
       </c>
@@ -3068,7 +3036,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>317</v>
       </c>
@@ -3082,7 +3050,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>317</v>
       </c>
@@ -3096,7 +3064,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>317</v>
       </c>
@@ -3110,7 +3078,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>317</v>
       </c>
@@ -3124,7 +3092,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>317</v>
       </c>
@@ -3138,7 +3106,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>317</v>
       </c>
@@ -3152,7 +3120,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>317</v>
       </c>
@@ -3166,7 +3134,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>317</v>
       </c>
@@ -3180,7 +3148,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>317</v>
       </c>
@@ -3194,7 +3162,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>317</v>
       </c>
@@ -3208,7 +3176,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>317</v>
       </c>
@@ -3222,7 +3190,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>317</v>
       </c>
@@ -3236,7 +3204,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>317</v>
       </c>
@@ -3250,7 +3218,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>317</v>
       </c>
@@ -3264,7 +3232,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>317</v>
       </c>
@@ -3278,7 +3246,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>317</v>
       </c>
@@ -3292,7 +3260,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>317</v>
       </c>
@@ -3306,7 +3274,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>317</v>
       </c>
@@ -3320,7 +3288,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>317</v>
       </c>
@@ -3334,7 +3302,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>317</v>
       </c>
@@ -3348,7 +3316,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>317</v>
       </c>
@@ -3362,7 +3330,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>317</v>
       </c>
@@ -3376,7 +3344,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>317</v>
       </c>
@@ -3390,7 +3358,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>317</v>
       </c>
@@ -3404,7 +3372,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>317</v>
       </c>
@@ -3418,7 +3386,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>317</v>
       </c>
@@ -3432,7 +3400,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>317</v>
       </c>
@@ -3446,7 +3414,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>317</v>
       </c>
@@ -3460,7 +3428,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>317</v>
       </c>
@@ -3474,7 +3442,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>317</v>
       </c>
@@ -3488,7 +3456,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>317</v>
       </c>
@@ -3502,7 +3470,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>317</v>
       </c>
@@ -3516,7 +3484,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>317</v>
       </c>
@@ -3530,7 +3498,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>317</v>
       </c>
@@ -3544,7 +3512,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>317</v>
       </c>
@@ -3558,7 +3526,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>317</v>
       </c>
@@ -3572,7 +3540,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>317</v>
       </c>
@@ -3586,7 +3554,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>317</v>
       </c>
@@ -3600,7 +3568,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>317</v>
       </c>
@@ -3614,7 +3582,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>317</v>
       </c>
@@ -3628,7 +3596,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>317</v>
       </c>
@@ -3645,7 +3613,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>317</v>
       </c>
@@ -3662,7 +3630,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>317</v>
       </c>
@@ -3676,7 +3644,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>317</v>
       </c>
@@ -3690,7 +3658,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>317</v>
       </c>
@@ -3704,7 +3672,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>317</v>
       </c>
@@ -3718,7 +3686,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>317</v>
       </c>
@@ -3732,7 +3700,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>317</v>
       </c>
@@ -3746,7 +3714,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>317</v>
       </c>
@@ -3760,7 +3728,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>317</v>
       </c>
@@ -3774,7 +3742,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>317</v>
       </c>
@@ -3788,7 +3756,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>317</v>
       </c>
@@ -3802,7 +3770,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>317</v>
       </c>
@@ -3816,7 +3784,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>317</v>
       </c>
@@ -3830,7 +3798,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>317</v>
       </c>
@@ -3844,7 +3812,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>317</v>
       </c>
@@ -3861,7 +3829,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>317</v>
       </c>
@@ -3875,7 +3843,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>317</v>
       </c>
@@ -3892,7 +3860,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>317</v>
       </c>
@@ -3906,7 +3874,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>317</v>
       </c>
@@ -3920,7 +3888,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>317</v>
       </c>
@@ -3934,7 +3902,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>317</v>
       </c>
@@ -3948,7 +3916,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>317</v>
       </c>
@@ -3962,7 +3930,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>317</v>
       </c>
@@ -3976,7 +3944,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>317</v>
       </c>
@@ -3990,7 +3958,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>317</v>
       </c>
@@ -4004,7 +3972,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>317</v>
       </c>
@@ -4018,7 +3986,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>317</v>
       </c>
@@ -4035,7 +4003,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>317</v>
       </c>
@@ -4049,7 +4017,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>317</v>
       </c>
@@ -4063,7 +4031,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>317</v>
       </c>
@@ -4077,7 +4045,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>317</v>
       </c>
@@ -4091,7 +4059,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>317</v>
       </c>
@@ -4105,7 +4073,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>317</v>
       </c>
@@ -4119,7 +4087,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>317</v>
       </c>
@@ -4133,7 +4101,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>317</v>
       </c>
@@ -4147,7 +4115,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>317</v>
       </c>
@@ -4161,7 +4129,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>317</v>
       </c>
@@ -4175,7 +4143,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>317</v>
       </c>
@@ -4189,7 +4157,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>317</v>
       </c>
@@ -4203,7 +4171,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>317</v>
       </c>
@@ -4217,7 +4185,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>317</v>
       </c>
@@ -4231,7 +4199,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>317</v>
       </c>
@@ -4245,7 +4213,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>317</v>
       </c>
@@ -4259,7 +4227,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>441</v>
       </c>
@@ -4273,7 +4241,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>441</v>
       </c>
@@ -4287,7 +4255,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>441</v>
       </c>
@@ -4301,7 +4269,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>441</v>
       </c>
@@ -4315,7 +4283,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>441</v>
       </c>
@@ -4329,7 +4297,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>441</v>
       </c>
@@ -4343,7 +4311,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>441</v>
       </c>
@@ -4357,7 +4325,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>441</v>
       </c>
@@ -4371,7 +4339,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>441</v>
       </c>
@@ -4388,7 +4356,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>441</v>
       </c>
@@ -4402,7 +4370,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>441</v>
       </c>
@@ -4419,7 +4387,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>441</v>
       </c>
@@ -4433,7 +4401,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>441</v>
       </c>
@@ -4447,7 +4415,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>441</v>
       </c>
@@ -4464,35 +4432,35 @@
         <v>316</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>441</v>
       </c>
       <c r="B159" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C159" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>441</v>
       </c>
       <c r="B160" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C160" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>459</v>
       </c>
@@ -4500,13 +4468,13 @@
         <v>460</v>
       </c>
       <c r="C161" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>459</v>
       </c>
@@ -4514,16 +4482,16 @@
         <v>460</v>
       </c>
       <c r="C162" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="F162" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>459</v>
       </c>
@@ -4531,13 +4499,13 @@
         <v>460</v>
       </c>
       <c r="C163" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>459</v>
       </c>
@@ -4545,13 +4513,13 @@
         <v>460</v>
       </c>
       <c r="C164" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>459</v>
       </c>
@@ -4559,13 +4527,13 @@
         <v>460</v>
       </c>
       <c r="C165" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>459</v>
       </c>
@@ -4573,7 +4541,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>355</v>
       </c>
@@ -4587,10 +4555,10 @@
         <v>319</v>
       </c>
       <c r="F167" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>355</v>
       </c>
@@ -4601,13 +4569,13 @@
         <v>361</v>
       </c>
       <c r="E168" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="F168" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>356</v>
       </c>
@@ -4621,7 +4589,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>356</v>
       </c>
@@ -4632,10 +4600,10 @@
         <v>456</v>
       </c>
       <c r="E170" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>356</v>
       </c>
@@ -4646,13 +4614,13 @@
         <v>321</v>
       </c>
       <c r="E171" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="F171" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>356</v>
       </c>
@@ -4666,10 +4634,10 @@
         <v>323</v>
       </c>
       <c r="F172" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>356</v>
       </c>
@@ -4683,10 +4651,10 @@
         <v>325</v>
       </c>
       <c r="F173" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>356</v>
       </c>
@@ -4700,10 +4668,10 @@
         <v>327</v>
       </c>
       <c r="F174" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>356</v>
       </c>
@@ -4717,10 +4685,10 @@
         <v>329</v>
       </c>
       <c r="F175" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>356</v>
       </c>
@@ -4734,10 +4702,10 @@
         <v>331</v>
       </c>
       <c r="F176" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>356</v>
       </c>
@@ -4751,10 +4719,10 @@
         <v>333</v>
       </c>
       <c r="F177" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>356</v>
       </c>
@@ -4768,10 +4736,10 @@
         <v>335</v>
       </c>
       <c r="F178" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>356</v>
       </c>
@@ -4785,7 +4753,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>356</v>
       </c>
@@ -4799,9 +4767,9 @@
         <v>339</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B181" t="s">
         <v>1</v>
@@ -4816,9 +4784,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B182" t="s">
         <v>1</v>
@@ -4833,9 +4801,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B183" t="s">
         <v>1</v>
@@ -4850,9 +4818,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B184" t="s">
         <v>1</v>
@@ -4867,9 +4835,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B185" t="s">
         <v>1</v>
@@ -4884,9 +4852,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B186" t="s">
         <v>1</v>
@@ -4901,7 +4869,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>357</v>
       </c>
@@ -4918,7 +4886,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>357</v>
       </c>
@@ -4935,7 +4903,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>357</v>
       </c>
@@ -4952,7 +4920,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>357</v>
       </c>
@@ -4969,7 +4937,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>357</v>
       </c>
@@ -4986,7 +4954,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>357</v>
       </c>
@@ -5003,7 +4971,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>357</v>
       </c>
@@ -5020,7 +4988,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>357</v>
       </c>
@@ -5037,7 +5005,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>357</v>
       </c>
@@ -5054,7 +5022,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>357</v>
       </c>
@@ -5071,7 +5039,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>357</v>
       </c>
@@ -5088,7 +5056,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>357</v>
       </c>
@@ -5105,7 +5073,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>357</v>
       </c>
@@ -5122,7 +5090,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>357</v>
       </c>
@@ -5139,7 +5107,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>357</v>
       </c>
@@ -5156,7 +5124,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>357</v>
       </c>
@@ -5173,7 +5141,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>357</v>
       </c>
@@ -5190,7 +5158,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>357</v>
       </c>
@@ -5207,7 +5175,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>357</v>
       </c>
@@ -5224,7 +5192,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>357</v>
       </c>
@@ -5241,7 +5209,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>357</v>
       </c>
@@ -5258,7 +5226,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>357</v>
       </c>
@@ -5275,7 +5243,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>357</v>
       </c>
@@ -5292,7 +5260,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>357</v>
       </c>
@@ -5309,7 +5277,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>357</v>
       </c>
@@ -5326,7 +5294,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>357</v>
       </c>
@@ -5343,7 +5311,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>357</v>
       </c>
@@ -5360,7 +5328,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>357</v>
       </c>
@@ -5377,7 +5345,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>357</v>
       </c>
@@ -5394,7 +5362,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>357</v>
       </c>
@@ -5411,7 +5379,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>423</v>
       </c>
@@ -5428,7 +5396,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>423</v>
       </c>
@@ -5445,7 +5413,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>423</v>
       </c>
@@ -5462,7 +5430,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>423</v>
       </c>
@@ -5479,7 +5447,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>423</v>
       </c>
@@ -5496,7 +5464,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>423</v>
       </c>
@@ -5513,7 +5481,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>423</v>
       </c>
@@ -5530,7 +5498,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>424</v>
       </c>
@@ -5547,7 +5515,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>424</v>
       </c>
@@ -5564,7 +5532,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>424</v>
       </c>
@@ -5581,7 +5549,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>424</v>
       </c>
@@ -5598,7 +5566,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>424</v>
       </c>
@@ -5615,7 +5583,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>464</v>
       </c>
@@ -5629,7 +5597,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>464</v>
       </c>
@@ -5640,355 +5608,318 @@
         <v>468</v>
       </c>
       <c r="E230" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B231" t="s">
+        <v>462</v>
+      </c>
+      <c r="C231" t="s">
+        <v>463</v>
+      </c>
+      <c r="E231" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B232" t="s">
+        <v>462</v>
+      </c>
+      <c r="C232" t="s">
+        <v>468</v>
+      </c>
+      <c r="E232" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B233" t="s">
+        <v>482</v>
+      </c>
+      <c r="C233" t="s">
+        <v>490</v>
+      </c>
+      <c r="E233" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="F233" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B234" t="s">
+        <v>482</v>
+      </c>
+      <c r="C234" t="s">
+        <v>491</v>
+      </c>
+      <c r="E234" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="F234" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B235" t="s">
+        <v>482</v>
+      </c>
+      <c r="C235" t="s">
+        <v>493</v>
+      </c>
+      <c r="E235" s="3" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B236" t="s">
+        <v>483</v>
+      </c>
+      <c r="C236" t="s">
         <v>484</v>
       </c>
-      <c r="B231" t="s">
-        <v>481</v>
-      </c>
-      <c r="C231" t="s">
-        <v>482</v>
-      </c>
-      <c r="E231" s="1" t="s">
+      <c r="E236" s="1" t="s">
         <v>495</v>
-      </c>
-      <c r="F231" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>484</v>
-      </c>
-      <c r="B232" t="s">
-        <v>481</v>
-      </c>
-      <c r="C232" t="s">
-        <v>483</v>
-      </c>
-      <c r="E232" t="s">
-        <v>496</v>
-      </c>
-      <c r="F232" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A233" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B233" t="s">
-        <v>462</v>
-      </c>
-      <c r="C233" t="s">
-        <v>463</v>
-      </c>
-      <c r="E233" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A234" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B234" t="s">
-        <v>462</v>
-      </c>
-      <c r="C234" t="s">
-        <v>468</v>
-      </c>
-      <c r="E234" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A235" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B235" t="s">
-        <v>480</v>
-      </c>
-      <c r="C235" t="s">
-        <v>488</v>
-      </c>
-      <c r="E235" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="F235" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A236" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B236" t="s">
-        <v>480</v>
-      </c>
-      <c r="C236" t="s">
-        <v>489</v>
-      </c>
-      <c r="E236" s="3" t="s">
-        <v>498</v>
       </c>
       <c r="F236" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="237" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B237" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="C237" t="s">
-        <v>491</v>
-      </c>
-      <c r="E237" s="3" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+        <v>485</v>
+      </c>
+      <c r="E237" t="s">
+        <v>496</v>
+      </c>
+      <c r="F237" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B238" t="s">
+        <v>501</v>
+      </c>
+      <c r="C238" t="s">
+        <v>502</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="F238" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B239" t="s">
+        <v>483</v>
+      </c>
+      <c r="C239" t="s">
+        <v>484</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="F239" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>486</v>
+      </c>
+      <c r="B240" t="s">
+        <v>483</v>
+      </c>
+      <c r="C240" t="s">
+        <v>485</v>
+      </c>
+      <c r="E240" t="s">
+        <v>498</v>
+      </c>
+      <c r="F240" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A241" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="C238" t="s">
-        <v>482</v>
-      </c>
-      <c r="E238" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="F238" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A239" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B239" t="s">
+      <c r="B241" t="s">
+        <v>508</v>
+      </c>
+      <c r="C241" t="s">
+        <v>510</v>
+      </c>
+      <c r="E241" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="F241" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="C239" t="s">
-        <v>483</v>
-      </c>
-      <c r="E239" t="s">
-        <v>494</v>
-      </c>
-      <c r="F239" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A240" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B240" t="s">
-        <v>499</v>
-      </c>
-      <c r="C240" t="s">
-        <v>500</v>
-      </c>
-      <c r="E240" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="F240" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A241" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B241" t="s">
-        <v>578</v>
-      </c>
-      <c r="C241" t="s">
-        <v>575</v>
-      </c>
-      <c r="E241" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="F241" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A242" s="1" t="s">
-        <v>479</v>
-      </c>
       <c r="B242" t="s">
-        <v>571</v>
+        <v>508</v>
       </c>
       <c r="C242" t="s">
-        <v>572</v>
-      </c>
-      <c r="E242" s="3" t="s">
-        <v>573</v>
-      </c>
-      <c r="F242" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="243" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>511</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="F242" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B243" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C243" t="s">
+        <v>513</v>
+      </c>
+      <c r="E243" s="3" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B244" t="s">
         <v>508</v>
       </c>
-      <c r="E243" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="F243" t="s">
+      <c r="C244" t="s">
+        <v>516</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="F244" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B245" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="244" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A244" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B244" t="s">
-        <v>506</v>
-      </c>
-      <c r="C244" t="s">
-        <v>509</v>
-      </c>
-      <c r="E244" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="F244" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="245" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A245" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B245" t="s">
-        <v>505</v>
-      </c>
       <c r="C245" t="s">
-        <v>511</v>
-      </c>
-      <c r="E245" s="3" t="s">
-        <v>569</v>
+        <v>518</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>519</v>
       </c>
       <c r="F245" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B246" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C246" t="s">
-        <v>513</v>
+        <v>528</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>562</v>
+        <v>521</v>
       </c>
       <c r="F246" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B247" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C247" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="F247" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B248" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C248" t="s">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>518</v>
+        <v>537</v>
       </c>
       <c r="F248" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B249" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="C249" t="s">
-        <v>517</v>
+        <v>534</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>518</v>
+        <v>536</v>
       </c>
       <c r="F249" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A250" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B250" t="s">
-        <v>505</v>
-      </c>
-      <c r="C250" t="s">
-        <v>529</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="F250" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A251" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B251" t="s">
-        <v>506</v>
-      </c>
-      <c r="C251" t="s">
-        <v>531</v>
-      </c>
-      <c r="E251" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="F251" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed mistakes which got it because of the merge...
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="568">
   <si>
     <t>set</t>
   </si>
@@ -1431,6 +1431,12 @@
   </si>
   <si>
     <t>css, style-sheet</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" href="@App.Path/assets/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" href="[App:Path]/assets/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
   </si>
   <si>
     <t>comment, server-side</t>
@@ -1583,6 +1589,12 @@
     <t>loop through items</t>
   </si>
   <si>
+    <t xml:space="preserve">@foreach(var ${103:item} in ${101:var}.${102:prop}){
+    @${103:item}.Render()
+}
+</t>
+  </si>
+  <si>
     <t>Render a content-block entity (remember that you can't render the list, this only renders one item).
 Note that if you try to render any kind of entity, this will not throw an error, but just render an HTML comment as there is no definition for how to render other types of entities as of now.</t>
   </si>
@@ -1707,53 +1719,6 @@
     <t>&lt;div class="sc-element"&gt;
     @Edit.Toolbar(ListContent)
 &lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>Toolbar with edit and replace buttons only</t>
-  </si>
-  <si>
-    <t>@Edit.Toolbar(actions: "new", contentType: "${10:BlogPost}")</t>
-  </si>
-  <si>
-    <t>@Edit.Toolbar(${1:Content}, actions: "edit,replace")</t>
-  </si>
-  <si>
-    <t>@Edit.Toolbar(actions: "new", contentType: "${10:BlogPost}", prefill: new { Title = "Hello", Color = "red" } )</t>
-  </si>
-  <si>
-    <t>Toolbar with new and prefill example</t>
-  </si>
-  <si>
-    <t>Toolbar for an item</t>
-  </si>
-  <si>
-    <t>ToolbarFloat for an item</t>
-  </si>
-  <si>
-    <t>Toolbar for item with edit / replace only</t>
-  </si>
-  <si>
-    <t>Toolbar to create new only</t>
-  </si>
-  <si>
-    <t>Toolbar to create new and prefill</t>
-  </si>
-  <si>
-    <t>@Edit.ContextAttributes(${101:var}, field: "${102:prop}")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div class="sc-content-block-list" @Edit.ContextAttributes(${101:var}, field: "${102:prop}")&gt;
-    @foreach(var contentBlock in AsDynamic(${101:var}.${102:prop})){
-        @contentBlock.Render()
-    }
-&lt;/div&gt;
-</t>
-  </si>
-  <si>
-    <t>&lt;link rel="stylesheet" href="[App:Path]/dist/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;link rel="stylesheet" href="@App.Path/dist/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
   </si>
   <si>
     <t>@foreach(var ${1:cont} in AsDynamic(Data["${2:Default}"])){
@@ -1761,46 +1726,48 @@
         @${1}.EntityTitle
         @$Edit.Toolbar({1})
     &lt;/div&gt;
-}</t>
-  </si>
-  <si>
-    <t>simple loop to show all items in the default list</t>
-  </si>
-  <si>
-    <t>for-each on the default list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@foreach(var ${103:item} in AsDynamic(${101:var}.${102:prop})){
-    @${103:item}.EntityId
-}
+}…</t>
+  </si>
+  <si>
+    <t>Toolbar with edit and replace buttons only</t>
+  </si>
+  <si>
+    <t>@Edit.Toolbar(actions: "new", contentType: "${10:BlogPost}")</t>
+  </si>
+  <si>
+    <t>@Edit.Toolbar(${1:Content}, actions: "edit,replace")</t>
+  </si>
+  <si>
+    <t>@Edit.Toolbar(actions: "new", contentType: "${10:BlogPost}", prefill: new { Title = "Hello", Color = "red" } )</t>
+  </si>
+  <si>
+    <t>Toolbar with new and prefill example</t>
+  </si>
+  <si>
+    <t>Toolbar for an item</t>
+  </si>
+  <si>
+    <t>ToolbarFloat for an item</t>
+  </si>
+  <si>
+    <t>Toolbar for item with edit / replace only</t>
+  </si>
+  <si>
+    <t>Toolbar to create new only</t>
+  </si>
+  <si>
+    <t>Toolbar to create new and prefill</t>
+  </si>
+  <si>
+    <t>@Edit.ContextAttributes(${101:var}, field: "${102:prop}")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div class="sc-content-block-list" @Edit.ContextAttributes(${101:var}, field: "${102:prop}")&gt;
+    @foreach(var contentBlock in ${101:var}.${102:prop}){
+        @contentBlock.Render()
+    }
+&lt;/div&gt;
 </t>
-  </si>
-  <si>
-    <t>loop over a list of sub-items</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>yyyy-MM-dd</t>
-  </si>
-  <si>
-    <t>@${1:var}.${2:prop}.ToString("yyyy-MM-dd")</t>
-  </si>
-  <si>
-    <t>format date with yyyy-MM-dd</t>
-  </si>
-  <si>
-    <t>link to url as parameter</t>
-  </si>
-  <si>
-    <t>Link to the same page but use this value as a url parameter</t>
-  </si>
-  <si>
-    <t>@Link.To(parameters: "${10:id}=" + ${1:var}.${2:prop})</t>
-  </si>
-  <si>
-    <t>string-url-path</t>
   </si>
 </sst>
 </file>
@@ -1863,8 +1830,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F251" totalsRowShown="0">
-  <autoFilter ref="A1:F251"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F249" totalsRowShown="0">
+  <autoFilter ref="A1:F249">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="@Edit.ContextAttributes(${101:var}, &quot;${102:prop}&quot;)"/>
+        <filter val="&lt;div class=&quot;sc-content-block-list&quot; @Edit.ContextAttributes(${101:var}, &quot;${102:prop}&quot;)&gt;_x000a_    @foreach(var contentBlock in ${101:var}.${102:prop}){_x000a_        @contentBlock.Render()_x000a_    }_x000a_&lt;/div&gt;_x000a_"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -2140,10 +2114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F251"/>
+  <dimension ref="A1:F249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="C241" sqref="C241"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E244" sqref="E244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2152,7 +2126,7 @@
     <col min="2" max="2" width="32.28515625" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.85546875" customWidth="1"/>
+    <col min="5" max="5" width="61.7109375" customWidth="1"/>
     <col min="6" max="6" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2176,9 +2150,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2196,9 +2170,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -2216,9 +2190,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -2236,9 +2210,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -2256,9 +2230,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -2276,9 +2250,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -2296,7 +2270,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>457</v>
       </c>
@@ -2304,16 +2278,16 @@
         <v>359</v>
       </c>
       <c r="C8" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="F8" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>457</v>
       </c>
@@ -2321,16 +2295,16 @@
         <v>359</v>
       </c>
       <c r="C9" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="F9" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>457</v>
       </c>
@@ -2338,16 +2312,16 @@
         <v>359</v>
       </c>
       <c r="C10" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
       <c r="F10" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>457</v>
       </c>
@@ -2355,16 +2329,16 @@
         <v>359</v>
       </c>
       <c r="C11" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
       <c r="F11" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>457</v>
       </c>
@@ -2372,16 +2346,16 @@
         <v>359</v>
       </c>
       <c r="C12" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="F12" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>458</v>
       </c>
@@ -2395,13 +2369,13 @@
         <v>307</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="F13" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>458</v>
       </c>
@@ -2412,10 +2386,10 @@
         <v>456</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>458</v>
       </c>
@@ -2425,17 +2399,11 @@
       <c r="C15" t="s">
         <v>461</v>
       </c>
-      <c r="D15" t="s">
-        <v>568</v>
-      </c>
       <c r="E15" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="F15" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>317</v>
       </c>
@@ -2449,7 +2417,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>317</v>
       </c>
@@ -2463,7 +2431,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>317</v>
       </c>
@@ -2477,7 +2445,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>317</v>
       </c>
@@ -2491,7 +2459,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>317</v>
       </c>
@@ -2505,7 +2473,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>317</v>
       </c>
@@ -2519,7 +2487,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>317</v>
       </c>
@@ -2533,7 +2501,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>317</v>
       </c>
@@ -2547,7 +2515,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>317</v>
       </c>
@@ -2561,7 +2529,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>317</v>
       </c>
@@ -2575,7 +2543,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>317</v>
       </c>
@@ -2589,7 +2557,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>317</v>
       </c>
@@ -2603,7 +2571,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>317</v>
       </c>
@@ -2617,7 +2585,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>317</v>
       </c>
@@ -2631,7 +2599,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>317</v>
       </c>
@@ -2645,7 +2613,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>317</v>
       </c>
@@ -2659,7 +2627,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>317</v>
       </c>
@@ -2673,7 +2641,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>317</v>
       </c>
@@ -2687,7 +2655,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>317</v>
       </c>
@@ -2701,7 +2669,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>317</v>
       </c>
@@ -2715,7 +2683,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>317</v>
       </c>
@@ -2729,7 +2697,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>317</v>
       </c>
@@ -2743,7 +2711,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>317</v>
       </c>
@@ -2757,7 +2725,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>317</v>
       </c>
@@ -2771,7 +2739,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>317</v>
       </c>
@@ -2785,7 +2753,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>317</v>
       </c>
@@ -2799,7 +2767,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>317</v>
       </c>
@@ -2813,7 +2781,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>317</v>
       </c>
@@ -2827,7 +2795,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>317</v>
       </c>
@@ -2841,7 +2809,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>317</v>
       </c>
@@ -2855,7 +2823,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>317</v>
       </c>
@@ -2869,7 +2837,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>317</v>
       </c>
@@ -2883,7 +2851,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>317</v>
       </c>
@@ -2897,7 +2865,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>317</v>
       </c>
@@ -2911,7 +2879,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>317</v>
       </c>
@@ -2925,7 +2893,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>317</v>
       </c>
@@ -2939,7 +2907,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>317</v>
       </c>
@@ -2953,7 +2921,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>317</v>
       </c>
@@ -2967,7 +2935,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>317</v>
       </c>
@@ -2981,7 +2949,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>317</v>
       </c>
@@ -2995,7 +2963,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>317</v>
       </c>
@@ -3009,7 +2977,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>317</v>
       </c>
@@ -3023,7 +2991,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>317</v>
       </c>
@@ -3037,7 +3005,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>317</v>
       </c>
@@ -3054,7 +3022,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>317</v>
       </c>
@@ -3068,7 +3036,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>317</v>
       </c>
@@ -3082,7 +3050,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>317</v>
       </c>
@@ -3096,7 +3064,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>317</v>
       </c>
@@ -3110,7 +3078,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>317</v>
       </c>
@@ -3124,7 +3092,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>317</v>
       </c>
@@ -3138,7 +3106,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>317</v>
       </c>
@@ -3152,7 +3120,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>317</v>
       </c>
@@ -3166,7 +3134,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>317</v>
       </c>
@@ -3180,7 +3148,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>317</v>
       </c>
@@ -3194,7 +3162,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>317</v>
       </c>
@@ -3208,7 +3176,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>317</v>
       </c>
@@ -3222,7 +3190,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>317</v>
       </c>
@@ -3236,7 +3204,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>317</v>
       </c>
@@ -3250,7 +3218,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>317</v>
       </c>
@@ -3264,7 +3232,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>317</v>
       </c>
@@ -3278,7 +3246,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>317</v>
       </c>
@@ -3292,7 +3260,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>317</v>
       </c>
@@ -3306,7 +3274,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>317</v>
       </c>
@@ -3320,7 +3288,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>317</v>
       </c>
@@ -3334,7 +3302,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>317</v>
       </c>
@@ -3348,7 +3316,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>317</v>
       </c>
@@ -3362,7 +3330,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>317</v>
       </c>
@@ -3376,7 +3344,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>317</v>
       </c>
@@ -3390,7 +3358,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>317</v>
       </c>
@@ -3404,7 +3372,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>317</v>
       </c>
@@ -3418,7 +3386,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>317</v>
       </c>
@@ -3432,7 +3400,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>317</v>
       </c>
@@ -3446,7 +3414,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>317</v>
       </c>
@@ -3460,7 +3428,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>317</v>
       </c>
@@ -3474,7 +3442,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>317</v>
       </c>
@@ -3488,7 +3456,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>317</v>
       </c>
@@ -3502,7 +3470,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>317</v>
       </c>
@@ -3516,7 +3484,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>317</v>
       </c>
@@ -3530,7 +3498,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>317</v>
       </c>
@@ -3544,7 +3512,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>317</v>
       </c>
@@ -3558,7 +3526,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>317</v>
       </c>
@@ -3572,7 +3540,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>317</v>
       </c>
@@ -3586,7 +3554,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>317</v>
       </c>
@@ -3600,7 +3568,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>317</v>
       </c>
@@ -3614,7 +3582,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>317</v>
       </c>
@@ -3628,7 +3596,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>317</v>
       </c>
@@ -3645,7 +3613,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>317</v>
       </c>
@@ -3662,7 +3630,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>317</v>
       </c>
@@ -3676,7 +3644,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>317</v>
       </c>
@@ -3690,7 +3658,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>317</v>
       </c>
@@ -3704,7 +3672,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>317</v>
       </c>
@@ -3718,7 +3686,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>317</v>
       </c>
@@ -3732,7 +3700,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>317</v>
       </c>
@@ -3746,7 +3714,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>317</v>
       </c>
@@ -3760,7 +3728,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>317</v>
       </c>
@@ -3774,7 +3742,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>317</v>
       </c>
@@ -3788,7 +3756,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>317</v>
       </c>
@@ -3802,7 +3770,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>317</v>
       </c>
@@ -3816,7 +3784,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>317</v>
       </c>
@@ -3830,7 +3798,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>317</v>
       </c>
@@ -3844,7 +3812,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>317</v>
       </c>
@@ -3861,7 +3829,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>317</v>
       </c>
@@ -3875,7 +3843,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>317</v>
       </c>
@@ -3892,7 +3860,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>317</v>
       </c>
@@ -3906,7 +3874,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>317</v>
       </c>
@@ -3920,7 +3888,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>317</v>
       </c>
@@ -3934,7 +3902,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>317</v>
       </c>
@@ -3948,7 +3916,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>317</v>
       </c>
@@ -3962,7 +3930,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>317</v>
       </c>
@@ -3976,7 +3944,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>317</v>
       </c>
@@ -3990,7 +3958,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>317</v>
       </c>
@@ -4004,7 +3972,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>317</v>
       </c>
@@ -4018,7 +3986,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>317</v>
       </c>
@@ -4035,7 +4003,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>317</v>
       </c>
@@ -4049,7 +4017,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>317</v>
       </c>
@@ -4063,7 +4031,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>317</v>
       </c>
@@ -4077,7 +4045,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>317</v>
       </c>
@@ -4091,7 +4059,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>317</v>
       </c>
@@ -4105,7 +4073,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>317</v>
       </c>
@@ -4119,7 +4087,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>317</v>
       </c>
@@ -4133,7 +4101,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>317</v>
       </c>
@@ -4147,7 +4115,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>317</v>
       </c>
@@ -4161,7 +4129,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>317</v>
       </c>
@@ -4175,7 +4143,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>317</v>
       </c>
@@ -4189,7 +4157,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>317</v>
       </c>
@@ -4203,7 +4171,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>317</v>
       </c>
@@ -4217,7 +4185,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>317</v>
       </c>
@@ -4231,7 +4199,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>317</v>
       </c>
@@ -4245,7 +4213,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>317</v>
       </c>
@@ -4259,7 +4227,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>441</v>
       </c>
@@ -4273,7 +4241,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>441</v>
       </c>
@@ -4287,7 +4255,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>441</v>
       </c>
@@ -4301,7 +4269,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>441</v>
       </c>
@@ -4315,7 +4283,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>441</v>
       </c>
@@ -4329,7 +4297,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>441</v>
       </c>
@@ -4343,7 +4311,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>441</v>
       </c>
@@ -4357,7 +4325,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>441</v>
       </c>
@@ -4371,7 +4339,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>441</v>
       </c>
@@ -4388,7 +4356,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>441</v>
       </c>
@@ -4402,7 +4370,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>441</v>
       </c>
@@ -4419,7 +4387,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>441</v>
       </c>
@@ -4433,7 +4401,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>441</v>
       </c>
@@ -4447,7 +4415,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>441</v>
       </c>
@@ -4464,35 +4432,35 @@
         <v>316</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>441</v>
       </c>
       <c r="B159" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C159" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>441</v>
       </c>
       <c r="B160" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C160" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>459</v>
       </c>
@@ -4500,13 +4468,13 @@
         <v>460</v>
       </c>
       <c r="C161" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>459</v>
       </c>
@@ -4514,16 +4482,16 @@
         <v>460</v>
       </c>
       <c r="C162" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="F162" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>459</v>
       </c>
@@ -4531,13 +4499,13 @@
         <v>460</v>
       </c>
       <c r="C163" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>459</v>
       </c>
@@ -4545,13 +4513,13 @@
         <v>460</v>
       </c>
       <c r="C164" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>459</v>
       </c>
@@ -4559,13 +4527,13 @@
         <v>460</v>
       </c>
       <c r="C165" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>459</v>
       </c>
@@ -4573,7 +4541,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>355</v>
       </c>
@@ -4587,10 +4555,10 @@
         <v>319</v>
       </c>
       <c r="F167" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>355</v>
       </c>
@@ -4601,13 +4569,13 @@
         <v>361</v>
       </c>
       <c r="E168" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="F168" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>356</v>
       </c>
@@ -4621,7 +4589,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>356</v>
       </c>
@@ -4632,10 +4600,10 @@
         <v>456</v>
       </c>
       <c r="E170" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>356</v>
       </c>
@@ -4646,13 +4614,13 @@
         <v>321</v>
       </c>
       <c r="E171" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="F171" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>356</v>
       </c>
@@ -4666,10 +4634,10 @@
         <v>323</v>
       </c>
       <c r="F172" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>356</v>
       </c>
@@ -4683,10 +4651,10 @@
         <v>325</v>
       </c>
       <c r="F173" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>356</v>
       </c>
@@ -4700,10 +4668,10 @@
         <v>327</v>
       </c>
       <c r="F174" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>356</v>
       </c>
@@ -4717,10 +4685,10 @@
         <v>329</v>
       </c>
       <c r="F175" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>356</v>
       </c>
@@ -4734,10 +4702,10 @@
         <v>331</v>
       </c>
       <c r="F176" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>356</v>
       </c>
@@ -4751,10 +4719,10 @@
         <v>333</v>
       </c>
       <c r="F177" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>356</v>
       </c>
@@ -4768,10 +4736,10 @@
         <v>335</v>
       </c>
       <c r="F178" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>356</v>
       </c>
@@ -4785,7 +4753,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>356</v>
       </c>
@@ -4799,9 +4767,9 @@
         <v>339</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B181" t="s">
         <v>1</v>
@@ -4816,9 +4784,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B182" t="s">
         <v>1</v>
@@ -4833,9 +4801,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B183" t="s">
         <v>1</v>
@@ -4850,9 +4818,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B184" t="s">
         <v>1</v>
@@ -4867,9 +4835,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B185" t="s">
         <v>1</v>
@@ -4884,9 +4852,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B186" t="s">
         <v>1</v>
@@ -4901,7 +4869,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>357</v>
       </c>
@@ -4918,7 +4886,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>357</v>
       </c>
@@ -4935,7 +4903,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>357</v>
       </c>
@@ -4952,7 +4920,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>357</v>
       </c>
@@ -4969,7 +4937,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>357</v>
       </c>
@@ -4986,7 +4954,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>357</v>
       </c>
@@ -5003,7 +4971,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>357</v>
       </c>
@@ -5020,7 +4988,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>357</v>
       </c>
@@ -5037,7 +5005,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>357</v>
       </c>
@@ -5054,7 +5022,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>357</v>
       </c>
@@ -5071,7 +5039,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>357</v>
       </c>
@@ -5088,7 +5056,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>357</v>
       </c>
@@ -5105,7 +5073,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>357</v>
       </c>
@@ -5122,7 +5090,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>357</v>
       </c>
@@ -5139,7 +5107,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>357</v>
       </c>
@@ -5156,7 +5124,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>357</v>
       </c>
@@ -5173,7 +5141,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>357</v>
       </c>
@@ -5190,7 +5158,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>357</v>
       </c>
@@ -5207,7 +5175,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>357</v>
       </c>
@@ -5224,7 +5192,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>357</v>
       </c>
@@ -5241,7 +5209,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>357</v>
       </c>
@@ -5258,7 +5226,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>357</v>
       </c>
@@ -5275,7 +5243,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>357</v>
       </c>
@@ -5292,7 +5260,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>357</v>
       </c>
@@ -5309,7 +5277,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>357</v>
       </c>
@@ -5326,7 +5294,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>357</v>
       </c>
@@ -5343,7 +5311,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>357</v>
       </c>
@@ -5360,7 +5328,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>357</v>
       </c>
@@ -5377,7 +5345,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>357</v>
       </c>
@@ -5394,7 +5362,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>357</v>
       </c>
@@ -5411,7 +5379,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>423</v>
       </c>
@@ -5428,7 +5396,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>423</v>
       </c>
@@ -5445,7 +5413,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>423</v>
       </c>
@@ -5462,7 +5430,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>423</v>
       </c>
@@ -5479,7 +5447,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>423</v>
       </c>
@@ -5496,7 +5464,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>423</v>
       </c>
@@ -5513,7 +5481,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>423</v>
       </c>
@@ -5530,7 +5498,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>424</v>
       </c>
@@ -5547,7 +5515,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>424</v>
       </c>
@@ -5564,7 +5532,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>424</v>
       </c>
@@ -5581,7 +5549,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>424</v>
       </c>
@@ -5598,7 +5566,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>424</v>
       </c>
@@ -5615,7 +5583,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>464</v>
       </c>
@@ -5629,7 +5597,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>464</v>
       </c>
@@ -5640,355 +5608,318 @@
         <v>468</v>
       </c>
       <c r="E230" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B231" t="s">
+        <v>462</v>
+      </c>
+      <c r="C231" t="s">
+        <v>463</v>
+      </c>
+      <c r="E231" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B232" t="s">
+        <v>462</v>
+      </c>
+      <c r="C232" t="s">
+        <v>468</v>
+      </c>
+      <c r="E232" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B233" t="s">
+        <v>482</v>
+      </c>
+      <c r="C233" t="s">
+        <v>490</v>
+      </c>
+      <c r="E233" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="F233" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" ht="150" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B234" t="s">
+        <v>482</v>
+      </c>
+      <c r="C234" t="s">
+        <v>491</v>
+      </c>
+      <c r="E234" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="F234" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B235" t="s">
+        <v>482</v>
+      </c>
+      <c r="C235" t="s">
+        <v>493</v>
+      </c>
+      <c r="E235" s="3" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B236" t="s">
+        <v>483</v>
+      </c>
+      <c r="C236" t="s">
         <v>484</v>
       </c>
-      <c r="B231" t="s">
-        <v>481</v>
-      </c>
-      <c r="C231" t="s">
-        <v>482</v>
-      </c>
-      <c r="E231" s="1" t="s">
+      <c r="E236" s="1" t="s">
         <v>495</v>
-      </c>
-      <c r="F231" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>484</v>
-      </c>
-      <c r="B232" t="s">
-        <v>481</v>
-      </c>
-      <c r="C232" t="s">
-        <v>483</v>
-      </c>
-      <c r="E232" t="s">
-        <v>496</v>
-      </c>
-      <c r="F232" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A233" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B233" t="s">
-        <v>462</v>
-      </c>
-      <c r="C233" t="s">
-        <v>463</v>
-      </c>
-      <c r="E233" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A234" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B234" t="s">
-        <v>462</v>
-      </c>
-      <c r="C234" t="s">
-        <v>468</v>
-      </c>
-      <c r="E234" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A235" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B235" t="s">
-        <v>480</v>
-      </c>
-      <c r="C235" t="s">
-        <v>488</v>
-      </c>
-      <c r="E235" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="F235" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A236" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B236" t="s">
-        <v>480</v>
-      </c>
-      <c r="C236" t="s">
-        <v>489</v>
-      </c>
-      <c r="E236" s="3" t="s">
-        <v>498</v>
       </c>
       <c r="F236" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="237" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B237" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="C237" t="s">
-        <v>491</v>
-      </c>
-      <c r="E237" s="3" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+        <v>485</v>
+      </c>
+      <c r="E237" t="s">
+        <v>496</v>
+      </c>
+      <c r="F237" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B238" t="s">
+        <v>501</v>
+      </c>
+      <c r="C238" t="s">
+        <v>502</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="F238" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B239" t="s">
+        <v>483</v>
+      </c>
+      <c r="C239" t="s">
+        <v>484</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="F239" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>486</v>
+      </c>
+      <c r="B240" t="s">
+        <v>483</v>
+      </c>
+      <c r="C240" t="s">
+        <v>485</v>
+      </c>
+      <c r="E240" t="s">
+        <v>498</v>
+      </c>
+      <c r="F240" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A241" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="C238" t="s">
-        <v>482</v>
-      </c>
-      <c r="E238" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="F238" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A239" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B239" t="s">
+      <c r="B241" t="s">
+        <v>508</v>
+      </c>
+      <c r="C241" t="s">
+        <v>510</v>
+      </c>
+      <c r="E241" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="F241" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="C239" t="s">
-        <v>483</v>
-      </c>
-      <c r="E239" t="s">
-        <v>494</v>
-      </c>
-      <c r="F239" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A240" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B240" t="s">
-        <v>499</v>
-      </c>
-      <c r="C240" t="s">
-        <v>500</v>
-      </c>
-      <c r="E240" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="F240" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A241" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B241" t="s">
-        <v>578</v>
-      </c>
-      <c r="C241" t="s">
-        <v>575</v>
-      </c>
-      <c r="E241" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="F241" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A242" s="1" t="s">
-        <v>479</v>
-      </c>
       <c r="B242" t="s">
-        <v>571</v>
+        <v>508</v>
       </c>
       <c r="C242" t="s">
-        <v>572</v>
-      </c>
-      <c r="E242" s="3" t="s">
-        <v>573</v>
-      </c>
-      <c r="F242" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="243" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>511</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="F242" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B243" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C243" t="s">
+        <v>513</v>
+      </c>
+      <c r="E243" s="3" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B244" t="s">
         <v>508</v>
       </c>
-      <c r="E243" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="F243" t="s">
+      <c r="C244" t="s">
+        <v>516</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="F244" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B245" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="244" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A244" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B244" t="s">
-        <v>506</v>
-      </c>
-      <c r="C244" t="s">
-        <v>509</v>
-      </c>
-      <c r="E244" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="F244" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="245" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A245" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B245" t="s">
-        <v>505</v>
-      </c>
       <c r="C245" t="s">
-        <v>511</v>
-      </c>
-      <c r="E245" s="3" t="s">
-        <v>569</v>
+        <v>518</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>519</v>
       </c>
       <c r="F245" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B246" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C246" t="s">
-        <v>513</v>
+        <v>528</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>562</v>
+        <v>521</v>
       </c>
       <c r="F246" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B247" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C247" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="F247" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B248" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C248" t="s">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>518</v>
+        <v>537</v>
       </c>
       <c r="F248" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="B249" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="C249" t="s">
-        <v>517</v>
+        <v>534</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>518</v>
+        <v>536</v>
       </c>
       <c r="F249" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A250" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B250" t="s">
-        <v>505</v>
-      </c>
-      <c r="C250" t="s">
-        <v>529</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="F250" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A251" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B251" t="s">
-        <v>506</v>
-      </c>
-      <c r="C251" t="s">
-        <v>531</v>
-      </c>
-      <c r="E251" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="F251" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed snippets to before merge
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="579">
   <si>
     <t>set</t>
   </si>
@@ -1431,12 +1431,6 @@
   </si>
   <si>
     <t>css, style-sheet</t>
-  </si>
-  <si>
-    <t>&lt;link rel="stylesheet" href="@App.Path/assets/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;link rel="stylesheet" href="[App:Path]/assets/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
   </si>
   <si>
     <t>comment, server-side</t>
@@ -1589,12 +1583,6 @@
     <t>loop through items</t>
   </si>
   <si>
-    <t xml:space="preserve">@foreach(var ${103:item} in ${101:var}.${102:prop}){
-    @${103:item}.Render()
-}
-</t>
-  </si>
-  <si>
     <t>Render a content-block entity (remember that you can't render the list, this only renders one item).
 Note that if you try to render any kind of entity, this will not throw an error, but just render an HTML comment as there is no definition for how to render other types of entities as of now.</t>
   </si>
@@ -1719,6 +1707,53 @@
     <t>&lt;div class="sc-element"&gt;
     @Edit.Toolbar(ListContent)
 &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Toolbar with edit and replace buttons only</t>
+  </si>
+  <si>
+    <t>@Edit.Toolbar(actions: "new", contentType: "${10:BlogPost}")</t>
+  </si>
+  <si>
+    <t>@Edit.Toolbar(${1:Content}, actions: "edit,replace")</t>
+  </si>
+  <si>
+    <t>@Edit.Toolbar(actions: "new", contentType: "${10:BlogPost}", prefill: new { Title = "Hello", Color = "red" } )</t>
+  </si>
+  <si>
+    <t>Toolbar with new and prefill example</t>
+  </si>
+  <si>
+    <t>Toolbar for an item</t>
+  </si>
+  <si>
+    <t>ToolbarFloat for an item</t>
+  </si>
+  <si>
+    <t>Toolbar for item with edit / replace only</t>
+  </si>
+  <si>
+    <t>Toolbar to create new only</t>
+  </si>
+  <si>
+    <t>Toolbar to create new and prefill</t>
+  </si>
+  <si>
+    <t>@Edit.ContextAttributes(${101:var}, field: "${102:prop}")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;div class="sc-content-block-list" @Edit.ContextAttributes(${101:var}, field: "${102:prop}")&gt;
+    @foreach(var contentBlock in AsDynamic(${101:var}.${102:prop})){
+        @contentBlock.Render()
+    }
+&lt;/div&gt;
+</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" href="[App:Path]/dist/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;link rel="stylesheet" href="@App.Path/dist/AppCatalog.css" data-enableoptimizations="100"/&gt;</t>
   </si>
   <si>
     <t>@foreach(var ${1:cont} in AsDynamic(Data["${2:Default}"])){
@@ -1726,48 +1761,46 @@
         @${1}.EntityTitle
         @$Edit.Toolbar({1})
     &lt;/div&gt;
-}…</t>
-  </si>
-  <si>
-    <t>Toolbar with edit and replace buttons only</t>
-  </si>
-  <si>
-    <t>@Edit.Toolbar(actions: "new", contentType: "${10:BlogPost}")</t>
-  </si>
-  <si>
-    <t>@Edit.Toolbar(${1:Content}, actions: "edit,replace")</t>
-  </si>
-  <si>
-    <t>@Edit.Toolbar(actions: "new", contentType: "${10:BlogPost}", prefill: new { Title = "Hello", Color = "red" } )</t>
-  </si>
-  <si>
-    <t>Toolbar with new and prefill example</t>
-  </si>
-  <si>
-    <t>Toolbar for an item</t>
-  </si>
-  <si>
-    <t>ToolbarFloat for an item</t>
-  </si>
-  <si>
-    <t>Toolbar for item with edit / replace only</t>
-  </si>
-  <si>
-    <t>Toolbar to create new only</t>
-  </si>
-  <si>
-    <t>Toolbar to create new and prefill</t>
-  </si>
-  <si>
-    <t>@Edit.ContextAttributes(${101:var}, field: "${102:prop}")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;div class="sc-content-block-list" @Edit.ContextAttributes(${101:var}, field: "${102:prop}")&gt;
-    @foreach(var contentBlock in ${101:var}.${102:prop}){
-        @contentBlock.Render()
-    }
-&lt;/div&gt;
+}</t>
+  </si>
+  <si>
+    <t>simple loop to show all items in the default list</t>
+  </si>
+  <si>
+    <t>for-each on the default list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@foreach(var ${103:item} in AsDynamic(${101:var}.${102:prop})){
+    @${103:item}.EntityId
+}
 </t>
+  </si>
+  <si>
+    <t>loop over a list of sub-items</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>yyyy-MM-dd</t>
+  </si>
+  <si>
+    <t>@${1:var}.${2:prop}.ToString("yyyy-MM-dd")</t>
+  </si>
+  <si>
+    <t>format date with yyyy-MM-dd</t>
+  </si>
+  <si>
+    <t>link to url as parameter</t>
+  </si>
+  <si>
+    <t>Link to the same page but use this value as a url parameter</t>
+  </si>
+  <si>
+    <t>@Link.To(parameters: "${10:id}=" + ${1:var}.${2:prop})</t>
+  </si>
+  <si>
+    <t>string-url-path</t>
   </si>
 </sst>
 </file>
@@ -1830,15 +1863,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F249" totalsRowShown="0">
-  <autoFilter ref="A1:F249">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="@Edit.ContextAttributes(${101:var}, &quot;${102:prop}&quot;)"/>
-        <filter val="&lt;div class=&quot;sc-content-block-list&quot; @Edit.ContextAttributes(${101:var}, &quot;${102:prop}&quot;)&gt;_x000a_    @foreach(var contentBlock in ${101:var}.${102:prop}){_x000a_        @contentBlock.Render()_x000a_    }_x000a_&lt;/div&gt;_x000a_"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F251" totalsRowShown="0">
+  <autoFilter ref="A1:F251"/>
   <tableColumns count="6">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -2114,10 +2140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F249"/>
+  <dimension ref="A1:F251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E244" sqref="E244"/>
+    <sheetView tabSelected="1" topLeftCell="A230" workbookViewId="0">
+      <selection activeCell="C241" sqref="C241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2126,7 +2152,7 @@
     <col min="2" max="2" width="32.28515625" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.7109375" customWidth="1"/>
+    <col min="5" max="5" width="71.85546875" customWidth="1"/>
     <col min="6" max="6" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2150,9 +2176,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2170,9 +2196,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -2190,9 +2216,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -2210,9 +2236,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -2230,9 +2256,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -2250,9 +2276,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -2270,7 +2296,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>457</v>
       </c>
@@ -2278,16 +2304,16 @@
         <v>359</v>
       </c>
       <c r="C8" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F8" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>457</v>
       </c>
@@ -2295,16 +2321,16 @@
         <v>359</v>
       </c>
       <c r="C9" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="F9" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>457</v>
       </c>
@@ -2312,16 +2338,16 @@
         <v>359</v>
       </c>
       <c r="C10" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="F10" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>457</v>
       </c>
@@ -2329,16 +2355,16 @@
         <v>359</v>
       </c>
       <c r="C11" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="F11" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>457</v>
       </c>
@@ -2346,16 +2372,16 @@
         <v>359</v>
       </c>
       <c r="C12" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="F12" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>458</v>
       </c>
@@ -2369,13 +2395,13 @@
         <v>307</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="F13" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>458</v>
       </c>
@@ -2386,10 +2412,10 @@
         <v>456</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>458</v>
       </c>
@@ -2399,11 +2425,17 @@
       <c r="C15" t="s">
         <v>461</v>
       </c>
+      <c r="D15" t="s">
+        <v>568</v>
+      </c>
       <c r="E15" s="3" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>566</v>
+      </c>
+      <c r="F15" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>317</v>
       </c>
@@ -2417,7 +2449,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>317</v>
       </c>
@@ -2431,7 +2463,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>317</v>
       </c>
@@ -2445,7 +2477,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>317</v>
       </c>
@@ -2459,7 +2491,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>317</v>
       </c>
@@ -2473,7 +2505,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>317</v>
       </c>
@@ -2487,7 +2519,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>317</v>
       </c>
@@ -2501,7 +2533,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>317</v>
       </c>
@@ -2515,7 +2547,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>317</v>
       </c>
@@ -2529,7 +2561,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>317</v>
       </c>
@@ -2543,7 +2575,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>317</v>
       </c>
@@ -2557,7 +2589,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>317</v>
       </c>
@@ -2571,7 +2603,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>317</v>
       </c>
@@ -2585,7 +2617,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>317</v>
       </c>
@@ -2599,7 +2631,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>317</v>
       </c>
@@ -2613,7 +2645,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>317</v>
       </c>
@@ -2627,7 +2659,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>317</v>
       </c>
@@ -2641,7 +2673,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>317</v>
       </c>
@@ -2655,7 +2687,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>317</v>
       </c>
@@ -2669,7 +2701,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>317</v>
       </c>
@@ -2683,7 +2715,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>317</v>
       </c>
@@ -2697,7 +2729,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>317</v>
       </c>
@@ -2711,7 +2743,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>317</v>
       </c>
@@ -2725,7 +2757,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>317</v>
       </c>
@@ -2739,7 +2771,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>317</v>
       </c>
@@ -2753,7 +2785,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>317</v>
       </c>
@@ -2767,7 +2799,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>317</v>
       </c>
@@ -2781,7 +2813,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>317</v>
       </c>
@@ -2795,7 +2827,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>317</v>
       </c>
@@ -2809,7 +2841,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>317</v>
       </c>
@@ -2823,7 +2855,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>317</v>
       </c>
@@ -2837,7 +2869,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>317</v>
       </c>
@@ -2851,7 +2883,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>317</v>
       </c>
@@ -2865,7 +2897,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>317</v>
       </c>
@@ -2879,7 +2911,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>317</v>
       </c>
@@ -2893,7 +2925,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>317</v>
       </c>
@@ -2907,7 +2939,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>317</v>
       </c>
@@ -2921,7 +2953,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>317</v>
       </c>
@@ -2935,7 +2967,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>317</v>
       </c>
@@ -2949,7 +2981,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>317</v>
       </c>
@@ -2963,7 +2995,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>317</v>
       </c>
@@ -2977,7 +3009,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>317</v>
       </c>
@@ -2991,7 +3023,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>317</v>
       </c>
@@ -3005,7 +3037,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>317</v>
       </c>
@@ -3022,7 +3054,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>317</v>
       </c>
@@ -3036,7 +3068,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>317</v>
       </c>
@@ -3050,7 +3082,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>317</v>
       </c>
@@ -3064,7 +3096,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>317</v>
       </c>
@@ -3078,7 +3110,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>317</v>
       </c>
@@ -3092,7 +3124,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>317</v>
       </c>
@@ -3106,7 +3138,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>317</v>
       </c>
@@ -3120,7 +3152,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>317</v>
       </c>
@@ -3134,7 +3166,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>317</v>
       </c>
@@ -3148,7 +3180,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>317</v>
       </c>
@@ -3162,7 +3194,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>317</v>
       </c>
@@ -3176,7 +3208,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>317</v>
       </c>
@@ -3190,7 +3222,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>317</v>
       </c>
@@ -3204,7 +3236,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>317</v>
       </c>
@@ -3218,7 +3250,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>317</v>
       </c>
@@ -3232,7 +3264,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>317</v>
       </c>
@@ -3246,7 +3278,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>317</v>
       </c>
@@ -3260,7 +3292,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>317</v>
       </c>
@@ -3274,7 +3306,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>317</v>
       </c>
@@ -3288,7 +3320,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>317</v>
       </c>
@@ -3302,7 +3334,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>317</v>
       </c>
@@ -3316,7 +3348,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>317</v>
       </c>
@@ -3330,7 +3362,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>317</v>
       </c>
@@ -3344,7 +3376,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>317</v>
       </c>
@@ -3358,7 +3390,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>317</v>
       </c>
@@ -3372,7 +3404,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>317</v>
       </c>
@@ -3386,7 +3418,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>317</v>
       </c>
@@ -3400,7 +3432,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>317</v>
       </c>
@@ -3414,7 +3446,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>317</v>
       </c>
@@ -3428,7 +3460,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>317</v>
       </c>
@@ -3442,7 +3474,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>317</v>
       </c>
@@ -3456,7 +3488,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>317</v>
       </c>
@@ -3470,7 +3502,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>317</v>
       </c>
@@ -3484,7 +3516,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>317</v>
       </c>
@@ -3498,7 +3530,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>317</v>
       </c>
@@ -3512,7 +3544,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>317</v>
       </c>
@@ -3526,7 +3558,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>317</v>
       </c>
@@ -3540,7 +3572,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>317</v>
       </c>
@@ -3554,7 +3586,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>317</v>
       </c>
@@ -3568,7 +3600,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>317</v>
       </c>
@@ -3582,7 +3614,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>317</v>
       </c>
@@ -3596,7 +3628,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>317</v>
       </c>
@@ -3613,7 +3645,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>317</v>
       </c>
@@ -3630,7 +3662,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>317</v>
       </c>
@@ -3644,7 +3676,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>317</v>
       </c>
@@ -3658,7 +3690,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>317</v>
       </c>
@@ -3672,7 +3704,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>317</v>
       </c>
@@ -3686,7 +3718,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>317</v>
       </c>
@@ -3700,7 +3732,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>317</v>
       </c>
@@ -3714,7 +3746,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>317</v>
       </c>
@@ -3728,7 +3760,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>317</v>
       </c>
@@ -3742,7 +3774,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>317</v>
       </c>
@@ -3756,7 +3788,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>317</v>
       </c>
@@ -3770,7 +3802,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>317</v>
       </c>
@@ -3784,7 +3816,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>317</v>
       </c>
@@ -3798,7 +3830,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>317</v>
       </c>
@@ -3812,7 +3844,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>317</v>
       </c>
@@ -3829,7 +3861,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>317</v>
       </c>
@@ -3843,7 +3875,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>317</v>
       </c>
@@ -3860,7 +3892,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>317</v>
       </c>
@@ -3874,7 +3906,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>317</v>
       </c>
@@ -3888,7 +3920,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>317</v>
       </c>
@@ -3902,7 +3934,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>317</v>
       </c>
@@ -3916,7 +3948,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>317</v>
       </c>
@@ -3930,7 +3962,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>317</v>
       </c>
@@ -3944,7 +3976,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>317</v>
       </c>
@@ -3958,7 +3990,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>317</v>
       </c>
@@ -3972,7 +4004,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>317</v>
       </c>
@@ -3986,7 +4018,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>317</v>
       </c>
@@ -4003,7 +4035,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>317</v>
       </c>
@@ -4017,7 +4049,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>317</v>
       </c>
@@ -4031,7 +4063,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>317</v>
       </c>
@@ -4045,7 +4077,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>317</v>
       </c>
@@ -4059,7 +4091,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>317</v>
       </c>
@@ -4073,7 +4105,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>317</v>
       </c>
@@ -4087,7 +4119,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>317</v>
       </c>
@@ -4101,7 +4133,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>317</v>
       </c>
@@ -4115,7 +4147,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>317</v>
       </c>
@@ -4129,7 +4161,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>317</v>
       </c>
@@ -4143,7 +4175,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>317</v>
       </c>
@@ -4157,7 +4189,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>317</v>
       </c>
@@ -4171,7 +4203,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>317</v>
       </c>
@@ -4185,7 +4217,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>317</v>
       </c>
@@ -4199,7 +4231,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>317</v>
       </c>
@@ -4213,7 +4245,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>317</v>
       </c>
@@ -4227,7 +4259,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>441</v>
       </c>
@@ -4241,7 +4273,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>441</v>
       </c>
@@ -4255,7 +4287,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>441</v>
       </c>
@@ -4269,7 +4301,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>441</v>
       </c>
@@ -4283,7 +4315,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>441</v>
       </c>
@@ -4297,7 +4329,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>441</v>
       </c>
@@ -4311,7 +4343,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>441</v>
       </c>
@@ -4325,7 +4357,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>441</v>
       </c>
@@ -4339,7 +4371,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>441</v>
       </c>
@@ -4356,7 +4388,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>441</v>
       </c>
@@ -4370,7 +4402,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>441</v>
       </c>
@@ -4387,7 +4419,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>441</v>
       </c>
@@ -4401,7 +4433,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>441</v>
       </c>
@@ -4415,7 +4447,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>441</v>
       </c>
@@ -4432,35 +4464,35 @@
         <v>316</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>441</v>
       </c>
       <c r="B159" t="s">
+        <v>474</v>
+      </c>
+      <c r="C159" t="s">
+        <v>475</v>
+      </c>
+      <c r="E159" s="3" t="s">
         <v>476</v>
       </c>
-      <c r="C159" t="s">
-        <v>477</v>
-      </c>
-      <c r="E159" s="3" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="160" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>441</v>
       </c>
       <c r="B160" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C160" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>459</v>
       </c>
@@ -4468,13 +4500,13 @@
         <v>460</v>
       </c>
       <c r="C161" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>459</v>
       </c>
@@ -4482,16 +4514,16 @@
         <v>460</v>
       </c>
       <c r="C162" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="F162" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>459</v>
       </c>
@@ -4499,13 +4531,13 @@
         <v>460</v>
       </c>
       <c r="C163" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>459</v>
       </c>
@@ -4513,13 +4545,13 @@
         <v>460</v>
       </c>
       <c r="C164" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>459</v>
       </c>
@@ -4527,13 +4559,13 @@
         <v>460</v>
       </c>
       <c r="C165" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>459</v>
       </c>
@@ -4541,7 +4573,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>355</v>
       </c>
@@ -4555,10 +4587,10 @@
         <v>319</v>
       </c>
       <c r="F167" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>355</v>
       </c>
@@ -4569,13 +4601,13 @@
         <v>361</v>
       </c>
       <c r="E168" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F168" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>356</v>
       </c>
@@ -4589,7 +4621,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>356</v>
       </c>
@@ -4600,10 +4632,10 @@
         <v>456</v>
       </c>
       <c r="E170" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>356</v>
       </c>
@@ -4614,13 +4646,13 @@
         <v>321</v>
       </c>
       <c r="E171" t="s">
+        <v>535</v>
+      </c>
+      <c r="F171" t="s">
         <v>538</v>
       </c>
-      <c r="F171" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>356</v>
       </c>
@@ -4634,10 +4666,10 @@
         <v>323</v>
       </c>
       <c r="F172" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>356</v>
       </c>
@@ -4651,10 +4683,10 @@
         <v>325</v>
       </c>
       <c r="F173" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>356</v>
       </c>
@@ -4668,10 +4700,10 @@
         <v>327</v>
       </c>
       <c r="F174" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>356</v>
       </c>
@@ -4685,10 +4717,10 @@
         <v>329</v>
       </c>
       <c r="F175" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>356</v>
       </c>
@@ -4702,10 +4734,10 @@
         <v>331</v>
       </c>
       <c r="F176" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>356</v>
       </c>
@@ -4719,10 +4751,10 @@
         <v>333</v>
       </c>
       <c r="F177" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>356</v>
       </c>
@@ -4736,10 +4768,10 @@
         <v>335</v>
       </c>
       <c r="F178" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>356</v>
       </c>
@@ -4753,7 +4785,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>356</v>
       </c>
@@ -4767,9 +4799,9 @@
         <v>339</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B181" t="s">
         <v>1</v>
@@ -4784,9 +4816,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B182" t="s">
         <v>1</v>
@@ -4801,9 +4833,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B183" t="s">
         <v>1</v>
@@ -4818,9 +4850,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B184" t="s">
         <v>1</v>
@@ -4835,9 +4867,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B185" t="s">
         <v>1</v>
@@ -4852,9 +4884,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B186" t="s">
         <v>1</v>
@@ -4869,7 +4901,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>357</v>
       </c>
@@ -4886,7 +4918,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>357</v>
       </c>
@@ -4903,7 +4935,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>357</v>
       </c>
@@ -4920,7 +4952,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>357</v>
       </c>
@@ -4937,7 +4969,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>357</v>
       </c>
@@ -4954,7 +4986,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>357</v>
       </c>
@@ -4971,7 +5003,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>357</v>
       </c>
@@ -4988,7 +5020,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>357</v>
       </c>
@@ -5005,7 +5037,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>357</v>
       </c>
@@ -5022,7 +5054,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>357</v>
       </c>
@@ -5039,7 +5071,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>357</v>
       </c>
@@ -5056,7 +5088,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>357</v>
       </c>
@@ -5073,7 +5105,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>357</v>
       </c>
@@ -5090,7 +5122,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>357</v>
       </c>
@@ -5107,7 +5139,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>357</v>
       </c>
@@ -5124,7 +5156,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>357</v>
       </c>
@@ -5141,7 +5173,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>357</v>
       </c>
@@ -5158,7 +5190,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>357</v>
       </c>
@@ -5175,7 +5207,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>357</v>
       </c>
@@ -5192,7 +5224,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>357</v>
       </c>
@@ -5209,7 +5241,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>357</v>
       </c>
@@ -5226,7 +5258,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>357</v>
       </c>
@@ -5243,7 +5275,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>357</v>
       </c>
@@ -5260,7 +5292,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>357</v>
       </c>
@@ -5277,7 +5309,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>357</v>
       </c>
@@ -5294,7 +5326,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>357</v>
       </c>
@@ -5311,7 +5343,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>357</v>
       </c>
@@ -5328,7 +5360,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>357</v>
       </c>
@@ -5345,7 +5377,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>357</v>
       </c>
@@ -5362,7 +5394,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>357</v>
       </c>
@@ -5379,7 +5411,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>423</v>
       </c>
@@ -5396,7 +5428,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>423</v>
       </c>
@@ -5413,7 +5445,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>423</v>
       </c>
@@ -5430,7 +5462,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>423</v>
       </c>
@@ -5447,7 +5479,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>423</v>
       </c>
@@ -5464,7 +5496,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>423</v>
       </c>
@@ -5481,7 +5513,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>423</v>
       </c>
@@ -5498,7 +5530,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>424</v>
       </c>
@@ -5515,7 +5547,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>424</v>
       </c>
@@ -5532,7 +5564,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>424</v>
       </c>
@@ -5549,7 +5581,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>424</v>
       </c>
@@ -5566,7 +5598,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>424</v>
       </c>
@@ -5583,7 +5615,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>464</v>
       </c>
@@ -5597,7 +5629,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>464</v>
       </c>
@@ -5608,318 +5640,355 @@
         <v>468</v>
       </c>
       <c r="E230" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B231" t="s">
+        <v>481</v>
+      </c>
+      <c r="C231" t="s">
+        <v>482</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="F231" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>484</v>
+      </c>
+      <c r="B232" t="s">
+        <v>481</v>
+      </c>
+      <c r="C232" t="s">
+        <v>483</v>
+      </c>
+      <c r="E232" t="s">
+        <v>496</v>
+      </c>
+      <c r="F232" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B233" t="s">
         <v>462</v>
       </c>
-      <c r="C231" t="s">
+      <c r="C233" t="s">
         <v>463</v>
       </c>
-      <c r="E231" t="s">
+      <c r="E233" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="1" t="s">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B234" t="s">
         <v>462</v>
       </c>
-      <c r="C232" t="s">
+      <c r="C234" t="s">
         <v>468</v>
       </c>
-      <c r="E232" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B233" t="s">
-        <v>482</v>
-      </c>
-      <c r="C233" t="s">
+      <c r="E234" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B235" t="s">
+        <v>480</v>
+      </c>
+      <c r="C235" t="s">
+        <v>488</v>
+      </c>
+      <c r="E235" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="F235" t="s">
         <v>490</v>
       </c>
-      <c r="E233" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="F233" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" ht="150" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B234" t="s">
-        <v>482</v>
-      </c>
-      <c r="C234" t="s">
-        <v>491</v>
-      </c>
-      <c r="E234" s="3" t="s">
-        <v>500</v>
-      </c>
-      <c r="F234" t="s">
+    </row>
+    <row r="236" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B236" t="s">
+        <v>480</v>
+      </c>
+      <c r="C236" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="235" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B235" t="s">
-        <v>482</v>
-      </c>
-      <c r="C235" t="s">
-        <v>493</v>
-      </c>
-      <c r="E235" s="3" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B236" t="s">
-        <v>483</v>
-      </c>
-      <c r="C236" t="s">
-        <v>484</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>495</v>
+      <c r="E236" s="3" t="s">
+        <v>498</v>
       </c>
       <c r="F236" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B237" t="s">
+        <v>480</v>
+      </c>
+      <c r="C237" t="s">
+        <v>491</v>
+      </c>
+      <c r="E237" s="3" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B238" t="s">
         <v>481</v>
       </c>
-      <c r="B237" t="s">
+      <c r="C238" t="s">
+        <v>482</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="F238" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A239" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B239" t="s">
+        <v>481</v>
+      </c>
+      <c r="C239" t="s">
         <v>483</v>
       </c>
-      <c r="C237" t="s">
-        <v>485</v>
-      </c>
-      <c r="E237" t="s">
-        <v>496</v>
-      </c>
-      <c r="F237" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B238" t="s">
+      <c r="E239" t="s">
+        <v>494</v>
+      </c>
+      <c r="F239" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A240" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B240" t="s">
+        <v>499</v>
+      </c>
+      <c r="C240" t="s">
+        <v>500</v>
+      </c>
+      <c r="E240" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="C238" t="s">
+      <c r="F240" t="s">
         <v>502</v>
       </c>
-      <c r="E238" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="F238" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="B239" t="s">
-        <v>483</v>
-      </c>
-      <c r="C239" t="s">
-        <v>484</v>
-      </c>
-      <c r="E239" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="F239" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="240" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
-        <v>486</v>
-      </c>
-      <c r="B240" t="s">
-        <v>483</v>
-      </c>
-      <c r="C240" t="s">
-        <v>485</v>
-      </c>
-      <c r="E240" t="s">
-        <v>498</v>
-      </c>
-      <c r="F240" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="241" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B241" t="s">
+        <v>578</v>
+      </c>
+      <c r="C241" t="s">
+        <v>575</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="F241" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B242" t="s">
+        <v>571</v>
+      </c>
+      <c r="C242" t="s">
+        <v>572</v>
+      </c>
+      <c r="E242" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="F242" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A243" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B243" t="s">
+        <v>506</v>
+      </c>
+      <c r="C243" t="s">
         <v>508</v>
       </c>
-      <c r="C241" t="s">
+      <c r="E243" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="F243" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B244" t="s">
+        <v>506</v>
+      </c>
+      <c r="C244" t="s">
+        <v>509</v>
+      </c>
+      <c r="E244" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="E241" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="F241" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="242" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B242" t="s">
-        <v>508</v>
-      </c>
-      <c r="C242" t="s">
+      <c r="F244" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A245" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B245" t="s">
+        <v>505</v>
+      </c>
+      <c r="C245" t="s">
         <v>511</v>
       </c>
-      <c r="E242" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="F242" s="2" t="s">
+      <c r="E245" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="F245" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A246" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B246" t="s">
+        <v>506</v>
+      </c>
+      <c r="C246" t="s">
+        <v>513</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="F246" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A247" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B247" t="s">
+        <v>505</v>
+      </c>
+      <c r="C247" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="243" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A243" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B243" t="s">
-        <v>507</v>
-      </c>
-      <c r="C243" t="s">
-        <v>513</v>
-      </c>
-      <c r="E243" s="3" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A244" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B244" t="s">
-        <v>508</v>
-      </c>
-      <c r="C244" t="s">
+      <c r="E247" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="E244" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="F244" t="s">
+      <c r="F247" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A248" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B248" t="s">
+        <v>505</v>
+      </c>
+      <c r="C248" t="s">
+        <v>525</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="F248" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B249" t="s">
+        <v>505</v>
+      </c>
+      <c r="C249" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B245" t="s">
-        <v>507</v>
-      </c>
-      <c r="C245" t="s">
+      <c r="E249" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="E245" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="F245" t="s">
+      <c r="F249" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B250" t="s">
+        <v>505</v>
+      </c>
+      <c r="C250" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B246" t="s">
-        <v>507</v>
-      </c>
-      <c r="C246" t="s">
-        <v>528</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="F246" t="s">
+      <c r="E250" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="F250" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A247" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B247" t="s">
-        <v>507</v>
-      </c>
-      <c r="C247" t="s">
-        <v>520</v>
-      </c>
-      <c r="E247" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="F247" t="s">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B251" t="s">
+        <v>506</v>
+      </c>
+      <c r="C251" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="248" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A248" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B248" t="s">
-        <v>507</v>
-      </c>
-      <c r="C248" t="s">
+      <c r="E251" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="F251" t="s">
         <v>532</v>
-      </c>
-      <c r="E248" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="F248" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A249" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B249" t="s">
-        <v>508</v>
-      </c>
-      <c r="C249" t="s">
-        <v>534</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="F249" t="s">
-        <v>535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added snippets - close #886
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="snippets" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="584">
   <si>
     <t>set</t>
   </si>
@@ -1801,6 +1801,25 @@
   </si>
   <si>
     <t>string-url-path</t>
+  </si>
+  <si>
+    <t>ASP.net Page</t>
+  </si>
+  <si>
+    <t>Set page title</t>
+  </si>
+  <si>
+    <t>Set header metadata</t>
+  </si>
+  <si>
+    <t>// set page title
+var page = HttpContext.Current.Handler as Page;
+page.Title = "${1:This page title works}";</t>
+  </si>
+  <si>
+    <t>// set MetaDescription - page variable must be declared before
+var metaDescription = (HtmlMeta)page.FindControl("metaDescription");
+metaDescription.Content = "${1:This MetaDescription works}";</t>
   </si>
 </sst>
 </file>
@@ -1863,8 +1882,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F251" totalsRowShown="0">
-  <autoFilter ref="A1:F251"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F253" totalsRowShown="0">
+  <autoFilter ref="A1:F253"/>
   <tableColumns count="6">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -2140,10 +2159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F251"/>
+  <dimension ref="A1:F253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="C241" sqref="C241"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="E169" sqref="E169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4573,66 +4592,66 @@
         <v>460</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>355</v>
+    <row r="167" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>459</v>
       </c>
       <c r="B167" t="s">
-        <v>359</v>
+        <v>579</v>
       </c>
       <c r="C167" t="s">
-        <v>360</v>
-      </c>
-      <c r="E167" t="s">
-        <v>319</v>
-      </c>
-      <c r="F167" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>355</v>
+        <v>580</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>459</v>
       </c>
       <c r="B168" t="s">
-        <v>359</v>
+        <v>579</v>
       </c>
       <c r="C168" t="s">
-        <v>361</v>
-      </c>
-      <c r="E168" t="s">
-        <v>536</v>
-      </c>
-      <c r="F168" t="s">
-        <v>545</v>
+        <v>581</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B169" t="s">
-        <v>58</v>
+        <v>359</v>
       </c>
       <c r="C169" t="s">
-        <v>455</v>
+        <v>360</v>
       </c>
       <c r="E169" t="s">
-        <v>320</v>
+        <v>319</v>
+      </c>
+      <c r="F169" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B170" t="s">
-        <v>58</v>
+        <v>359</v>
       </c>
       <c r="C170" t="s">
-        <v>456</v>
+        <v>361</v>
       </c>
       <c r="E170" t="s">
-        <v>537</v>
+        <v>536</v>
+      </c>
+      <c r="F170" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -4640,16 +4659,13 @@
         <v>356</v>
       </c>
       <c r="B171" t="s">
-        <v>321</v>
+        <v>58</v>
       </c>
       <c r="C171" t="s">
-        <v>321</v>
+        <v>455</v>
       </c>
       <c r="E171" t="s">
-        <v>535</v>
-      </c>
-      <c r="F171" t="s">
-        <v>538</v>
+        <v>320</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -4657,16 +4673,13 @@
         <v>356</v>
       </c>
       <c r="B172" t="s">
-        <v>358</v>
+        <v>58</v>
       </c>
       <c r="C172" t="s">
-        <v>322</v>
+        <v>456</v>
       </c>
       <c r="E172" t="s">
-        <v>323</v>
-      </c>
-      <c r="F172" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -4674,16 +4687,16 @@
         <v>356</v>
       </c>
       <c r="B173" t="s">
-        <v>358</v>
+        <v>321</v>
       </c>
       <c r="C173" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E173" t="s">
-        <v>325</v>
+        <v>535</v>
       </c>
       <c r="F173" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -4694,13 +4707,13 @@
         <v>358</v>
       </c>
       <c r="C174" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E174" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F174" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -4711,13 +4724,13 @@
         <v>358</v>
       </c>
       <c r="C175" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E175" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F175" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -4728,13 +4741,13 @@
         <v>358</v>
       </c>
       <c r="C176" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E176" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F176" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -4745,13 +4758,13 @@
         <v>358</v>
       </c>
       <c r="C177" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E177" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F177" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -4762,13 +4775,13 @@
         <v>358</v>
       </c>
       <c r="C178" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E178" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F178" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -4779,10 +4792,13 @@
         <v>358</v>
       </c>
       <c r="C179" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E179" t="s">
-        <v>337</v>
+        <v>333</v>
+      </c>
+      <c r="F179" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
@@ -4793,44 +4809,41 @@
         <v>358</v>
       </c>
       <c r="C180" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E180" t="s">
-        <v>339</v>
+        <v>335</v>
+      </c>
+      <c r="F180" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>478</v>
+        <v>356</v>
       </c>
       <c r="B181" t="s">
-        <v>1</v>
+        <v>358</v>
       </c>
       <c r="C181" t="s">
-        <v>2</v>
+        <v>336</v>
       </c>
       <c r="E181" t="s">
-        <v>340</v>
-      </c>
-      <c r="F181" t="s">
-        <v>28</v>
+        <v>337</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>478</v>
+        <v>356</v>
       </c>
       <c r="B182" t="s">
-        <v>1</v>
+        <v>358</v>
       </c>
       <c r="C182" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="E182" t="s">
-        <v>341</v>
-      </c>
-      <c r="F182" t="s">
-        <v>27</v>
+        <v>339</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
@@ -4841,13 +4854,13 @@
         <v>1</v>
       </c>
       <c r="C183" t="s">
-        <v>215</v>
+        <v>2</v>
       </c>
       <c r="E183" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F183" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
@@ -4858,13 +4871,13 @@
         <v>1</v>
       </c>
       <c r="C184" t="s">
-        <v>22</v>
+        <v>362</v>
       </c>
       <c r="E184" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F184" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
@@ -4875,13 +4888,13 @@
         <v>1</v>
       </c>
       <c r="C185" t="s">
-        <v>363</v>
+        <v>215</v>
       </c>
       <c r="E185" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F185" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
@@ -4892,47 +4905,47 @@
         <v>1</v>
       </c>
       <c r="C186" t="s">
-        <v>364</v>
+        <v>22</v>
       </c>
       <c r="E186" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F186" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>357</v>
+        <v>478</v>
       </c>
       <c r="B187" t="s">
-        <v>303</v>
+        <v>1</v>
       </c>
       <c r="C187" t="s">
-        <v>112</v>
+        <v>363</v>
       </c>
       <c r="E187" t="s">
-        <v>387</v>
+        <v>344</v>
       </c>
       <c r="F187" t="s">
-        <v>388</v>
+        <v>14</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>357</v>
+        <v>478</v>
       </c>
       <c r="B188" t="s">
-        <v>303</v>
+        <v>1</v>
       </c>
       <c r="C188" t="s">
-        <v>54</v>
+        <v>364</v>
       </c>
       <c r="E188" t="s">
-        <v>389</v>
+        <v>345</v>
       </c>
       <c r="F188" t="s">
-        <v>390</v>
+        <v>18</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
@@ -4943,13 +4956,13 @@
         <v>303</v>
       </c>
       <c r="C189" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="E189" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="F189" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
@@ -4960,13 +4973,13 @@
         <v>303</v>
       </c>
       <c r="C190" t="s">
-        <v>426</v>
+        <v>54</v>
       </c>
       <c r="E190" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F190" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
@@ -4977,13 +4990,13 @@
         <v>303</v>
       </c>
       <c r="C191" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E191" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F191" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
@@ -4994,13 +5007,13 @@
         <v>303</v>
       </c>
       <c r="C192" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E192" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="F192" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -5011,13 +5024,13 @@
         <v>303</v>
       </c>
       <c r="C193" t="s">
-        <v>427</v>
+        <v>58</v>
       </c>
       <c r="E193" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="F193" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
@@ -5028,13 +5041,13 @@
         <v>303</v>
       </c>
       <c r="C194" t="s">
-        <v>174</v>
+        <v>428</v>
       </c>
       <c r="E194" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="F194" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
@@ -5045,13 +5058,13 @@
         <v>303</v>
       </c>
       <c r="C195" t="s">
-        <v>84</v>
+        <v>427</v>
       </c>
       <c r="E195" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="F195" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
@@ -5062,13 +5075,13 @@
         <v>303</v>
       </c>
       <c r="C196" t="s">
-        <v>90</v>
+        <v>174</v>
       </c>
       <c r="E196" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="F196" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
@@ -5076,16 +5089,16 @@
         <v>357</v>
       </c>
       <c r="B197" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C197" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="E197" t="s">
-        <v>365</v>
+        <v>403</v>
       </c>
       <c r="F197" t="s">
-        <v>366</v>
+        <v>404</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
@@ -5093,16 +5106,16 @@
         <v>357</v>
       </c>
       <c r="B198" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C198" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="E198" t="s">
-        <v>367</v>
+        <v>405</v>
       </c>
       <c r="F198" t="s">
-        <v>368</v>
+        <v>406</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
@@ -5113,13 +5126,13 @@
         <v>304</v>
       </c>
       <c r="C199" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E199" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="F199" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
@@ -5130,13 +5143,13 @@
         <v>304</v>
       </c>
       <c r="C200" t="s">
-        <v>427</v>
+        <v>54</v>
       </c>
       <c r="E200" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F200" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
@@ -5147,13 +5160,13 @@
         <v>304</v>
       </c>
       <c r="C201" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="E201" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F201" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
@@ -5164,13 +5177,13 @@
         <v>304</v>
       </c>
       <c r="C202" t="s">
-        <v>141</v>
+        <v>427</v>
       </c>
       <c r="E202" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="F202" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
@@ -5181,13 +5194,13 @@
         <v>304</v>
       </c>
       <c r="C203" t="s">
-        <v>90</v>
+        <v>131</v>
       </c>
       <c r="E203" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="F203" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
@@ -5198,13 +5211,13 @@
         <v>304</v>
       </c>
       <c r="C204" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="E204" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="F204" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
@@ -5215,13 +5228,13 @@
         <v>304</v>
       </c>
       <c r="C205" t="s">
-        <v>166</v>
+        <v>90</v>
       </c>
       <c r="E205" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="F205" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
@@ -5232,13 +5245,13 @@
         <v>304</v>
       </c>
       <c r="C206" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E206" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="F206" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
@@ -5249,13 +5262,13 @@
         <v>304</v>
       </c>
       <c r="C207" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="E207" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F207" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
@@ -5263,16 +5276,16 @@
         <v>357</v>
       </c>
       <c r="B208" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C208" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="E208" t="s">
-        <v>346</v>
+        <v>383</v>
       </c>
       <c r="F208" t="s">
-        <v>439</v>
+        <v>384</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
@@ -5280,16 +5293,16 @@
         <v>357</v>
       </c>
       <c r="B209" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C209" t="s">
-        <v>112</v>
+        <v>177</v>
       </c>
       <c r="E209" t="s">
-        <v>347</v>
+        <v>385</v>
       </c>
       <c r="F209" t="s">
-        <v>438</v>
+        <v>386</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
@@ -5300,13 +5313,13 @@
         <v>305</v>
       </c>
       <c r="C210" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="E210" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F210" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
@@ -5317,13 +5330,13 @@
         <v>305</v>
       </c>
       <c r="C211" t="s">
-        <v>213</v>
+        <v>112</v>
       </c>
       <c r="E211" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F211" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
@@ -5334,13 +5347,13 @@
         <v>305</v>
       </c>
       <c r="C212" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="E212" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F212" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
@@ -5351,13 +5364,13 @@
         <v>305</v>
       </c>
       <c r="C213" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="E213" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F213" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
@@ -5368,13 +5381,13 @@
         <v>305</v>
       </c>
       <c r="C214" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="E214" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F214" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
@@ -5385,13 +5398,13 @@
         <v>305</v>
       </c>
       <c r="C215" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E215" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F215" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
@@ -5402,47 +5415,47 @@
         <v>305</v>
       </c>
       <c r="C216" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="E216" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F216" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B217" t="s">
-        <v>425</v>
+        <v>305</v>
       </c>
       <c r="C217" t="s">
-        <v>278</v>
+        <v>230</v>
       </c>
       <c r="E217" t="s">
-        <v>409</v>
+        <v>353</v>
       </c>
       <c r="F217" t="s">
-        <v>410</v>
+        <v>432</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B218" t="s">
-        <v>425</v>
+        <v>305</v>
       </c>
       <c r="C218" t="s">
-        <v>205</v>
+        <v>262</v>
       </c>
       <c r="E218" t="s">
-        <v>411</v>
+        <v>354</v>
       </c>
       <c r="F218" t="s">
-        <v>412</v>
+        <v>431</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
@@ -5453,13 +5466,13 @@
         <v>425</v>
       </c>
       <c r="C219" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E219" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="F219" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
@@ -5470,13 +5483,13 @@
         <v>425</v>
       </c>
       <c r="C220" t="s">
-        <v>283</v>
+        <v>205</v>
       </c>
       <c r="E220" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F220" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
@@ -5487,13 +5500,13 @@
         <v>425</v>
       </c>
       <c r="C221" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="E221" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F221" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
@@ -5504,13 +5517,13 @@
         <v>425</v>
       </c>
       <c r="C222" t="s">
-        <v>430</v>
+        <v>283</v>
       </c>
       <c r="E222" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F222" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
@@ -5518,50 +5531,50 @@
         <v>423</v>
       </c>
       <c r="B223" t="s">
-        <v>306</v>
+        <v>425</v>
       </c>
       <c r="C223" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="E223" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F223" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B224" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C224" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E224" t="s">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="F224" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B225" t="s">
-        <v>442</v>
+        <v>306</v>
       </c>
       <c r="C225" t="s">
-        <v>443</v>
+        <v>306</v>
       </c>
       <c r="E225" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
       <c r="F225" t="s">
-        <v>445</v>
+        <v>422</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
@@ -5569,16 +5582,16 @@
         <v>424</v>
       </c>
       <c r="B226" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="C226" t="s">
-        <v>448</v>
+        <v>429</v>
       </c>
       <c r="E226" t="s">
-        <v>446</v>
+        <v>407</v>
       </c>
       <c r="F226" t="s">
-        <v>447</v>
+        <v>408</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
@@ -5589,13 +5602,13 @@
         <v>442</v>
       </c>
       <c r="C227" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="E227" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="F227" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5606,140 +5619,140 @@
         <v>442</v>
       </c>
       <c r="C228" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="E228" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="F228" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
+        <v>424</v>
+      </c>
+      <c r="B229" t="s">
+        <v>442</v>
+      </c>
+      <c r="C229" t="s">
+        <v>449</v>
+      </c>
+      <c r="E229" t="s">
+        <v>450</v>
+      </c>
+      <c r="F229" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>424</v>
+      </c>
+      <c r="B230" t="s">
+        <v>442</v>
+      </c>
+      <c r="C230" t="s">
+        <v>452</v>
+      </c>
+      <c r="E230" t="s">
+        <v>453</v>
+      </c>
+      <c r="F230" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
         <v>464</v>
       </c>
-      <c r="B229" t="s">
+      <c r="B231" t="s">
         <v>462</v>
       </c>
-      <c r="C229" t="s">
+      <c r="C231" t="s">
         <v>463</v>
       </c>
-      <c r="E229" t="s">
+      <c r="E231" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A230" s="1" t="s">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B232" t="s">
         <v>462</v>
       </c>
-      <c r="C230" t="s">
+      <c r="C232" t="s">
         <v>468</v>
       </c>
-      <c r="E230" t="s">
+      <c r="E232" t="s">
         <v>564</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A231" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="B231" t="s">
-        <v>481</v>
-      </c>
-      <c r="C231" t="s">
-        <v>482</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="F231" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>484</v>
-      </c>
-      <c r="B232" t="s">
-        <v>481</v>
-      </c>
-      <c r="C232" t="s">
-        <v>483</v>
-      </c>
-      <c r="E232" t="s">
-        <v>496</v>
-      </c>
-      <c r="F232" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B233" t="s">
+        <v>481</v>
+      </c>
+      <c r="C233" t="s">
+        <v>482</v>
+      </c>
+      <c r="E233" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="F233" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>484</v>
+      </c>
+      <c r="B234" t="s">
+        <v>481</v>
+      </c>
+      <c r="C234" t="s">
+        <v>483</v>
+      </c>
+      <c r="E234" t="s">
+        <v>496</v>
+      </c>
+      <c r="F234" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B233" t="s">
+      <c r="B235" t="s">
         <v>462</v>
       </c>
-      <c r="C233" t="s">
+      <c r="C235" t="s">
         <v>463</v>
       </c>
-      <c r="E233" t="s">
+      <c r="E235" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A234" s="1" t="s">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B234" t="s">
+      <c r="B236" t="s">
         <v>462</v>
       </c>
-      <c r="C234" t="s">
+      <c r="C236" t="s">
         <v>468</v>
       </c>
-      <c r="E234" t="s">
+      <c r="E236" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A235" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B235" t="s">
-        <v>480</v>
-      </c>
-      <c r="C235" t="s">
-        <v>488</v>
-      </c>
-      <c r="E235" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="F235" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A236" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B236" t="s">
-        <v>480</v>
-      </c>
-      <c r="C236" t="s">
-        <v>489</v>
-      </c>
-      <c r="E236" s="3" t="s">
-        <v>498</v>
-      </c>
-      <c r="F236" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>479</v>
       </c>
@@ -5747,44 +5760,44 @@
         <v>480</v>
       </c>
       <c r="C237" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E237" s="3" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+        <v>497</v>
+      </c>
+      <c r="F237" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B238" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C238" t="s">
-        <v>482</v>
-      </c>
-      <c r="E238" s="1" t="s">
-        <v>493</v>
+        <v>489</v>
+      </c>
+      <c r="E238" s="3" t="s">
+        <v>498</v>
       </c>
       <c r="F238" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B239" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C239" t="s">
-        <v>483</v>
-      </c>
-      <c r="E239" t="s">
-        <v>494</v>
-      </c>
-      <c r="F239" t="s">
-        <v>486</v>
+        <v>491</v>
+      </c>
+      <c r="E239" s="3" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
@@ -5792,16 +5805,16 @@
         <v>479</v>
       </c>
       <c r="B240" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
       <c r="C240" t="s">
-        <v>500</v>
+        <v>482</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="F240" t="s">
-        <v>502</v>
+        <v>485</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
@@ -5809,16 +5822,16 @@
         <v>479</v>
       </c>
       <c r="B241" t="s">
-        <v>578</v>
+        <v>481</v>
       </c>
       <c r="C241" t="s">
-        <v>575</v>
-      </c>
-      <c r="E241" s="1" t="s">
-        <v>577</v>
+        <v>483</v>
+      </c>
+      <c r="E241" t="s">
+        <v>494</v>
       </c>
       <c r="F241" t="s">
-        <v>576</v>
+        <v>486</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
@@ -5826,70 +5839,70 @@
         <v>479</v>
       </c>
       <c r="B242" t="s">
-        <v>571</v>
+        <v>499</v>
       </c>
       <c r="C242" t="s">
-        <v>572</v>
-      </c>
-      <c r="E242" s="3" t="s">
-        <v>573</v>
+        <v>500</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>501</v>
       </c>
       <c r="F242" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="243" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B243" t="s">
-        <v>506</v>
+        <v>578</v>
       </c>
       <c r="C243" t="s">
-        <v>508</v>
-      </c>
-      <c r="E243" s="2" t="s">
-        <v>563</v>
+        <v>575</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>577</v>
       </c>
       <c r="F243" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="244" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B244" t="s">
-        <v>506</v>
+        <v>571</v>
       </c>
       <c r="C244" t="s">
-        <v>509</v>
-      </c>
-      <c r="E244" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="F244" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="245" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>572</v>
+      </c>
+      <c r="E244" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="F244" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B245" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C245" t="s">
-        <v>511</v>
-      </c>
-      <c r="E245" s="3" t="s">
-        <v>569</v>
+        <v>508</v>
+      </c>
+      <c r="E245" s="2" t="s">
+        <v>563</v>
       </c>
       <c r="F245" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>479</v>
       </c>
@@ -5897,16 +5910,16 @@
         <v>506</v>
       </c>
       <c r="C246" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="F246" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+      <c r="F246" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>479</v>
       </c>
@@ -5914,13 +5927,13 @@
         <v>505</v>
       </c>
       <c r="C247" t="s">
-        <v>515</v>
-      </c>
-      <c r="E247" s="1" t="s">
-        <v>516</v>
+        <v>511</v>
+      </c>
+      <c r="E247" s="3" t="s">
+        <v>569</v>
       </c>
       <c r="F247" t="s">
-        <v>526</v>
+        <v>570</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
@@ -5928,16 +5941,16 @@
         <v>479</v>
       </c>
       <c r="B248" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C248" t="s">
-        <v>525</v>
+        <v>513</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>518</v>
+        <v>562</v>
       </c>
       <c r="F248" t="s">
-        <v>527</v>
+        <v>514</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
@@ -5948,13 +5961,13 @@
         <v>505</v>
       </c>
       <c r="C249" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F249" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
@@ -5965,13 +5978,13 @@
         <v>505</v>
       </c>
       <c r="C250" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>534</v>
+        <v>518</v>
       </c>
       <c r="F250" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
@@ -5979,15 +5992,49 @@
         <v>479</v>
       </c>
       <c r="B251" t="s">
+        <v>505</v>
+      </c>
+      <c r="C251" t="s">
+        <v>517</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="F251" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B252" t="s">
+        <v>505</v>
+      </c>
+      <c r="C252" t="s">
+        <v>529</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="F252" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B253" t="s">
         <v>506</v>
       </c>
-      <c r="C251" t="s">
+      <c r="C253" t="s">
         <v>531</v>
       </c>
-      <c r="E251" s="1" t="s">
+      <c r="E253" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="F251" t="s">
+      <c r="F253" t="s">
         <v>532</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added some permission snippets for #581
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="591">
   <si>
     <t>set</t>
   </si>
@@ -1817,9 +1817,30 @@
 page.Title = "${1:This page title works}";</t>
   </si>
   <si>
+    <t>Set a meta-tag - in this case the Meta Description</t>
+  </si>
+  <si>
     <t>// set MetaDescription - page variable must be declared before
-var metaDescription = (HtmlMeta)page.FindControl("metaDescription");
+var metaDescription = (HtmlMeta)page.FindControl("${2:metaDescription}");
 metaDescription.Content = "${1:This MetaDescription works}";</t>
+  </si>
+  <si>
+    <t>Set the page title of the dnn-page. Remember that this could happen multiple times, and the last one would always win.</t>
+  </si>
+  <si>
+    <t>User is in role</t>
+  </si>
+  <si>
+    <t>@Dnn.User.IsInRole("${1:Administrators}")</t>
+  </si>
+  <si>
+    <t>Check if the current user is in a specific role</t>
+  </si>
+  <si>
+    <t>User is super user / host</t>
+  </si>
+  <si>
+    <t>Check if the current user is the super-user aka host</t>
   </si>
 </sst>
 </file>
@@ -1882,8 +1903,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F253" totalsRowShown="0">
-  <autoFilter ref="A1:F253"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F255" totalsRowShown="0">
+  <autoFilter ref="A1:F255"/>
   <tableColumns count="6">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -2159,10 +2180,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F253"/>
+  <dimension ref="A1:F255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="E169" sqref="E169"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="F161" sqref="F161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4497,7 +4518,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>441</v>
       </c>
@@ -4513,33 +4534,36 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
       <c r="B161" t="s">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="C161" t="s">
-        <v>471</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>586</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="F161" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
       <c r="B162" t="s">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="C162" t="s">
-        <v>519</v>
+        <v>589</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>520</v>
+        <v>289</v>
       </c>
       <c r="F162" t="s">
-        <v>524</v>
+        <v>590</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -4550,13 +4574,13 @@
         <v>460</v>
       </c>
       <c r="C163" t="s">
-        <v>521</v>
-      </c>
-      <c r="E163" s="3" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>471</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>459</v>
       </c>
@@ -4564,13 +4588,16 @@
         <v>460</v>
       </c>
       <c r="C164" t="s">
-        <v>469</v>
+        <v>519</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+      <c r="F164" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>459</v>
       </c>
@@ -4578,18 +4605,24 @@
         <v>460</v>
       </c>
       <c r="C165" t="s">
-        <v>472</v>
+        <v>521</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>459</v>
       </c>
       <c r="B166" t="s">
         <v>460</v>
+      </c>
+      <c r="C166" t="s">
+        <v>469</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -4597,89 +4630,89 @@
         <v>459</v>
       </c>
       <c r="B167" t="s">
-        <v>579</v>
+        <v>460</v>
       </c>
       <c r="C167" t="s">
-        <v>580</v>
-      </c>
-      <c r="E167" s="2" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>472</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>459</v>
       </c>
       <c r="B168" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B169" t="s">
         <v>579</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C169" t="s">
+        <v>580</v>
+      </c>
+      <c r="E169" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="F169" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B170" t="s">
+        <v>579</v>
+      </c>
+      <c r="C170" t="s">
         <v>581</v>
       </c>
-      <c r="E168" s="2" t="s">
+      <c r="E170" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="F170" t="s">
         <v>583</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>355</v>
-      </c>
-      <c r="B169" t="s">
-        <v>359</v>
-      </c>
-      <c r="C169" t="s">
-        <v>360</v>
-      </c>
-      <c r="E169" t="s">
-        <v>319</v>
-      </c>
-      <c r="F169" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>355</v>
-      </c>
-      <c r="B170" t="s">
-        <v>359</v>
-      </c>
-      <c r="C170" t="s">
-        <v>361</v>
-      </c>
-      <c r="E170" t="s">
-        <v>536</v>
-      </c>
-      <c r="F170" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B171" t="s">
-        <v>58</v>
+        <v>359</v>
       </c>
       <c r="C171" t="s">
-        <v>455</v>
+        <v>360</v>
       </c>
       <c r="E171" t="s">
-        <v>320</v>
+        <v>319</v>
+      </c>
+      <c r="F171" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B172" t="s">
-        <v>58</v>
+        <v>359</v>
       </c>
       <c r="C172" t="s">
-        <v>456</v>
+        <v>361</v>
       </c>
       <c r="E172" t="s">
-        <v>537</v>
+        <v>536</v>
+      </c>
+      <c r="F172" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -4687,16 +4720,13 @@
         <v>356</v>
       </c>
       <c r="B173" t="s">
-        <v>321</v>
+        <v>58</v>
       </c>
       <c r="C173" t="s">
-        <v>321</v>
+        <v>455</v>
       </c>
       <c r="E173" t="s">
-        <v>535</v>
-      </c>
-      <c r="F173" t="s">
-        <v>538</v>
+        <v>320</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -4704,16 +4734,13 @@
         <v>356</v>
       </c>
       <c r="B174" t="s">
-        <v>358</v>
+        <v>58</v>
       </c>
       <c r="C174" t="s">
-        <v>322</v>
+        <v>456</v>
       </c>
       <c r="E174" t="s">
-        <v>323</v>
-      </c>
-      <c r="F174" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -4721,16 +4748,16 @@
         <v>356</v>
       </c>
       <c r="B175" t="s">
-        <v>358</v>
+        <v>321</v>
       </c>
       <c r="C175" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E175" t="s">
-        <v>325</v>
+        <v>535</v>
       </c>
       <c r="F175" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -4741,13 +4768,13 @@
         <v>358</v>
       </c>
       <c r="C176" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E176" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F176" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -4758,13 +4785,13 @@
         <v>358</v>
       </c>
       <c r="C177" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E177" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F177" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -4775,13 +4802,13 @@
         <v>358</v>
       </c>
       <c r="C178" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E178" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F178" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -4792,13 +4819,13 @@
         <v>358</v>
       </c>
       <c r="C179" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E179" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F179" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
@@ -4809,13 +4836,13 @@
         <v>358</v>
       </c>
       <c r="C180" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E180" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F180" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
@@ -4826,10 +4853,13 @@
         <v>358</v>
       </c>
       <c r="C181" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E181" t="s">
-        <v>337</v>
+        <v>333</v>
+      </c>
+      <c r="F181" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
@@ -4840,44 +4870,41 @@
         <v>358</v>
       </c>
       <c r="C182" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E182" t="s">
-        <v>339</v>
+        <v>335</v>
+      </c>
+      <c r="F182" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>478</v>
+        <v>356</v>
       </c>
       <c r="B183" t="s">
-        <v>1</v>
+        <v>358</v>
       </c>
       <c r="C183" t="s">
-        <v>2</v>
+        <v>336</v>
       </c>
       <c r="E183" t="s">
-        <v>340</v>
-      </c>
-      <c r="F183" t="s">
-        <v>28</v>
+        <v>337</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>478</v>
+        <v>356</v>
       </c>
       <c r="B184" t="s">
-        <v>1</v>
+        <v>358</v>
       </c>
       <c r="C184" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="E184" t="s">
-        <v>341</v>
-      </c>
-      <c r="F184" t="s">
-        <v>27</v>
+        <v>339</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
@@ -4888,13 +4915,13 @@
         <v>1</v>
       </c>
       <c r="C185" t="s">
-        <v>215</v>
+        <v>2</v>
       </c>
       <c r="E185" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F185" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
@@ -4905,13 +4932,13 @@
         <v>1</v>
       </c>
       <c r="C186" t="s">
-        <v>22</v>
+        <v>362</v>
       </c>
       <c r="E186" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F186" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
@@ -4922,13 +4949,13 @@
         <v>1</v>
       </c>
       <c r="C187" t="s">
-        <v>363</v>
+        <v>215</v>
       </c>
       <c r="E187" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F187" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
@@ -4939,47 +4966,47 @@
         <v>1</v>
       </c>
       <c r="C188" t="s">
-        <v>364</v>
+        <v>22</v>
       </c>
       <c r="E188" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F188" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>357</v>
+        <v>478</v>
       </c>
       <c r="B189" t="s">
-        <v>303</v>
+        <v>1</v>
       </c>
       <c r="C189" t="s">
-        <v>112</v>
+        <v>363</v>
       </c>
       <c r="E189" t="s">
-        <v>387</v>
+        <v>344</v>
       </c>
       <c r="F189" t="s">
-        <v>388</v>
+        <v>14</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>357</v>
+        <v>478</v>
       </c>
       <c r="B190" t="s">
-        <v>303</v>
+        <v>1</v>
       </c>
       <c r="C190" t="s">
-        <v>54</v>
+        <v>364</v>
       </c>
       <c r="E190" t="s">
-        <v>389</v>
+        <v>345</v>
       </c>
       <c r="F190" t="s">
-        <v>390</v>
+        <v>18</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
@@ -4990,13 +5017,13 @@
         <v>303</v>
       </c>
       <c r="C191" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="E191" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="F191" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
@@ -5007,13 +5034,13 @@
         <v>303</v>
       </c>
       <c r="C192" t="s">
-        <v>426</v>
+        <v>54</v>
       </c>
       <c r="E192" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F192" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -5024,13 +5051,13 @@
         <v>303</v>
       </c>
       <c r="C193" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E193" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F193" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
@@ -5041,13 +5068,13 @@
         <v>303</v>
       </c>
       <c r="C194" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E194" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="F194" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
@@ -5058,13 +5085,13 @@
         <v>303</v>
       </c>
       <c r="C195" t="s">
-        <v>427</v>
+        <v>58</v>
       </c>
       <c r="E195" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="F195" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
@@ -5075,13 +5102,13 @@
         <v>303</v>
       </c>
       <c r="C196" t="s">
-        <v>174</v>
+        <v>428</v>
       </c>
       <c r="E196" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="F196" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
@@ -5092,13 +5119,13 @@
         <v>303</v>
       </c>
       <c r="C197" t="s">
-        <v>84</v>
+        <v>427</v>
       </c>
       <c r="E197" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="F197" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
@@ -5109,13 +5136,13 @@
         <v>303</v>
       </c>
       <c r="C198" t="s">
-        <v>90</v>
+        <v>174</v>
       </c>
       <c r="E198" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="F198" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
@@ -5123,16 +5150,16 @@
         <v>357</v>
       </c>
       <c r="B199" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C199" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="E199" t="s">
-        <v>365</v>
+        <v>403</v>
       </c>
       <c r="F199" t="s">
-        <v>366</v>
+        <v>404</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
@@ -5140,16 +5167,16 @@
         <v>357</v>
       </c>
       <c r="B200" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C200" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="E200" t="s">
-        <v>367</v>
+        <v>405</v>
       </c>
       <c r="F200" t="s">
-        <v>368</v>
+        <v>406</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
@@ -5160,13 +5187,13 @@
         <v>304</v>
       </c>
       <c r="C201" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E201" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="F201" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
@@ -5177,13 +5204,13 @@
         <v>304</v>
       </c>
       <c r="C202" t="s">
-        <v>427</v>
+        <v>54</v>
       </c>
       <c r="E202" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F202" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
@@ -5194,13 +5221,13 @@
         <v>304</v>
       </c>
       <c r="C203" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="E203" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F203" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
@@ -5211,13 +5238,13 @@
         <v>304</v>
       </c>
       <c r="C204" t="s">
-        <v>141</v>
+        <v>427</v>
       </c>
       <c r="E204" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="F204" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
@@ -5228,13 +5255,13 @@
         <v>304</v>
       </c>
       <c r="C205" t="s">
-        <v>90</v>
+        <v>131</v>
       </c>
       <c r="E205" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="F205" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
@@ -5245,13 +5272,13 @@
         <v>304</v>
       </c>
       <c r="C206" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="E206" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="F206" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
@@ -5262,13 +5289,13 @@
         <v>304</v>
       </c>
       <c r="C207" t="s">
-        <v>166</v>
+        <v>90</v>
       </c>
       <c r="E207" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="F207" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
@@ -5279,13 +5306,13 @@
         <v>304</v>
       </c>
       <c r="C208" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E208" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="F208" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
@@ -5296,13 +5323,13 @@
         <v>304</v>
       </c>
       <c r="C209" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="E209" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F209" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
@@ -5310,16 +5337,16 @@
         <v>357</v>
       </c>
       <c r="B210" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C210" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="E210" t="s">
-        <v>346</v>
+        <v>383</v>
       </c>
       <c r="F210" t="s">
-        <v>439</v>
+        <v>384</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
@@ -5327,16 +5354,16 @@
         <v>357</v>
       </c>
       <c r="B211" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C211" t="s">
-        <v>112</v>
+        <v>177</v>
       </c>
       <c r="E211" t="s">
-        <v>347</v>
+        <v>385</v>
       </c>
       <c r="F211" t="s">
-        <v>438</v>
+        <v>386</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
@@ -5347,13 +5374,13 @@
         <v>305</v>
       </c>
       <c r="C212" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="E212" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F212" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
@@ -5364,13 +5391,13 @@
         <v>305</v>
       </c>
       <c r="C213" t="s">
-        <v>213</v>
+        <v>112</v>
       </c>
       <c r="E213" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F213" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
@@ -5381,13 +5408,13 @@
         <v>305</v>
       </c>
       <c r="C214" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="E214" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F214" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
@@ -5398,13 +5425,13 @@
         <v>305</v>
       </c>
       <c r="C215" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="E215" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F215" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
@@ -5415,13 +5442,13 @@
         <v>305</v>
       </c>
       <c r="C216" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="E216" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F216" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
@@ -5432,13 +5459,13 @@
         <v>305</v>
       </c>
       <c r="C217" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E217" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F217" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
@@ -5449,47 +5476,47 @@
         <v>305</v>
       </c>
       <c r="C218" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="E218" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F218" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B219" t="s">
-        <v>425</v>
+        <v>305</v>
       </c>
       <c r="C219" t="s">
-        <v>278</v>
+        <v>230</v>
       </c>
       <c r="E219" t="s">
-        <v>409</v>
+        <v>353</v>
       </c>
       <c r="F219" t="s">
-        <v>410</v>
+        <v>432</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>423</v>
+        <v>357</v>
       </c>
       <c r="B220" t="s">
-        <v>425</v>
+        <v>305</v>
       </c>
       <c r="C220" t="s">
-        <v>205</v>
+        <v>262</v>
       </c>
       <c r="E220" t="s">
-        <v>411</v>
+        <v>354</v>
       </c>
       <c r="F220" t="s">
-        <v>412</v>
+        <v>431</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
@@ -5500,13 +5527,13 @@
         <v>425</v>
       </c>
       <c r="C221" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E221" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="F221" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
@@ -5517,13 +5544,13 @@
         <v>425</v>
       </c>
       <c r="C222" t="s">
-        <v>283</v>
+        <v>205</v>
       </c>
       <c r="E222" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F222" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
@@ -5534,13 +5561,13 @@
         <v>425</v>
       </c>
       <c r="C223" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="E223" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F223" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
@@ -5551,13 +5578,13 @@
         <v>425</v>
       </c>
       <c r="C224" t="s">
-        <v>430</v>
+        <v>283</v>
       </c>
       <c r="E224" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F224" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
@@ -5565,50 +5592,50 @@
         <v>423</v>
       </c>
       <c r="B225" t="s">
-        <v>306</v>
+        <v>425</v>
       </c>
       <c r="C225" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="E225" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F225" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B226" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C226" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E226" t="s">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="F226" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B227" t="s">
-        <v>442</v>
+        <v>306</v>
       </c>
       <c r="C227" t="s">
-        <v>443</v>
+        <v>306</v>
       </c>
       <c r="E227" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
       <c r="F227" t="s">
-        <v>445</v>
+        <v>422</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5616,16 +5643,16 @@
         <v>424</v>
       </c>
       <c r="B228" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="C228" t="s">
-        <v>448</v>
+        <v>429</v>
       </c>
       <c r="E228" t="s">
-        <v>446</v>
+        <v>407</v>
       </c>
       <c r="F228" t="s">
-        <v>447</v>
+        <v>408</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -5636,13 +5663,13 @@
         <v>442</v>
       </c>
       <c r="C229" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="E229" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="F229" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -5653,140 +5680,140 @@
         <v>442</v>
       </c>
       <c r="C230" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="E230" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="F230" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
+        <v>424</v>
+      </c>
+      <c r="B231" t="s">
+        <v>442</v>
+      </c>
+      <c r="C231" t="s">
+        <v>449</v>
+      </c>
+      <c r="E231" t="s">
+        <v>450</v>
+      </c>
+      <c r="F231" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>424</v>
+      </c>
+      <c r="B232" t="s">
+        <v>442</v>
+      </c>
+      <c r="C232" t="s">
+        <v>452</v>
+      </c>
+      <c r="E232" t="s">
+        <v>453</v>
+      </c>
+      <c r="F232" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
         <v>464</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B233" t="s">
         <v>462</v>
       </c>
-      <c r="C231" t="s">
+      <c r="C233" t="s">
         <v>463</v>
       </c>
-      <c r="E231" t="s">
+      <c r="E233" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A232" s="1" t="s">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B234" t="s">
         <v>462</v>
       </c>
-      <c r="C232" t="s">
+      <c r="C234" t="s">
         <v>468</v>
       </c>
-      <c r="E232" t="s">
+      <c r="E234" t="s">
         <v>564</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A233" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="B233" t="s">
-        <v>481</v>
-      </c>
-      <c r="C233" t="s">
-        <v>482</v>
-      </c>
-      <c r="E233" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="F233" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
-        <v>484</v>
-      </c>
-      <c r="B234" t="s">
-        <v>481</v>
-      </c>
-      <c r="C234" t="s">
-        <v>483</v>
-      </c>
-      <c r="E234" t="s">
-        <v>496</v>
-      </c>
-      <c r="F234" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B235" t="s">
+        <v>481</v>
+      </c>
+      <c r="C235" t="s">
+        <v>482</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="F235" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>484</v>
+      </c>
+      <c r="B236" t="s">
+        <v>481</v>
+      </c>
+      <c r="C236" t="s">
+        <v>483</v>
+      </c>
+      <c r="E236" t="s">
+        <v>496</v>
+      </c>
+      <c r="F236" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B235" t="s">
+      <c r="B237" t="s">
         <v>462</v>
       </c>
-      <c r="C235" t="s">
+      <c r="C237" t="s">
         <v>463</v>
       </c>
-      <c r="E235" t="s">
+      <c r="E237" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A236" s="1" t="s">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B236" t="s">
+      <c r="B238" t="s">
         <v>462</v>
       </c>
-      <c r="C236" t="s">
+      <c r="C238" t="s">
         <v>468</v>
       </c>
-      <c r="E236" t="s">
+      <c r="E238" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="237" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A237" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B237" t="s">
-        <v>480</v>
-      </c>
-      <c r="C237" t="s">
-        <v>488</v>
-      </c>
-      <c r="E237" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="F237" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A238" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B238" t="s">
-        <v>480</v>
-      </c>
-      <c r="C238" t="s">
-        <v>489</v>
-      </c>
-      <c r="E238" s="3" t="s">
-        <v>498</v>
-      </c>
-      <c r="F238" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="239" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>479</v>
       </c>
@@ -5794,44 +5821,44 @@
         <v>480</v>
       </c>
       <c r="C239" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E239" s="3" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+        <v>497</v>
+      </c>
+      <c r="F239" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B240" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C240" t="s">
-        <v>482</v>
-      </c>
-      <c r="E240" s="1" t="s">
-        <v>493</v>
+        <v>489</v>
+      </c>
+      <c r="E240" s="3" t="s">
+        <v>498</v>
       </c>
       <c r="F240" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B241" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C241" t="s">
-        <v>483</v>
-      </c>
-      <c r="E241" t="s">
-        <v>494</v>
-      </c>
-      <c r="F241" t="s">
-        <v>486</v>
+        <v>491</v>
+      </c>
+      <c r="E241" s="3" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
@@ -5839,16 +5866,16 @@
         <v>479</v>
       </c>
       <c r="B242" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
       <c r="C242" t="s">
-        <v>500</v>
+        <v>482</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="F242" t="s">
-        <v>502</v>
+        <v>485</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
@@ -5856,16 +5883,16 @@
         <v>479</v>
       </c>
       <c r="B243" t="s">
-        <v>578</v>
+        <v>481</v>
       </c>
       <c r="C243" t="s">
-        <v>575</v>
-      </c>
-      <c r="E243" s="1" t="s">
-        <v>577</v>
+        <v>483</v>
+      </c>
+      <c r="E243" t="s">
+        <v>494</v>
       </c>
       <c r="F243" t="s">
-        <v>576</v>
+        <v>486</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
@@ -5873,70 +5900,70 @@
         <v>479</v>
       </c>
       <c r="B244" t="s">
-        <v>571</v>
+        <v>499</v>
       </c>
       <c r="C244" t="s">
-        <v>572</v>
-      </c>
-      <c r="E244" s="3" t="s">
-        <v>573</v>
+        <v>500</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>501</v>
       </c>
       <c r="F244" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="245" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B245" t="s">
-        <v>506</v>
+        <v>578</v>
       </c>
       <c r="C245" t="s">
-        <v>508</v>
-      </c>
-      <c r="E245" s="2" t="s">
-        <v>563</v>
+        <v>575</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>577</v>
       </c>
       <c r="F245" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B246" t="s">
-        <v>506</v>
+        <v>571</v>
       </c>
       <c r="C246" t="s">
-        <v>509</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="F246" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>572</v>
+      </c>
+      <c r="E246" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="F246" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>479</v>
       </c>
       <c r="B247" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C247" t="s">
-        <v>511</v>
-      </c>
-      <c r="E247" s="3" t="s">
-        <v>569</v>
+        <v>508</v>
+      </c>
+      <c r="E247" s="2" t="s">
+        <v>563</v>
       </c>
       <c r="F247" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>479</v>
       </c>
@@ -5944,16 +5971,16 @@
         <v>506</v>
       </c>
       <c r="C248" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="F248" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+      <c r="F248" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>479</v>
       </c>
@@ -5961,13 +5988,13 @@
         <v>505</v>
       </c>
       <c r="C249" t="s">
-        <v>515</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>516</v>
+        <v>511</v>
+      </c>
+      <c r="E249" s="3" t="s">
+        <v>569</v>
       </c>
       <c r="F249" t="s">
-        <v>526</v>
+        <v>570</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
@@ -5975,16 +6002,16 @@
         <v>479</v>
       </c>
       <c r="B250" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C250" t="s">
-        <v>525</v>
+        <v>513</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>518</v>
+        <v>562</v>
       </c>
       <c r="F250" t="s">
-        <v>527</v>
+        <v>514</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.25">
@@ -5995,13 +6022,13 @@
         <v>505</v>
       </c>
       <c r="C251" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F251" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.25">
@@ -6012,13 +6039,13 @@
         <v>505</v>
       </c>
       <c r="C252" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>534</v>
+        <v>518</v>
       </c>
       <c r="F252" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
@@ -6026,23 +6053,58 @@
         <v>479</v>
       </c>
       <c r="B253" t="s">
+        <v>505</v>
+      </c>
+      <c r="C253" t="s">
+        <v>517</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="F253" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B254" t="s">
+        <v>505</v>
+      </c>
+      <c r="C254" t="s">
+        <v>529</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="F254" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B255" t="s">
         <v>506</v>
       </c>
-      <c r="C253" t="s">
+      <c r="C255" t="s">
         <v>531</v>
       </c>
-      <c r="E253" s="1" t="s">
+      <c r="E255" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="F253" t="s">
+      <c r="F255" t="s">
         <v>532</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Start work on snippet-api linking...
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="597">
   <si>
     <t>set</t>
   </si>
@@ -1855,6 +1855,15 @@
   </si>
   <si>
     <t>Check if the user is logged in.</t>
+  </si>
+  <si>
+    <t>links</t>
+  </si>
+  <si>
+    <t>Show an inline-toolbar. If you wat it hovering, make sure you have an HTML-element around it with the class sc-element.</t>
+  </si>
+  <si>
+    <t>api: https://github.com/2sic/2sxc/wiki/Razor-Edit</t>
   </si>
 </sst>
 </file>
@@ -1917,15 +1926,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F256" totalsRowShown="0">
-  <autoFilter ref="A1:F256"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G256" totalsRowShown="0">
+  <autoFilter ref="A1:G256">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="@Content"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="7">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
     <tableColumn id="2" name="name"/>
     <tableColumn id="3" name="title"/>
     <tableColumn id="5" name="content"/>
     <tableColumn id="6" name="help"/>
+    <tableColumn id="4" name="links"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2194,10 +2210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F256"/>
+  <dimension ref="A1:G256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="E164" sqref="E164"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2210,7 +2226,7 @@
     <col min="6" max="6" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2229,8 +2245,11 @@
       <c r="F1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>477</v>
       </c>
@@ -2250,7 +2269,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>477</v>
       </c>
@@ -2270,7 +2289,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>477</v>
       </c>
@@ -2290,7 +2309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>477</v>
       </c>
@@ -2310,7 +2329,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>477</v>
       </c>
@@ -2330,7 +2349,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>477</v>
       </c>
@@ -2350,7 +2369,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>457</v>
       </c>
@@ -2364,10 +2383,13 @@
         <v>548</v>
       </c>
       <c r="F8" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+      <c r="G8" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>457</v>
       </c>
@@ -2384,7 +2406,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>457</v>
       </c>
@@ -2401,7 +2423,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>457</v>
       </c>
@@ -2418,7 +2440,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>457</v>
       </c>
@@ -2435,7 +2457,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>458</v>
       </c>
@@ -2455,7 +2477,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>458</v>
       </c>
@@ -2469,7 +2491,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>458</v>
       </c>
@@ -2489,7 +2511,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>317</v>
       </c>
@@ -2503,7 +2525,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>317</v>
       </c>
@@ -2517,7 +2539,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>317</v>
       </c>
@@ -2531,7 +2553,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>317</v>
       </c>
@@ -2545,7 +2567,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>317</v>
       </c>
@@ -2559,7 +2581,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>317</v>
       </c>
@@ -2573,7 +2595,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>317</v>
       </c>
@@ -2587,7 +2609,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>317</v>
       </c>
@@ -2601,7 +2623,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>317</v>
       </c>
@@ -2615,7 +2637,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>317</v>
       </c>
@@ -2629,7 +2651,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>317</v>
       </c>
@@ -2643,7 +2665,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>317</v>
       </c>
@@ -2657,7 +2679,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>317</v>
       </c>
@@ -2671,7 +2693,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>317</v>
       </c>
@@ -2685,7 +2707,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>317</v>
       </c>
@@ -2699,7 +2721,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>317</v>
       </c>
@@ -2713,7 +2735,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>317</v>
       </c>
@@ -2727,7 +2749,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>317</v>
       </c>
@@ -2741,7 +2763,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>317</v>
       </c>
@@ -2755,7 +2777,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>317</v>
       </c>
@@ -2769,7 +2791,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>317</v>
       </c>
@@ -2783,7 +2805,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>317</v>
       </c>
@@ -2797,7 +2819,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>317</v>
       </c>
@@ -2811,7 +2833,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>317</v>
       </c>
@@ -2825,7 +2847,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>317</v>
       </c>
@@ -2839,7 +2861,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>317</v>
       </c>
@@ -2853,7 +2875,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>317</v>
       </c>
@@ -2867,7 +2889,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>317</v>
       </c>
@@ -2881,7 +2903,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>317</v>
       </c>
@@ -2895,7 +2917,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>317</v>
       </c>
@@ -2909,7 +2931,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>317</v>
       </c>
@@ -2923,7 +2945,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>317</v>
       </c>
@@ -2937,7 +2959,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>317</v>
       </c>
@@ -2951,7 +2973,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>317</v>
       </c>
@@ -2965,7 +2987,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>317</v>
       </c>
@@ -2979,7 +3001,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>317</v>
       </c>
@@ -2993,7 +3015,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>317</v>
       </c>
@@ -3007,7 +3029,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>317</v>
       </c>
@@ -3021,7 +3043,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>317</v>
       </c>
@@ -3035,7 +3057,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>317</v>
       </c>
@@ -3049,7 +3071,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>317</v>
       </c>
@@ -3063,7 +3085,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>317</v>
       </c>
@@ -3077,7 +3099,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>317</v>
       </c>
@@ -3091,7 +3113,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>317</v>
       </c>
@@ -3108,7 +3130,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>317</v>
       </c>
@@ -3122,7 +3144,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>317</v>
       </c>
@@ -3136,7 +3158,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>317</v>
       </c>
@@ -3150,7 +3172,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>317</v>
       </c>
@@ -3164,7 +3186,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>317</v>
       </c>
@@ -3178,7 +3200,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>317</v>
       </c>
@@ -3192,7 +3214,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>317</v>
       </c>
@@ -3206,7 +3228,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>317</v>
       </c>
@@ -3220,7 +3242,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>317</v>
       </c>
@@ -3234,7 +3256,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>317</v>
       </c>
@@ -3248,7 +3270,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>317</v>
       </c>
@@ -3262,7 +3284,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>317</v>
       </c>
@@ -3276,7 +3298,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>317</v>
       </c>
@@ -3290,7 +3312,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>317</v>
       </c>
@@ -3304,7 +3326,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>317</v>
       </c>
@@ -3318,7 +3340,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>317</v>
       </c>
@@ -3332,7 +3354,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>317</v>
       </c>
@@ -3346,7 +3368,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>317</v>
       </c>
@@ -3360,7 +3382,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>317</v>
       </c>
@@ -3374,7 +3396,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>317</v>
       </c>
@@ -3388,7 +3410,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>317</v>
       </c>
@@ -3402,7 +3424,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>317</v>
       </c>
@@ -3416,7 +3438,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>317</v>
       </c>
@@ -3430,7 +3452,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>317</v>
       </c>
@@ -3444,7 +3466,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>317</v>
       </c>
@@ -3458,7 +3480,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>317</v>
       </c>
@@ -3472,7 +3494,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>317</v>
       </c>
@@ -3486,7 +3508,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>317</v>
       </c>
@@ -3500,7 +3522,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>317</v>
       </c>
@@ -3514,7 +3536,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>317</v>
       </c>
@@ -3528,7 +3550,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>317</v>
       </c>
@@ -3542,7 +3564,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>317</v>
       </c>
@@ -3556,7 +3578,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>317</v>
       </c>
@@ -3570,7 +3592,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>317</v>
       </c>
@@ -3584,7 +3606,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>317</v>
       </c>
@@ -3598,7 +3620,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>317</v>
       </c>
@@ -3612,7 +3634,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>317</v>
       </c>
@@ -3626,7 +3648,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>317</v>
       </c>
@@ -3640,7 +3662,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>317</v>
       </c>
@@ -3654,7 +3676,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>317</v>
       </c>
@@ -3668,7 +3690,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>317</v>
       </c>
@@ -3682,7 +3704,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>317</v>
       </c>
@@ -3699,7 +3721,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>317</v>
       </c>
@@ -3716,7 +3738,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>317</v>
       </c>
@@ -3730,7 +3752,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>317</v>
       </c>
@@ -3744,7 +3766,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>317</v>
       </c>
@@ -3758,7 +3780,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>317</v>
       </c>
@@ -3772,7 +3794,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>317</v>
       </c>
@@ -3786,7 +3808,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>317</v>
       </c>
@@ -3800,7 +3822,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>317</v>
       </c>
@@ -3814,7 +3836,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>317</v>
       </c>
@@ -3828,7 +3850,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>317</v>
       </c>
@@ -3842,7 +3864,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>317</v>
       </c>
@@ -3856,7 +3878,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>317</v>
       </c>
@@ -3870,7 +3892,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>317</v>
       </c>
@@ -3884,7 +3906,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>317</v>
       </c>
@@ -3898,7 +3920,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>317</v>
       </c>
@@ -3915,7 +3937,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>317</v>
       </c>
@@ -3929,7 +3951,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>317</v>
       </c>
@@ -3946,7 +3968,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>317</v>
       </c>
@@ -3960,7 +3982,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>317</v>
       </c>
@@ -3974,7 +3996,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>317</v>
       </c>
@@ -3988,7 +4010,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>317</v>
       </c>
@@ -4002,7 +4024,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>317</v>
       </c>
@@ -4016,7 +4038,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>317</v>
       </c>
@@ -4030,7 +4052,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>317</v>
       </c>
@@ -4044,7 +4066,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>317</v>
       </c>
@@ -4058,7 +4080,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>317</v>
       </c>
@@ -4072,7 +4094,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>317</v>
       </c>
@@ -4089,7 +4111,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>317</v>
       </c>
@@ -4103,7 +4125,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>317</v>
       </c>
@@ -4117,7 +4139,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>317</v>
       </c>
@@ -4131,7 +4153,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>317</v>
       </c>
@@ -4145,7 +4167,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>317</v>
       </c>
@@ -4159,7 +4181,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>317</v>
       </c>
@@ -4173,7 +4195,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>317</v>
       </c>
@@ -4187,7 +4209,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>317</v>
       </c>
@@ -4201,7 +4223,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>317</v>
       </c>
@@ -4215,7 +4237,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>317</v>
       </c>
@@ -4229,7 +4251,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>317</v>
       </c>
@@ -4243,7 +4265,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>317</v>
       </c>
@@ -4257,7 +4279,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>317</v>
       </c>
@@ -4271,7 +4293,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>317</v>
       </c>
@@ -4285,7 +4307,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>317</v>
       </c>
@@ -4299,7 +4321,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>317</v>
       </c>
@@ -4313,7 +4335,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>441</v>
       </c>
@@ -4327,7 +4349,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>441</v>
       </c>
@@ -4341,7 +4363,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>441</v>
       </c>
@@ -4355,7 +4377,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>441</v>
       </c>
@@ -4369,7 +4391,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>441</v>
       </c>
@@ -4383,7 +4405,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>441</v>
       </c>
@@ -4397,7 +4419,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>441</v>
       </c>
@@ -4411,7 +4433,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>441</v>
       </c>
@@ -4425,7 +4447,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>441</v>
       </c>
@@ -4442,7 +4464,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>441</v>
       </c>
@@ -4456,7 +4478,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>441</v>
       </c>
@@ -4473,7 +4495,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>441</v>
       </c>
@@ -4487,7 +4509,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>441</v>
       </c>
@@ -4501,7 +4523,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>441</v>
       </c>
@@ -4518,7 +4540,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>441</v>
       </c>
@@ -4532,7 +4554,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>441</v>
       </c>
@@ -4546,7 +4568,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>441</v>
       </c>
@@ -4563,7 +4585,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>441</v>
       </c>
@@ -4580,7 +4602,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>441</v>
       </c>
@@ -4597,7 +4619,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>459</v>
       </c>
@@ -4611,7 +4633,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>459</v>
       </c>
@@ -4628,7 +4650,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>459</v>
       </c>
@@ -4642,7 +4664,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>459</v>
       </c>
@@ -4656,7 +4678,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>459</v>
       </c>
@@ -4670,7 +4692,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>459</v>
       </c>
@@ -4678,7 +4700,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>459</v>
       </c>
@@ -4695,7 +4717,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>459</v>
       </c>
@@ -4712,7 +4734,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>355</v>
       </c>
@@ -4729,7 +4751,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>355</v>
       </c>
@@ -4746,7 +4768,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>356</v>
       </c>
@@ -4760,7 +4782,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>356</v>
       </c>
@@ -4774,7 +4796,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>356</v>
       </c>
@@ -4791,7 +4813,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>356</v>
       </c>
@@ -4808,7 +4830,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>356</v>
       </c>
@@ -4825,7 +4847,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>356</v>
       </c>
@@ -4842,7 +4864,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>356</v>
       </c>
@@ -4859,7 +4881,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>356</v>
       </c>
@@ -4876,7 +4898,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>356</v>
       </c>
@@ -4893,7 +4915,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>356</v>
       </c>
@@ -4910,7 +4932,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>356</v>
       </c>
@@ -4924,7 +4946,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>356</v>
       </c>
@@ -4938,7 +4960,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>478</v>
       </c>
@@ -4955,7 +4977,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>478</v>
       </c>
@@ -4972,7 +4994,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>478</v>
       </c>
@@ -4989,7 +5011,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>478</v>
       </c>
@@ -5006,7 +5028,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>478</v>
       </c>
@@ -5023,7 +5045,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>478</v>
       </c>
@@ -5040,7 +5062,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>357</v>
       </c>
@@ -5057,7 +5079,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>357</v>
       </c>
@@ -5074,7 +5096,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>357</v>
       </c>
@@ -5091,7 +5113,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>357</v>
       </c>
@@ -5108,7 +5130,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>357</v>
       </c>
@@ -5125,7 +5147,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>357</v>
       </c>
@@ -5142,7 +5164,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>357</v>
       </c>
@@ -5159,7 +5181,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>357</v>
       </c>
@@ -5176,7 +5198,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>357</v>
       </c>
@@ -5193,7 +5215,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>357</v>
       </c>
@@ -5210,7 +5232,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>357</v>
       </c>
@@ -5227,7 +5249,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>357</v>
       </c>
@@ -5244,7 +5266,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>357</v>
       </c>
@@ -5261,7 +5283,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>357</v>
       </c>
@@ -5278,7 +5300,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>357</v>
       </c>
@@ -5295,7 +5317,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>357</v>
       </c>
@@ -5312,7 +5334,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>357</v>
       </c>
@@ -5329,7 +5351,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>357</v>
       </c>
@@ -5346,7 +5368,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>357</v>
       </c>
@@ -5363,7 +5385,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>357</v>
       </c>
@@ -5380,7 +5402,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>357</v>
       </c>
@@ -5397,7 +5419,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>357</v>
       </c>
@@ -5414,7 +5436,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>357</v>
       </c>
@@ -5431,7 +5453,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>357</v>
       </c>
@@ -5448,7 +5470,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>357</v>
       </c>
@@ -5465,7 +5487,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>357</v>
       </c>
@@ -5482,7 +5504,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>357</v>
       </c>
@@ -5499,7 +5521,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>357</v>
       </c>
@@ -5516,7 +5538,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>357</v>
       </c>
@@ -5533,7 +5555,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>357</v>
       </c>
@@ -5550,7 +5572,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>423</v>
       </c>
@@ -5567,7 +5589,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>423</v>
       </c>
@@ -5584,7 +5606,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>423</v>
       </c>
@@ -5601,7 +5623,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>423</v>
       </c>
@@ -5618,7 +5640,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>423</v>
       </c>
@@ -5635,7 +5657,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>423</v>
       </c>
@@ -5652,7 +5674,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>423</v>
       </c>
@@ -5669,7 +5691,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>424</v>
       </c>
@@ -5686,7 +5708,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>424</v>
       </c>
@@ -5703,7 +5725,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>424</v>
       </c>
@@ -5720,7 +5742,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>424</v>
       </c>
@@ -5737,7 +5759,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>424</v>
       </c>
@@ -5754,7 +5776,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>464</v>
       </c>
@@ -5768,7 +5790,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>464</v>
       </c>
@@ -5782,7 +5804,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>484</v>
       </c>
@@ -5799,7 +5821,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>484</v>
       </c>
@@ -5816,7 +5838,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>466</v>
       </c>
@@ -5830,7 +5852,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>466</v>
       </c>
@@ -5844,7 +5866,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="240" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>479</v>
       </c>
@@ -5861,7 +5883,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="241" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>479</v>
       </c>
@@ -5878,7 +5900,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="242" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>479</v>
       </c>
@@ -5892,7 +5914,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>479</v>
       </c>
@@ -5909,7 +5931,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>479</v>
       </c>
@@ -5926,7 +5948,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>479</v>
       </c>
@@ -5943,7 +5965,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>479</v>
       </c>
@@ -5960,7 +5982,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>479</v>
       </c>
@@ -5977,7 +5999,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="248" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>479</v>
       </c>
@@ -5994,7 +6016,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="249" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>479</v>
       </c>
@@ -6011,7 +6033,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="250" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>479</v>
       </c>
@@ -6028,7 +6050,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>479</v>
       </c>
@@ -6045,7 +6067,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>479</v>
       </c>
@@ -6062,7 +6084,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>479</v>
       </c>
@@ -6079,7 +6101,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>479</v>
       </c>
@@ -6096,7 +6118,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>479</v>
       </c>
@@ -6113,7 +6135,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>479</v>
       </c>

</xml_diff>

<commit_message>
enhanced dev with help-api-links
</commit_message>
<xml_diff>
--- a/src/sxc-develop/source-editor/snippets.xlsx
+++ b/src/sxc-develop/source-editor/snippets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11475"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11473"/>
   </bookViews>
   <sheets>
     <sheet name="snippets" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="600">
   <si>
     <t>set</t>
   </si>
@@ -1860,10 +1860,19 @@
     <t>links</t>
   </si>
   <si>
-    <t>Show an inline-toolbar. If you wat it hovering, make sure you have an HTML-element around it with the class sc-element.</t>
-  </si>
-  <si>
-    <t>api: https://github.com/2sic/2sxc/wiki/Razor-Edit</t>
+    <t>Show an inline-toolbar. If you want it hovering, make sure you have an HTML-element around it with the class sc-element.</t>
+  </si>
+  <si>
+    <t>read api-docs:https://github.com/2sic/2sxc/wiki/Razor-Edit</t>
+  </si>
+  <si>
+    <t>read api-docs:https://github.com/2sic/2sxc/wiki/Razor-Dnn</t>
+  </si>
+  <si>
+    <t>read API docs: https://github.com/2sic/2sxc/wiki/Razor-App</t>
+  </si>
+  <si>
+    <t>read API docs: https://github.com/2sic/2sxc/wiki/Razor-Data</t>
   </si>
 </sst>
 </file>
@@ -1930,8 +1939,15 @@
   <autoFilter ref="A1:G256">
     <filterColumn colId="0">
       <filters>
-        <filter val="@Content"/>
+        <filter val="@\InputType"/>
+        <filter val="@C#"/>
+        <filter val="@Html"/>
+        <filter val="@List"/>
+        <filter val="@User"/>
       </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <tableColumns count="7">
@@ -2212,21 +2228,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G256"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="B159" sqref="B159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.46875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.64453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.85546875" customWidth="1"/>
-    <col min="6" max="6" width="50.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.52734375" customWidth="1"/>
+    <col min="5" max="5" width="54.41015625" customWidth="1"/>
+    <col min="6" max="6" width="40.52734375" customWidth="1"/>
+    <col min="7" max="7" width="44.234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2249,7 +2266,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>477</v>
       </c>
@@ -2268,8 +2285,11 @@
       <c r="F2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>477</v>
       </c>
@@ -2288,8 +2308,11 @@
       <c r="F3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>477</v>
       </c>
@@ -2308,8 +2331,11 @@
       <c r="F4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>477</v>
       </c>
@@ -2328,8 +2354,11 @@
       <c r="F5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>477</v>
       </c>
@@ -2348,8 +2377,11 @@
       <c r="F6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>477</v>
       </c>
@@ -2368,8 +2400,11 @@
       <c r="F7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>457</v>
       </c>
@@ -2389,7 +2424,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="43" hidden="1" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>457</v>
       </c>
@@ -2405,8 +2440,11 @@
       <c r="F9" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>457</v>
       </c>
@@ -2422,8 +2460,11 @@
       <c r="F10" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>457</v>
       </c>
@@ -2439,8 +2480,11 @@
       <c r="F11" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>457</v>
       </c>
@@ -2456,8 +2500,11 @@
       <c r="F12" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>458</v>
       </c>
@@ -2477,7 +2524,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="43" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>458</v>
       </c>
@@ -2491,7 +2538,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="86" hidden="1" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>458</v>
       </c>
@@ -2510,8 +2557,11 @@
       <c r="F15" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>317</v>
       </c>
@@ -2524,8 +2574,11 @@
       <c r="E16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>317</v>
       </c>
@@ -2538,8 +2591,11 @@
       <c r="E17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>317</v>
       </c>
@@ -2552,8 +2608,11 @@
       <c r="E18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>317</v>
       </c>
@@ -2566,8 +2625,11 @@
       <c r="E19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>317</v>
       </c>
@@ -2580,8 +2642,11 @@
       <c r="E20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>317</v>
       </c>
@@ -2594,8 +2659,11 @@
       <c r="E21" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>317</v>
       </c>
@@ -2608,8 +2676,11 @@
       <c r="E22" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>317</v>
       </c>
@@ -2622,8 +2693,11 @@
       <c r="E23" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
         <v>317</v>
       </c>
@@ -2636,8 +2710,11 @@
       <c r="E24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
         <v>317</v>
       </c>
@@ -2650,8 +2727,11 @@
       <c r="E25" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
         <v>317</v>
       </c>
@@ -2664,8 +2744,11 @@
       <c r="E26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
         <v>317</v>
       </c>
@@ -2678,8 +2761,11 @@
       <c r="E27" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>317</v>
       </c>
@@ -2692,8 +2778,11 @@
       <c r="E28" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
         <v>317</v>
       </c>
@@ -2706,8 +2795,11 @@
       <c r="E29" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
         <v>317</v>
       </c>
@@ -2720,8 +2812,11 @@
       <c r="E30" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
         <v>317</v>
       </c>
@@ -2734,8 +2829,11 @@
       <c r="E31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
         <v>317</v>
       </c>
@@ -2748,8 +2846,11 @@
       <c r="E32" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
         <v>317</v>
       </c>
@@ -2762,8 +2863,11 @@
       <c r="E33" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
         <v>317</v>
       </c>
@@ -2776,8 +2880,11 @@
       <c r="E34" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
         <v>317</v>
       </c>
@@ -2790,8 +2897,11 @@
       <c r="E35" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
         <v>317</v>
       </c>
@@ -2804,8 +2914,11 @@
       <c r="E36" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
         <v>317</v>
       </c>
@@ -2818,8 +2931,11 @@
       <c r="E37" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
         <v>317</v>
       </c>
@@ -2832,8 +2948,11 @@
       <c r="E38" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
         <v>317</v>
       </c>
@@ -2846,8 +2965,11 @@
       <c r="E39" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
         <v>317</v>
       </c>
@@ -2860,8 +2982,11 @@
       <c r="E40" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A41" s="1" t="s">
         <v>317</v>
       </c>
@@ -2874,8 +2999,11 @@
       <c r="E41" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A42" s="1" t="s">
         <v>317</v>
       </c>
@@ -2888,8 +3016,11 @@
       <c r="E42" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A43" s="1" t="s">
         <v>317</v>
       </c>
@@ -2902,8 +3033,11 @@
       <c r="E43" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A44" s="1" t="s">
         <v>317</v>
       </c>
@@ -2916,8 +3050,11 @@
       <c r="E44" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
         <v>317</v>
       </c>
@@ -2930,8 +3067,11 @@
       <c r="E45" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
         <v>317</v>
       </c>
@@ -2944,8 +3084,11 @@
       <c r="E46" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A47" s="1" t="s">
         <v>317</v>
       </c>
@@ -2958,8 +3101,11 @@
       <c r="E47" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A48" s="1" t="s">
         <v>317</v>
       </c>
@@ -2972,8 +3118,11 @@
       <c r="E48" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A49" s="1" t="s">
         <v>317</v>
       </c>
@@ -2986,8 +3135,11 @@
       <c r="E49" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A50" s="1" t="s">
         <v>317</v>
       </c>
@@ -3000,8 +3152,11 @@
       <c r="E50" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A51" s="1" t="s">
         <v>317</v>
       </c>
@@ -3014,8 +3169,11 @@
       <c r="E51" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A52" s="1" t="s">
         <v>317</v>
       </c>
@@ -3028,8 +3186,11 @@
       <c r="E52" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A53" s="1" t="s">
         <v>317</v>
       </c>
@@ -3042,8 +3203,11 @@
       <c r="E53" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A54" s="1" t="s">
         <v>317</v>
       </c>
@@ -3056,8 +3220,11 @@
       <c r="E54" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A55" s="1" t="s">
         <v>317</v>
       </c>
@@ -3070,8 +3237,11 @@
       <c r="E55" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A56" s="1" t="s">
         <v>317</v>
       </c>
@@ -3084,8 +3254,11 @@
       <c r="E56" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A57" s="1" t="s">
         <v>317</v>
       </c>
@@ -3098,8 +3271,11 @@
       <c r="E57" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A58" s="1" t="s">
         <v>317</v>
       </c>
@@ -3112,8 +3288,11 @@
       <c r="E58" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A59" s="1" t="s">
         <v>317</v>
       </c>
@@ -3129,8 +3308,11 @@
       <c r="F59" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A60" s="1" t="s">
         <v>317</v>
       </c>
@@ -3143,8 +3325,11 @@
       <c r="E60" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G60" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A61" s="1" t="s">
         <v>317</v>
       </c>
@@ -3157,8 +3342,11 @@
       <c r="E61" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G61" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A62" s="1" t="s">
         <v>317</v>
       </c>
@@ -3171,8 +3359,11 @@
       <c r="E62" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G62" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A63" s="1" t="s">
         <v>317</v>
       </c>
@@ -3185,8 +3376,11 @@
       <c r="E63" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A64" s="1" t="s">
         <v>317</v>
       </c>
@@ -3199,8 +3393,11 @@
       <c r="E64" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G64" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A65" s="1" t="s">
         <v>317</v>
       </c>
@@ -3213,8 +3410,11 @@
       <c r="E65" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A66" s="1" t="s">
         <v>317</v>
       </c>
@@ -3227,8 +3427,11 @@
       <c r="E66" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G66" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A67" s="1" t="s">
         <v>317</v>
       </c>
@@ -3241,8 +3444,11 @@
       <c r="E67" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G67" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A68" s="1" t="s">
         <v>317</v>
       </c>
@@ -3255,8 +3461,11 @@
       <c r="E68" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G68" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A69" s="1" t="s">
         <v>317</v>
       </c>
@@ -3269,8 +3478,11 @@
       <c r="E69" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G69" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A70" s="1" t="s">
         <v>317</v>
       </c>
@@ -3283,8 +3495,11 @@
       <c r="E70" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G70" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A71" s="1" t="s">
         <v>317</v>
       </c>
@@ -3297,8 +3512,11 @@
       <c r="E71" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G71" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A72" s="1" t="s">
         <v>317</v>
       </c>
@@ -3311,8 +3529,11 @@
       <c r="E72" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G72" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A73" s="1" t="s">
         <v>317</v>
       </c>
@@ -3325,8 +3546,11 @@
       <c r="E73" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G73" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A74" s="1" t="s">
         <v>317</v>
       </c>
@@ -3339,8 +3563,11 @@
       <c r="E74" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A75" s="1" t="s">
         <v>317</v>
       </c>
@@ -3353,8 +3580,11 @@
       <c r="E75" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A76" s="1" t="s">
         <v>317</v>
       </c>
@@ -3367,8 +3597,11 @@
       <c r="E76" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G76" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A77" s="1" t="s">
         <v>317</v>
       </c>
@@ -3381,8 +3614,11 @@
       <c r="E77" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G77" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A78" s="1" t="s">
         <v>317</v>
       </c>
@@ -3395,8 +3631,11 @@
       <c r="E78" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G78" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A79" s="1" t="s">
         <v>317</v>
       </c>
@@ -3409,8 +3648,11 @@
       <c r="E79" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G79" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A80" s="1" t="s">
         <v>317</v>
       </c>
@@ -3423,8 +3665,11 @@
       <c r="E80" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G80" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A81" s="1" t="s">
         <v>317</v>
       </c>
@@ -3437,8 +3682,11 @@
       <c r="E81" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G81" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A82" s="1" t="s">
         <v>317</v>
       </c>
@@ -3451,8 +3699,11 @@
       <c r="E82" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G82" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A83" s="1" t="s">
         <v>317</v>
       </c>
@@ -3465,8 +3716,11 @@
       <c r="E83" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G83" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A84" s="1" t="s">
         <v>317</v>
       </c>
@@ -3479,8 +3733,11 @@
       <c r="E84" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G84" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A85" s="1" t="s">
         <v>317</v>
       </c>
@@ -3493,8 +3750,11 @@
       <c r="E85" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G85" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A86" s="1" t="s">
         <v>317</v>
       </c>
@@ -3507,8 +3767,11 @@
       <c r="E86" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G86" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A87" s="1" t="s">
         <v>317</v>
       </c>
@@ -3521,8 +3784,11 @@
       <c r="E87" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G87" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A88" s="1" t="s">
         <v>317</v>
       </c>
@@ -3535,8 +3801,11 @@
       <c r="E88" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G88" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A89" s="1" t="s">
         <v>317</v>
       </c>
@@ -3549,8 +3818,11 @@
       <c r="E89" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G89" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A90" s="1" t="s">
         <v>317</v>
       </c>
@@ -3563,8 +3835,11 @@
       <c r="E90" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G90" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A91" s="1" t="s">
         <v>317</v>
       </c>
@@ -3577,8 +3852,11 @@
       <c r="E91" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G91" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A92" s="1" t="s">
         <v>317</v>
       </c>
@@ -3591,8 +3869,11 @@
       <c r="E92" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G92" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A93" s="1" t="s">
         <v>317</v>
       </c>
@@ -3605,8 +3886,11 @@
       <c r="E93" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G93" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A94" s="1" t="s">
         <v>317</v>
       </c>
@@ -3619,8 +3903,11 @@
       <c r="E94" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G94" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A95" s="1" t="s">
         <v>317</v>
       </c>
@@ -3633,8 +3920,11 @@
       <c r="E95" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G95" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A96" s="1" t="s">
         <v>317</v>
       </c>
@@ -3647,8 +3937,11 @@
       <c r="E96" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G96" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A97" s="1" t="s">
         <v>317</v>
       </c>
@@ -3661,8 +3954,11 @@
       <c r="E97" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G97" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A98" s="1" t="s">
         <v>317</v>
       </c>
@@ -3675,8 +3971,11 @@
       <c r="E98" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G98" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A99" s="1" t="s">
         <v>317</v>
       </c>
@@ -3689,8 +3988,11 @@
       <c r="E99" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G99" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A100" s="1" t="s">
         <v>317</v>
       </c>
@@ -3703,8 +4005,11 @@
       <c r="E100" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G100" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A101" s="1" t="s">
         <v>317</v>
       </c>
@@ -3720,8 +4025,11 @@
       <c r="F101" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G101" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A102" s="1" t="s">
         <v>317</v>
       </c>
@@ -3737,8 +4045,11 @@
       <c r="F102" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G102" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A103" s="1" t="s">
         <v>317</v>
       </c>
@@ -3751,8 +4062,11 @@
       <c r="E103" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G103" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A104" s="1" t="s">
         <v>317</v>
       </c>
@@ -3765,8 +4079,11 @@
       <c r="E104" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G104" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A105" s="1" t="s">
         <v>317</v>
       </c>
@@ -3779,8 +4096,11 @@
       <c r="E105" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G105" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A106" s="1" t="s">
         <v>317</v>
       </c>
@@ -3793,8 +4113,11 @@
       <c r="E106" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G106" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A107" s="1" t="s">
         <v>317</v>
       </c>
@@ -3807,8 +4130,11 @@
       <c r="E107" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G107" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A108" s="1" t="s">
         <v>317</v>
       </c>
@@ -3821,8 +4147,11 @@
       <c r="E108" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G108" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A109" s="1" t="s">
         <v>317</v>
       </c>
@@ -3835,8 +4164,11 @@
       <c r="E109" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G109" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A110" s="1" t="s">
         <v>317</v>
       </c>
@@ -3849,8 +4181,11 @@
       <c r="E110" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G110" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A111" s="1" t="s">
         <v>317</v>
       </c>
@@ -3863,8 +4198,11 @@
       <c r="E111" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G111" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A112" s="1" t="s">
         <v>317</v>
       </c>
@@ -3877,8 +4215,11 @@
       <c r="E112" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G112" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A113" s="1" t="s">
         <v>317</v>
       </c>
@@ -3891,8 +4232,11 @@
       <c r="E113" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G113" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A114" s="1" t="s">
         <v>317</v>
       </c>
@@ -3905,8 +4249,11 @@
       <c r="E114" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G114" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A115" s="1" t="s">
         <v>317</v>
       </c>
@@ -3919,8 +4266,11 @@
       <c r="E115" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G115" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A116" s="1" t="s">
         <v>317</v>
       </c>
@@ -3936,8 +4286,11 @@
       <c r="F116" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G116" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A117" s="1" t="s">
         <v>317</v>
       </c>
@@ -3950,8 +4303,11 @@
       <c r="E117" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G117" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A118" s="1" t="s">
         <v>317</v>
       </c>
@@ -3967,8 +4323,11 @@
       <c r="F118" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G118" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A119" s="1" t="s">
         <v>317</v>
       </c>
@@ -3981,8 +4340,11 @@
       <c r="E119" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G119" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A120" s="1" t="s">
         <v>317</v>
       </c>
@@ -3995,8 +4357,11 @@
       <c r="E120" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G120" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A121" s="1" t="s">
         <v>317</v>
       </c>
@@ -4009,8 +4374,11 @@
       <c r="E121" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G121" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A122" s="1" t="s">
         <v>317</v>
       </c>
@@ -4023,8 +4391,11 @@
       <c r="E122" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G122" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A123" s="1" t="s">
         <v>317</v>
       </c>
@@ -4037,8 +4408,11 @@
       <c r="E123" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G123" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A124" s="1" t="s">
         <v>317</v>
       </c>
@@ -4051,8 +4425,11 @@
       <c r="E124" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G124" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A125" s="1" t="s">
         <v>317</v>
       </c>
@@ -4065,8 +4442,11 @@
       <c r="E125" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G125" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A126" s="1" t="s">
         <v>317</v>
       </c>
@@ -4079,8 +4459,11 @@
       <c r="E126" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G126" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A127" s="1" t="s">
         <v>317</v>
       </c>
@@ -4093,8 +4476,11 @@
       <c r="E127" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G127" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A128" s="1" t="s">
         <v>317</v>
       </c>
@@ -4110,8 +4496,11 @@
       <c r="F128" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G128" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A129" s="1" t="s">
         <v>317</v>
       </c>
@@ -4124,8 +4513,11 @@
       <c r="E129" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G129" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A130" s="1" t="s">
         <v>317</v>
       </c>
@@ -4138,8 +4530,11 @@
       <c r="E130" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G130" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A131" s="1" t="s">
         <v>317</v>
       </c>
@@ -4152,8 +4547,11 @@
       <c r="E131" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G131" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A132" s="1" t="s">
         <v>317</v>
       </c>
@@ -4166,8 +4564,11 @@
       <c r="E132" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G132" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A133" s="1" t="s">
         <v>317</v>
       </c>
@@ -4180,8 +4581,11 @@
       <c r="E133" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G133" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A134" s="1" t="s">
         <v>317</v>
       </c>
@@ -4194,8 +4598,11 @@
       <c r="E134" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G134" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A135" s="1" t="s">
         <v>317</v>
       </c>
@@ -4208,8 +4615,11 @@
       <c r="E135" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G135" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A136" s="1" t="s">
         <v>317</v>
       </c>
@@ -4222,8 +4632,11 @@
       <c r="E136" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G136" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A137" s="1" t="s">
         <v>317</v>
       </c>
@@ -4236,8 +4649,11 @@
       <c r="E137" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G137" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A138" s="1" t="s">
         <v>317</v>
       </c>
@@ -4250,8 +4666,11 @@
       <c r="E138" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G138" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A139" s="1" t="s">
         <v>317</v>
       </c>
@@ -4264,8 +4683,11 @@
       <c r="E139" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G139" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A140" s="1" t="s">
         <v>317</v>
       </c>
@@ -4278,8 +4700,11 @@
       <c r="E140" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G140" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A141" s="1" t="s">
         <v>317</v>
       </c>
@@ -4292,8 +4717,11 @@
       <c r="E141" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G141" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A142" s="1" t="s">
         <v>317</v>
       </c>
@@ -4306,8 +4734,11 @@
       <c r="E142" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G142" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A143" s="1" t="s">
         <v>317</v>
       </c>
@@ -4320,8 +4751,11 @@
       <c r="E143" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G143" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A144" s="1" t="s">
         <v>317</v>
       </c>
@@ -4334,8 +4768,11 @@
       <c r="E144" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G144" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A145" s="1" t="s">
         <v>441</v>
       </c>
@@ -4348,8 +4785,11 @@
       <c r="E145" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G145" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A146" s="1" t="s">
         <v>441</v>
       </c>
@@ -4362,8 +4802,11 @@
       <c r="E146" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G146" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A147" s="1" t="s">
         <v>441</v>
       </c>
@@ -4376,8 +4819,11 @@
       <c r="E147" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G147" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A148" s="1" t="s">
         <v>441</v>
       </c>
@@ -4390,8 +4836,11 @@
       <c r="E148" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G148" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A149" s="1" t="s">
         <v>441</v>
       </c>
@@ -4404,8 +4853,11 @@
       <c r="E149" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G149" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A150" s="1" t="s">
         <v>441</v>
       </c>
@@ -4418,8 +4870,11 @@
       <c r="E150" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G150" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A151" s="1" t="s">
         <v>441</v>
       </c>
@@ -4432,8 +4887,11 @@
       <c r="E151" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G151" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A152" s="1" t="s">
         <v>441</v>
       </c>
@@ -4446,8 +4904,11 @@
       <c r="E152" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G152" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A153" s="1" t="s">
         <v>441</v>
       </c>
@@ -4463,8 +4924,11 @@
       <c r="F153" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G153" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A154" s="1" t="s">
         <v>441</v>
       </c>
@@ -4477,8 +4941,11 @@
       <c r="E154" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G154" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A155" s="1" t="s">
         <v>441</v>
       </c>
@@ -4494,8 +4961,11 @@
       <c r="F155" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G155" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A156" s="1" t="s">
         <v>441</v>
       </c>
@@ -4508,8 +4978,11 @@
       <c r="E156" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G156" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A157" s="1" t="s">
         <v>441</v>
       </c>
@@ -4522,8 +4995,11 @@
       <c r="E157" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G157" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A158" s="1" t="s">
         <v>441</v>
       </c>
@@ -4539,8 +5015,11 @@
       <c r="F158" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G158" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A159" s="1" t="s">
         <v>441</v>
       </c>
@@ -4554,7 +5033,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" ht="86" x14ac:dyDescent="0.5">
       <c r="A160" s="1" t="s">
         <v>441</v>
       </c>
@@ -4568,7 +5047,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A161" s="1" t="s">
         <v>441</v>
       </c>
@@ -4584,8 +5063,11 @@
       <c r="F161" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G161" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A162" s="1" t="s">
         <v>441</v>
       </c>
@@ -4601,8 +5083,11 @@
       <c r="F162" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G162" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="86" x14ac:dyDescent="0.5">
       <c r="A163" s="1" t="s">
         <v>441</v>
       </c>
@@ -4619,7 +5104,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A164" s="1" t="s">
         <v>459</v>
       </c>
@@ -4633,7 +5118,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A165" s="1" t="s">
         <v>459</v>
       </c>
@@ -4650,7 +5135,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A166" s="1" t="s">
         <v>459</v>
       </c>
@@ -4664,7 +5149,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A167" s="1" t="s">
         <v>459</v>
       </c>
@@ -4678,7 +5163,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="43" x14ac:dyDescent="0.5">
       <c r="A168" s="1" t="s">
         <v>459</v>
       </c>
@@ -4692,7 +5177,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A169" s="1" t="s">
         <v>459</v>
       </c>
@@ -4700,7 +5185,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" ht="43" x14ac:dyDescent="0.5">
       <c r="A170" s="1" t="s">
         <v>459</v>
       </c>
@@ -4717,7 +5202,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" ht="43" x14ac:dyDescent="0.5">
       <c r="A171" s="1" t="s">
         <v>459</v>
       </c>
@@ -4734,7 +5219,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A172" t="s">
         <v>355</v>
       </c>
@@ -4751,7 +5236,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A173" t="s">
         <v>355</v>
       </c>
@@ -4768,7 +5253,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A174" t="s">
         <v>356</v>
       </c>
@@ -4782,7 +5267,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A175" t="s">
         <v>356</v>
       </c>
@@ -4796,7 +5281,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.5">
       <c r="A176" t="s">
         <v>356</v>
       </c>
@@ -4813,7 +5298,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A177" t="s">
         <v>356</v>
       </c>
@@ -4830,7 +5315,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A178" t="s">
         <v>356</v>
       </c>
@@ -4847,7 +5332,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A179" t="s">
         <v>356</v>
       </c>
@@ -4864,7 +5349,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A180" t="s">
         <v>356</v>
       </c>
@@ -4881,7 +5366,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A181" t="s">
         <v>356</v>
       </c>
@@ -4898,7 +5383,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A182" t="s">
         <v>356</v>
       </c>
@@ -4915,7 +5400,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A183" t="s">
         <v>356</v>
       </c>
@@ -4932,7 +5417,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A184" t="s">
         <v>356</v>
       </c>
@@ -4946,7 +5431,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A185" t="s">
         <v>356</v>
       </c>
@@ -4960,7 +5445,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A186" t="s">
         <v>478</v>
       </c>
@@ -4977,7 +5462,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A187" t="s">
         <v>478</v>
       </c>
@@ -4994,7 +5479,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A188" t="s">
         <v>478</v>
       </c>
@@ -5011,7 +5496,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A189" t="s">
         <v>478</v>
       </c>
@@ -5028,7 +5513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A190" t="s">
         <v>478</v>
       </c>
@@ -5045,7 +5530,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A191" t="s">
         <v>478</v>
       </c>
@@ -5062,7 +5547,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A192" t="s">
         <v>357</v>
       </c>
@@ -5079,7 +5564,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A193" t="s">
         <v>357</v>
       </c>
@@ -5096,7 +5581,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A194" t="s">
         <v>357</v>
       </c>
@@ -5113,7 +5598,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A195" t="s">
         <v>357</v>
       </c>
@@ -5130,7 +5615,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A196" t="s">
         <v>357</v>
       </c>
@@ -5147,7 +5632,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A197" t="s">
         <v>357</v>
       </c>
@@ -5164,7 +5649,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A198" t="s">
         <v>357</v>
       </c>
@@ -5181,7 +5666,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A199" t="s">
         <v>357</v>
       </c>
@@ -5198,7 +5683,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A200" t="s">
         <v>357</v>
       </c>
@@ -5215,7 +5700,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A201" t="s">
         <v>357</v>
       </c>
@@ -5232,7 +5717,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A202" t="s">
         <v>357</v>
       </c>
@@ -5249,7 +5734,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A203" t="s">
         <v>357</v>
       </c>
@@ -5266,7 +5751,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A204" t="s">
         <v>357</v>
       </c>
@@ -5283,7 +5768,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A205" t="s">
         <v>357</v>
       </c>
@@ -5300,7 +5785,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A206" t="s">
         <v>357</v>
       </c>
@@ -5317,7 +5802,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A207" t="s">
         <v>357</v>
       </c>
@@ -5334,7 +5819,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A208" t="s">
         <v>357</v>
       </c>
@@ -5351,7 +5836,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A209" t="s">
         <v>357</v>
       </c>
@@ -5368,7 +5853,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A210" t="s">
         <v>357</v>
       </c>
@@ -5385,7 +5870,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A211" t="s">
         <v>357</v>
       </c>
@@ -5402,7 +5887,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A212" t="s">
         <v>357</v>
       </c>
@@ -5419,7 +5904,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A213" t="s">
         <v>357</v>
       </c>
@@ -5436,7 +5921,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A214" t="s">
         <v>357</v>
       </c>
@@ -5453,7 +5938,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A215" t="s">
         <v>357</v>
       </c>
@@ -5470,7 +5955,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A216" t="s">
         <v>357</v>
       </c>
@@ -5487,7 +5972,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A217" t="s">
         <v>357</v>
       </c>
@@ -5504,7 +5989,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A218" t="s">
         <v>357</v>
       </c>
@@ -5521,7 +6006,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A219" t="s">
         <v>357</v>
       </c>
@@ -5538,7 +6023,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A220" t="s">
         <v>357</v>
       </c>
@@ -5555,7 +6040,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A221" t="s">
         <v>357</v>
       </c>
@@ -5572,7 +6057,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A222" t="s">
         <v>423</v>
       </c>
@@ -5589,7 +6074,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A223" t="s">
         <v>423</v>
       </c>
@@ -5606,7 +6091,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A224" t="s">
         <v>423</v>
       </c>
@@ -5623,7 +6108,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A225" t="s">
         <v>423</v>
       </c>
@@ -5640,7 +6125,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A226" t="s">
         <v>423</v>
       </c>
@@ -5657,7 +6142,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A227" t="s">
         <v>423</v>
       </c>
@@ -5674,7 +6159,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A228" t="s">
         <v>423</v>
       </c>
@@ -5691,7 +6176,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A229" t="s">
         <v>424</v>
       </c>
@@ -5708,7 +6193,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A230" t="s">
         <v>424</v>
       </c>
@@ -5725,7 +6210,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A231" t="s">
         <v>424</v>
       </c>
@@ -5742,7 +6227,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A232" t="s">
         <v>424</v>
       </c>
@@ -5759,7 +6244,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A233" t="s">
         <v>424</v>
       </c>
@@ -5776,7 +6261,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A234" t="s">
         <v>464</v>
       </c>
@@ -5790,7 +6275,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A235" s="1" t="s">
         <v>464</v>
       </c>
@@ -5804,7 +6289,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A236" s="1" t="s">
         <v>484</v>
       </c>
@@ -5821,7 +6306,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" hidden="1" x14ac:dyDescent="0.5">
       <c r="A237" t="s">
         <v>484</v>
       </c>
@@ -5838,7 +6323,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="238" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A238" s="1" t="s">
         <v>466</v>
       </c>
@@ -5852,7 +6337,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="239" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A239" s="1" t="s">
         <v>466</v>
       </c>
@@ -5866,7 +6351,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="240" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" ht="43" x14ac:dyDescent="0.5">
       <c r="A240" s="1" t="s">
         <v>479</v>
       </c>
@@ -5883,7 +6368,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="241" spans="1:6" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" ht="129" x14ac:dyDescent="0.5">
       <c r="A241" s="1" t="s">
         <v>479</v>
       </c>
@@ -5900,7 +6385,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="242" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A242" s="1" t="s">
         <v>479</v>
       </c>
@@ -5914,7 +6399,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="243" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A243" s="1" t="s">
         <v>479</v>
       </c>
@@ -5931,7 +6416,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="244" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A244" s="1" t="s">
         <v>479</v>
       </c>
@@ -5948,7 +6433,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="245" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A245" s="1" t="s">
         <v>479</v>
       </c>
@@ -5965,7 +6450,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="246" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A246" s="1" t="s">
         <v>479</v>
       </c>
@@ -5982,7 +6467,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="247" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A247" s="1" t="s">
         <v>479</v>
       </c>
@@ -5999,7 +6484,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="248" spans="1:6" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" ht="100.35" x14ac:dyDescent="0.5">
       <c r="A248" s="1" t="s">
         <v>479</v>
       </c>
@@ -6016,7 +6501,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="249" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" ht="86" x14ac:dyDescent="0.5">
       <c r="A249" s="1" t="s">
         <v>479</v>
       </c>
@@ -6033,7 +6518,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="250" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A250" s="1" t="s">
         <v>479</v>
       </c>
@@ -6050,7 +6535,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="251" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A251" s="1" t="s">
         <v>479</v>
       </c>
@@ -6067,7 +6552,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="252" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A252" s="1" t="s">
         <v>479</v>
       </c>
@@ -6084,7 +6569,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="253" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A253" s="1" t="s">
         <v>479</v>
       </c>
@@ -6101,7 +6586,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="254" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A254" s="1" t="s">
         <v>479</v>
       </c>
@@ -6118,7 +6603,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="255" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A255" s="1" t="s">
         <v>479</v>
       </c>
@@ -6135,7 +6620,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="256" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A256" s="1" t="s">
         <v>479</v>
       </c>

</xml_diff>